<commit_message>
modified:   Brighway/LCA_plots.py 	modified:   Brighway/Ofir.ipynb 	modified:   Brighway/Results/Ananas - CONSQ_recipe.xlsx 	new file:   Brighway/Results/Ananas contribution - CONSQ_recipe.xlsx 	new file:   Brighway/Results/Lobster - CONSQ_recipe.xlsx 	modified:   Brighway/Single-use-vs-multi-use-in-health-care/Results/GWP_life_stage_CONSQ.jpg 	modified:   Brighway/Single-use-vs-multi-use-in-health-care/Results/scaled_impact_score_multi_CONSQ_ReCiPe 2016 v1.03, endpoint (H).jpg 	modified:   Brighway/Single-use-vs-multi-use-in-health-care/Results/scaled_impact_score_multi_CONSQ_ReCiPe 2016 v1.03, midpoint (H).jpg 	new file:   Brighway/Stine.ipynb 	modified:   Brighway/__pycache__/LCA_plots.cpython-311.pyc 	modified:   Brighway/__pycache__/life_cycle_assessment.cpython-311.pyc 	modified:   Brighway/df_idx_ofir 	new file:   Brighway/df_idx_ofir_CONSQ 	modified:   Brighway/life_cycle_assessment.py
</commit_message>
<xml_diff>
--- a/Brighway/Results/Ananas - CONSQ_recipe.xlsx
+++ b/Brighway/Results/Ananas - CONSQ_recipe.xlsx
@@ -79,193 +79,193 @@
     <t>('ReCiPe 2016 v1.03, endpoint (H)', 'total: natural resources', 'natural resources')</t>
   </si>
   <si>
-    <t>[["alubox raw materials - CONSQ", 0.0006775653291214696], ["alubox production - CONSQ", 6.629550602005674e-05], ["autoclave - CONSQ", 0.0008168335382818346], ["Handwash - CONSQ", 8.905819244255838e-05], ["alubox EoL melting - CONSQ", 0.0005884192390184658], ["alubox EoL mixed sorting - CONSQ", 8.5626348897486e-06], ["transport Alu - CONSQ", 3.228776205788375e-06], ["avoided alubox raw materials - CONSQ", -0.0006339914261942786]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0005945666949553682], ["autoclave - CONSQ", 0.0008168335382818346], ["market for corrugated board box", 2.5837221571970654e-05], ["packaging film production, low density polyethylene", 6.376674759785153e-05], ["market for polypropylene, granulate", 0.0004018382259604529], ["market for electricity, high voltage", -6.326849386338696e-05], ["transport Plastic - CONSQ", 0.00029561069063068147], ["PE incineration no Energy Recovery - CONSQ", 2.036580944412297e-06], ["PP incineration no Energy Recovery - CONSQ", 1.5021306204305053e-05], ["marginal heating grid projection updated - CONSQ", -0.00022017492766633167]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0005945666949553682], ["autoclave - CONSQ", 0.0008168335382818346], ["market for corrugated board box", 2.5837221571970654e-05], ["packaging film production, low density polyethylene", 6.376674759785153e-05], ["market for polypropylene, granulate", 0.0004018382259604529], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -2.5817207918465817e-05], ["market for polypropylene, granulate", -0.00021699264202029305], ["market for electricity, high voltage", -2.9103507177158007e-05], ["transport Plastic - CONSQ", 0.00029561069063068147], ["PE incineration no Energy Recovery - CONSQ", 9.368272342888135e-07], ["PP incineration no Energy Recovery - CONSQ", 6.9098008569590785e-06], ["marginal heating grid projection updated - CONSQ", -0.00010128046671714267]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.16065411473479815], ["alubox production - CONSQ", 0.02831917737938991], ["autoclave - CONSQ", 0.9514917534489937], ["Handwash - CONSQ", 0.053194985477380365], ["alubox EoL melting - CONSQ", 0.1351832677158519], ["alubox EoL mixed sorting - CONSQ", 0.0033103760101259065], ["transport Alu - CONSQ", 0.0022070189181995397], ["avoided alubox raw materials - CONSQ", -0.14898660207151987]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.24557815917583573], ["autoclave - CONSQ", 0.9514917534489937], ["market for corrugated board box", 0.013204980950018264], ["packaging film production, low density polyethylene", 0.028359676338399035], ["market for polypropylene, granulate", 0.18813136805414704], ["market for electricity, high voltage", -0.07106972416995291], ["transport Plastic - CONSQ", 0.06422041919014608], ["PE incineration no Energy Recovery - CONSQ", 0.03038603791590037], ["PP incineration no Energy Recovery - CONSQ", 0.2222611045485942], ["marginal heating grid projection updated - CONSQ", -0.2671565541994551]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.24557815917583573], ["autoclave - CONSQ", 0.9514917534489937], ["market for corrugated board box", 0.013204980950018264], ["packaging film production, low density polyethylene", 0.028359676338399035], ["market for polypropylene, granulate", 0.18813136805414704], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.011961150087913522], ["market for polypropylene, granulate", -0.10159093874999724], ["market for electricity, high voltage", -0.03269207311817847], ["transport Plastic - CONSQ", 0.06422041919014608], ["PE incineration no Energy Recovery - CONSQ", 0.013977577441307487], ["PP incineration no Energy Recovery - CONSQ", 0.10224010809265972], ["marginal heating grid projection updated - CONSQ", -0.12289201493091992]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.004857366128195334], ["alubox production - CONSQ", 0.0017893668031139633], ["autoclave - CONSQ", 0.04265337222864427], ["Handwash - CONSQ", 0.001511555692377246], ["alubox EoL melting - CONSQ", 0.0017729271065047105], ["alubox EoL mixed sorting - CONSQ", 0.0008989760159706329], ["transport Alu - CONSQ", 5.9933956930798026e-05], ["avoided alubox raw materials - CONSQ", -0.004217495270988052]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0064123842070893024], ["autoclave - CONSQ", 0.04265337222864427], ["market for corrugated board box", 0.0002611840476741577], ["packaging film production, low density polyethylene", 0.0006539456792695441], ["market for polypropylene, granulate", 0.0031418480748664867], ["market for electricity, high voltage", -0.002938841162242666], ["transport Plastic - CONSQ", 0.002278424105907691], ["PE incineration no Energy Recovery - CONSQ", 0.001585628623996276], ["PP incineration no Energy Recovery - CONSQ", 0.011602460208341894], ["marginal heating grid projection updated - CONSQ", -0.005950773212900693]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0064123842070893024], ["autoclave - CONSQ", 0.04265337222864427], ["market for corrugated board box", 0.0002611840476741577], ["packaging film production, low density polyethylene", 0.0006539456792695441], ["market for polypropylene, granulate", 0.0031418480748664867], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.00020579922897293133], ["market for polypropylene, granulate", -0.0016965979604118935], ["market for electricity, high voltage", -0.0013518669346316548], ["transport Plastic - CONSQ", 0.002278424105907691], ["PE incineration no Energy Recovery - CONSQ", 0.0007293891670346102], ["PP incineration no Energy Recovery - CONSQ", 0.00533713169590558], ["marginal heating grid projection updated - CONSQ", -0.0027373556777008806]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.006751992919744967], ["alubox production - CONSQ", 0.0023508468663048536], ["autoclave - CONSQ", 0.05250688745632648], ["Handwash - CONSQ", 0.001740772693413934], ["alubox EoL melting - CONSQ", 0.0025003886662588065], ["alubox EoL mixed sorting - CONSQ", 0.0011115381054173595], ["transport Alu - CONSQ", 0.00010128822659251569], ["avoided alubox raw materials - CONSQ", -0.005873426730980366]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.008523811736175751], ["autoclave - CONSQ", 0.05250688745632648], ["market for corrugated board box", 0.0003621664954644836], ["packaging film production, low density polyethylene", 0.0008697010162811554], ["market for polypropylene, granulate", 0.0042630945982127105], ["market for electricity, high voltage", -0.0036282928476571844], ["transport Plastic - CONSQ", 0.003058344480169973], ["PE incineration no Energy Recovery - CONSQ", 0.002295784818484778], ["PP incineration no Energy Recovery - CONSQ", 0.016797606943568195], ["marginal heating grid projection updated - CONSQ", -0.007628174041368469]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.008523811736175751], ["autoclave - CONSQ", 0.05250688745632648], ["market for corrugated board box", 0.0003621664954644836], ["packaging film production, low density polyethylene", 0.0008697010162811554], ["market for polypropylene, granulate", 0.0042630945982127105], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.00027891919263887786], ["market for polypropylene, granulate", -0.0023020710830179395], ["market for electricity, high voltage", -0.0016690147099223404], ["transport Plastic - CONSQ", 0.003058344480169973], ["PE incineration no Energy Recovery - CONSQ", 0.0010560610164978847], ["PP incineration no Energy Recovery - CONSQ", 0.007726899194135489], ["marginal heating grid projection updated - CONSQ", -0.003508960058708388]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.3759023151854832], ["alubox production - CONSQ", 0.12963524348861682], ["autoclave - CONSQ", 2.796804363972611], ["Handwash - CONSQ", 0.11127580026625142], ["alubox EoL melting - CONSQ", -0.09392069859161326], ["alubox EoL mixed sorting - CONSQ", 0.020102297412730338], ["transport Alu - CONSQ", 0.04144820926422995], ["avoided alubox raw materials - CONSQ", -0.2819864416149727]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.8401285409572375], ["autoclave - CONSQ", 2.796804363972611], ["market for corrugated board box", 0.03017058176478913], ["packaging film production, low density polyethylene", 0.07006761610492501], ["market for polypropylene, granulate", 0.5179952808941972], ["market for electricity, high voltage", -0.18417119408315813], ["transport Plastic - CONSQ", 0.24405019146629844], ["PE incineration no Energy Recovery - CONSQ", 0.08828092784747552], ["PP incineration no Energy Recovery - CONSQ", 0.6457914444398691], ["marginal heating grid projection updated - CONSQ", -0.5986092474915773]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.8401285409572375], ["autoclave - CONSQ", 2.796804363972611], ["market for corrugated board box", 0.03017058176478913], ["packaging film production, low density polyethylene", 0.07006761610492501], ["market for polypropylene, granulate", 0.5179952808941972], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.034323148728948046], ["market for polypropylene, granulate", -0.27971745168817114], ["market for electricity, high voltage", -0.08471874927824764], ["transport Plastic - CONSQ", 0.24405019146629844], ["PE incineration no Energy Recovery - CONSQ", 0.04060922680853886], ["PP incineration no Energy Recovery - CONSQ", 0.2970640644614118], ["marginal heating grid projection updated - CONSQ", -0.27536025378017226]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.03486045202302537], ["alubox production - CONSQ", 0.006912374841593515], ["autoclave - CONSQ", 0.06318683146872511], ["Handwash - CONSQ", 0.003951335836075654], ["alubox EoL melting - CONSQ", 0.02878277194072873], ["alubox EoL mixed sorting - CONSQ", 0.0008417001438567534], ["transport Alu - CONSQ", 0.0006922450866290449], ["avoided alubox raw materials - CONSQ", -0.03229125436738581]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.15748810250534676], ["autoclave - CONSQ", 0.06318683146872511], ["market for corrugated board box", 0.0014061075334226376], ["packaging film production, low density polyethylene", 0.017987128602816135], ["market for polypropylene, granulate", 0.14340516514392737], ["market for electricity, high voltage", -0.001480827968056739], ["transport Plastic - CONSQ", 0.0176105247311969], ["PE incineration no Energy Recovery - CONSQ", 0.00011028712725006705], ["PP incineration no Energy Recovery - CONSQ", 0.000822342607897708], ["marginal heating grid projection updated - CONSQ", -0.040344705531723216]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.15748810250534676], ["autoclave - CONSQ", 0.06318683146872511], ["market for corrugated board box", 0.0014061075334226376], ["packaging film production, low density polyethylene", 0.017987128602816135], ["market for polypropylene, granulate", 0.14340516514392737], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.008778008074957903], ["market for polypropylene, granulate", -0.07743878917855443], ["market for electricity, high voltage", -0.0006811808653061771], ["transport Plastic - CONSQ", 0.0176105247311969], ["PE incineration no Energy Recovery - CONSQ", 5.073207853434645e-05], ["PP incineration no Energy Recovery - CONSQ", 0.0003782775997048625], ["marginal heating grid projection updated - CONSQ", -0.018558564544429473]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 5.674689072520567e-05], ["alubox production - CONSQ", 1.3998613322346925e-05], ["autoclave - CONSQ", 3.532670422374631e-05], ["Handwash - CONSQ", 0.00018763526794536933], ["alubox EoL melting - CONSQ", 4.490172565760039e-05], ["alubox EoL mixed sorting - CONSQ", 2.915806882562605e-06], ["transport Alu - CONSQ", 2.1648705350448494e-07], ["avoided alubox raw materials - CONSQ", -5.145723028294836e-05]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 4.645599492310459e-05], ["autoclave - CONSQ", 3.532670422374631e-05], ["market for corrugated board box", 6.06066020511809e-06], ["packaging film production, low density polyethylene", 6.4122449313985585e-06], ["market for polypropylene, granulate", 1.964683665613263e-05], ["market for electricity, high voltage", -2.4210043726611105e-06], ["transport Plastic - CONSQ", 1.3666018003575128e-05], ["PE incineration no Energy Recovery - CONSQ", 4.700623400921132e-08], ["PP incineration no Energy Recovery - CONSQ", 3.726141326394346e-07], ["marginal heating grid projection updated - CONSQ", -2.3169237072898118e-05]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 4.645599492310459e-05], ["autoclave - CONSQ", 3.532670422374631e-05], ["market for corrugated board box", 6.06066020511809e-06], ["packaging film production, low density polyethylene", 6.4122449313985585e-06], ["market for polypropylene, granulate", 1.964683665613263e-05], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -1.3837296222243698e-06], ["market for polypropylene, granulate", -1.060929179428487e-05], ["market for electricity, high voltage", -1.1136620114242214e-06], ["transport Plastic - CONSQ", 1.3666018003575128e-05], ["PE incineration no Energy Recovery - CONSQ", 2.1622867637801865e-08], ["PP incineration no Energy Recovery - CONSQ", 1.714025011608132e-07], ["marginal heating grid projection updated - CONSQ", -1.0657849053051023e-05]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 3.807305699037143e-06], ["alubox production - CONSQ", 2.2529251963788977e-06], ["autoclave - CONSQ", 4.150004785784196e-05], ["Handwash - CONSQ", 9.585919061117324e-05], ["alubox EoL melting - CONSQ", 3.2952848528349646e-06], ["alubox EoL mixed sorting - CONSQ", 1.2776676442955444e-07], ["transport Alu - CONSQ", 5.890105738717062e-08], ["avoided alubox raw materials - CONSQ", -3.525946157865783e-06]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 5.488323124418135e-06], ["autoclave - CONSQ", 4.150004785784196e-05], ["market for corrugated board box", 3.8612259228844765e-07], ["packaging film production, low density polyethylene", 8.931098200818854e-07], ["market for polypropylene, granulate", 2.3047807636825643e-06], ["market for electricity, high voltage", -2.5865098072986024e-07], ["transport Plastic - CONSQ", 1.585718535587094e-06], ["PE incineration no Energy Recovery - CONSQ", 4.725445040866733e-08], ["PP incineration no Energy Recovery - CONSQ", 3.4690323686800294e-07], ["marginal heating grid projection updated - CONSQ", -2.0408849537624103e-06]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 5.488323124418135e-06], ["autoclave - CONSQ", 4.150004785784196e-05], ["market for corrugated board box", 3.8612259228844765e-07], ["packaging film production, low density polyethylene", 8.931098200818854e-07], ["market for polypropylene, granulate", 2.3047807636825643e-06], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -1.536964550964375e-07], ["market for polypropylene, granulate", -1.2445816124297446e-06], ["market for electricity, high voltage", -1.1897945113574372e-07], ["transport Plastic - CONSQ", 1.585718535587094e-06], ["PE incineration no Energy Recovery - CONSQ", 2.1737047188151964e-08], ["PP incineration no Energy Recovery - CONSQ", 1.5957548897079732e-07], ["marginal heating grid projection updated - CONSQ", -9.388070787080571e-07]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.03618091952136528], ["alubox production - CONSQ", 0.002802918631369497], ["autoclave - CONSQ", 0.012800098541810273], ["Handwash - CONSQ", 0.003205934990335598], ["alubox EoL melting - CONSQ", 0.02668139673543732], ["alubox EoL mixed sorting - CONSQ", -0.010000873466723091], ["transport Alu - CONSQ", 2.8936991254661035e-05], ["avoided alubox raw materials - CONSQ", -0.03219876077563191]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.006459424083728573], ["autoclave - CONSQ", 0.012800098541810273], ["market for corrugated board box", 0.0003079234064602862], ["packaging film production, low density polyethylene", 0.0007490979899267339], ["market for polypropylene, granulate", 0.004290057233679009], ["market for electricity, high voltage", -0.0009023851508517537], ["transport Plastic - CONSQ", 0.001352133426703654], ["PE incineration no Energy Recovery - CONSQ", 7.043862153000954e-05], ["PP incineration no Energy Recovery - CONSQ", 0.0005141072547311531], ["marginal heating grid projection updated - CONSQ", -0.0022590076583807596]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.006459424083728573], ["autoclave - CONSQ", 0.012800098541810273], ["market for corrugated board box", 0.0003079234064602862], ["packaging film production, low density polyethylene", 0.0007490979899267339], ["market for polypropylene, granulate", 0.004290057233679009], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.0003578493652562967], ["market for polypropylene, granulate", -0.0023166309062040437], ["market for electricity, high voltage", -0.000415097169391784], ["transport Plastic - CONSQ", 0.001352133426703654], ["PE incineration no Energy Recovery - CONSQ", 3.240176590182773e-05], ["PP incineration no Energy Recovery - CONSQ", 0.00023648933721108712], ["marginal heating grid projection updated - CONSQ", -0.00103914352273167]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.14399189342699173], ["alubox production - CONSQ", 0.03422369551082981], ["autoclave - CONSQ", 0.43237058124408256], ["Handwash - CONSQ", 0.05715187220635177], ["alubox EoL melting - CONSQ", 0.0600731686418045], ["alubox EoL mixed sorting - CONSQ", 0.01025578116793676], ["transport Alu - CONSQ", 0.0018208619424319717], ["avoided alubox raw materials - CONSQ", -0.13069794729761924]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.13081523583495647], ["autoclave - CONSQ", 0.43237058124408256], ["market for corrugated board box", 0.00997482064110965], ["packaging film production, low density polyethylene", 0.0150342046587877], ["market for polypropylene, granulate", 0.07156715003699723], ["market for electricity, high voltage", -0.029259968209803033], ["transport Plastic - CONSQ", 0.039116311061299494], ["PE incineration no Energy Recovery - CONSQ", 0.019130751398285014], ["PP incineration no Energy Recovery - CONSQ", 0.13997609610912873], ["marginal heating grid projection updated - CONSQ", -0.0897472805432895]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.13081523583495647], ["autoclave - CONSQ", 0.43237058124408256], ["market for corrugated board box", 0.00997482064110965], ["packaging film production, low density polyethylene", 0.0150342046587877], ["market for polypropylene, granulate", 0.07156715003699723], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.0047580063349078935], ["market for polypropylene, granulate", -0.038646261019972594], ["market for electricity, high voltage", -0.013459585376509552], ["transport Plastic - CONSQ", 0.039116311061299494], ["PE incineration no Energy Recovery - CONSQ", 0.008800145643101043], ["PP incineration no Energy Recovery - CONSQ", 0.06438900421213135], ["marginal heating grid projection updated - CONSQ", -0.04128374904340956]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.0005062928627309998], ["alubox production - CONSQ", 0.001830362817578603], ["autoclave - CONSQ", -0.0050337016375417085], ["Handwash - CONSQ", 0.001604097503814595], ["alubox EoL melting - CONSQ", 0.001078928618325496], ["alubox EoL mixed sorting - CONSQ", -0.00014209540004928974], ["transport Alu - CONSQ", 9.393569902242495e-06], ["avoided alubox raw materials - CONSQ", -0.0005646553300523532]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.00816860351443792], ["autoclave - CONSQ", -0.0050337016375417085], ["market for corrugated board box", -0.00019329161513200805], ["packaging film production, low density polyethylene", 0.0012730945337941888], ["market for polypropylene, granulate", 0.002750892066170575], ["market for electricity, high voltage", -1.5033729725594517e-05], ["transport Plastic - CONSQ", 0.00023580918814396272], ["PE incineration no Energy Recovery - CONSQ", 2.8633182280103825e-07], ["PP incineration no Energy Recovery - CONSQ", 1.5701255282162766e-06], ["marginal heating grid projection updated - CONSQ", -0.009154251912550239]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.00816860351443792], ["autoclave - CONSQ", -0.0050337016375417085], ["market for corrugated board box", -0.00019329161513200805], ["packaging film production, low density polyethylene", 0.0012730945337941888], ["market for polypropylene, granulate", 0.002750892066170575], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.00021279553450212322], ["market for polypropylene, granulate", -0.0014854817157459717], ["market for electricity, high voltage", -6.915515673764167e-06], ["transport Plastic - CONSQ", 0.00023580918814396272], ["PE incineration no Energy Recovery - CONSQ", 1.317126382953847e-07], ["PP incineration no Energy Recovery - CONSQ", 7.222577462919841e-07], ["marginal heating grid projection updated - CONSQ", -0.0042109558797614206]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.002334714686429374], ["alubox production - CONSQ", 0.003071740429498711], ["autoclave - CONSQ", 0.3712100048184407], ["Handwash - CONSQ", 0.017318120822377946], ["alubox EoL melting - CONSQ", 0.0011909714387468016], ["alubox EoL mixed sorting - CONSQ", 2.52013836223735e-05], ["transport Alu - CONSQ", 8.898246414492742e-05], ["avoided alubox raw materials - CONSQ", -0.0019446684188544406]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.005127791570007857], ["autoclave - CONSQ", 0.3712100048184407], ["market for corrugated board box", 0.00769024222237969], ["packaging film production, low density polyethylene", 0.0011214908538673086], ["market for polypropylene, granulate", 0.0020736297474166663], ["market for electricity, high voltage", -0.02960764092131087], ["transport Plastic - CONSQ", 0.002924785747056368], ["PE incineration no Energy Recovery - CONSQ", -6.92648548515381e-06], ["PP incineration no Energy Recovery - CONSQ", -5.013513201684267e-05], ["marginal heating grid projection updated - CONSQ", -0.04382531537631146]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.005127791570007857], ["autoclave - CONSQ", 0.3712100048184407], ["market for corrugated board box", 0.00769024222237969], ["packaging film production, low density polyethylene", 0.0011214908538673086], ["market for polypropylene, granulate", 0.0020736297474166663], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.00013435578904063823], ["market for polypropylene, granulate", -0.0011197600630719088], ["market for electricity, high voltage", -0.013619514823803198], ["transport Plastic - CONSQ", 0.002924785747056368], ["PE incineration no Energy Recovery - CONSQ", -3.1861833221186155e-06], ["PP incineration no Energy Recovery - CONSQ", -2.306216067010477e-05], ["marginal heating grid projection updated - CONSQ", -0.02015964507236595]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.002701247943326531], ["alubox production - CONSQ", 0.0002572924700333938], ["autoclave - CONSQ", 0.0012409999199104874], ["Handwash - CONSQ", 0.00037346125659892565], ["alubox EoL melting - CONSQ", 0.0016443236333685011], ["alubox EoL mixed sorting - CONSQ", 0.00024798070202281094], ["transport Alu - CONSQ", 9.387436924279312e-06], ["avoided alubox raw materials - CONSQ", -0.002299553382649486]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.00027852080704722363], ["autoclave - CONSQ", 0.0012409999199104874], ["market for corrugated board box", 1.4358495269997662e-05], ["packaging film production, low density polyethylene", 3.0265462195767782e-05], ["market for polypropylene, granulate", 0.0001883616490990964], ["market for electricity, high voltage", -7.804085909302624e-05], ["transport Plastic - CONSQ", 0.0005351351661778195], ["PE incineration no Energy Recovery - CONSQ", 2.8330989961623315e-06], ["PP incineration no Energy Recovery - CONSQ", 2.306474777885249e-05], ["marginal heating grid projection updated - CONSQ", -0.0001424373546744192]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.00027852080704722363], ["autoclave - CONSQ", 0.0012409999199104874], ["market for corrugated board box", 1.4358495269997662e-05], ["packaging film production, low density polyethylene", 3.0265462195767782e-05], ["market for polypropylene, granulate", 0.0001883616490990964], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -9.1367656341591e-06], ["market for polypropylene, granulate", -0.00010171529052578622], ["market for electricity, high voltage", -3.589879518232533e-05], ["transport Plastic - CONSQ", 0.0005351351661778195], ["PE incineration no Energy Recovery - CONSQ", 1.3032255388436012e-06], ["PP incineration no Energy Recovery - CONSQ", 1.0609783976981098e-05], ["marginal heating grid projection updated - CONSQ", -6.552118315558796e-05]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 3.005247744207215e-08], ["alubox production - CONSQ", 6.7557037325842665e-09], ["autoclave - CONSQ", 3.7977946695091095e-07], ["Handwash - CONSQ", 8.840767116093183e-08], ["alubox EoL melting - CONSQ", 2.30962570646764e-08], ["alubox EoL mixed sorting - CONSQ", 2.9826205287214324e-10], ["transport Alu - CONSQ", 9.717378819636507e-10], ["avoided alubox raw materials - CONSQ", -2.7911719772239275e-08]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 3.2635340952323063e-08], ["autoclave - CONSQ", 3.7977946695091095e-07], ["market for corrugated board box", 2.7834470776847915e-09], ["packaging film production, low density polyethylene", 4.2284699991133815e-09], ["market for polypropylene, granulate", 1.3893127747635222e-08], ["market for electricity, high voltage", -2.8427305229240823e-08], ["transport Plastic - CONSQ", 1.848104771149103e-08], ["PE incineration no Energy Recovery - CONSQ", 2.358692474437959e-09], ["PP incineration no Energy Recovery - CONSQ", 1.725654569019887e-08], ["marginal heating grid projection updated - CONSQ", -7.096087531430904e-08]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 3.2635340952323063e-08], ["autoclave - CONSQ", 3.7977946695091095e-07], ["market for corrugated board box", 2.7834470776847915e-09], ["packaging film production, low density polyethylene", 4.2284699991133815e-09], ["market for polypropylene, granulate", 1.3893127747635222e-08], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -1.767432103351432e-09], ["market for polypropylene, granulate", -7.502288983978914e-09], ["market for electricity, high voltage", -1.3076560405451121e-08], ["transport Plastic - CONSQ", 1.848104771149103e-08], ["PE incineration no Energy Recovery - CONSQ", 1.0849985382369117e-09], ["PP incineration no Energy Recovery - CONSQ", 7.938011017599437e-09], ["marginal heating grid projection updated - CONSQ", -3.264200264425988e-08]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.0003320543296888726], ["alubox production - CONSQ", 4.162180470938677e-05], ["autoclave - CONSQ", 0.00026490567079616174], ["Handwash - CONSQ", 3.96833649130533e-05], ["alubox EoL melting - CONSQ", 0.000269443750223278], ["alubox EoL mixed sorting - CONSQ", 7.353934229761277e-06], ["transport Alu - CONSQ", 1.8259531686334647e-06], ["avoided alubox raw materials - CONSQ", -0.00030326437197377115]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.000308673215149162], ["autoclave - CONSQ", 0.00026490567079616174], ["market for corrugated board box", 1.9898656197765445e-05], ["packaging film production, low density polyethylene", 3.3140475682123626e-05], ["market for polypropylene, granulate", 0.00017282185237223164], ["market for electricity, high voltage", -2.231079196579252e-05], ["transport Plastic - CONSQ", 0.00013190421511387288], ["PE incineration no Energy Recovery - CONSQ", 7.002033471167449e-07], ["PP incineration no Energy Recovery - CONSQ", 5.29286539044413e-06], ["marginal heating grid projection updated - CONSQ", -0.00013466525500075482]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.000308673215149162], ["autoclave - CONSQ", 0.00026490567079616174], ["market for corrugated board box", 1.9898656197765445e-05], ["packaging film production, low density polyethylene", 3.3140475682123626e-05], ["market for polypropylene, granulate", 0.00017282185237223164], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -1.1414481711249861e-05], ["market for polypropylene, granulate", -9.332380028186167e-05], ["market for electricity, high voltage", -1.0262964304264338e-05], ["transport Plastic - CONSQ", 0.00013190421511387288], ["PE incineration no Energy Recovery - CONSQ", 3.220935396306108e-07], ["PP incineration no Energy Recovery - CONSQ", 2.434718080607002e-06], ["marginal heating grid projection updated - CONSQ", -6.194601729696267e-05]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.0004063397665523169], ["alubox production - CONSQ", 4.14067532662198e-05], ["autoclave - CONSQ", 0.0010409637092836518], ["Handwash - CONSQ", 5.6548055094571396e-05], ["alubox EoL melting - CONSQ", 0.0003492472950974516], ["alubox EoL mixed sorting - CONSQ", 8.31969883499261e-06], ["transport Alu - CONSQ", 4.0007846526209655e-06], ["avoided alubox raw materials - CONSQ", -0.0003787683220887762]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0005273455625662271], ["autoclave - CONSQ", 0.0010409637092836518], ["market for corrugated board box", 1.992769356693832e-05], ["packaging film production, low density polyethylene", 5.9443267000911506e-05], ["market for polypropylene, granulate", 0.00035807878978268956], ["market for electricity, high voltage", -7.38730784244868e-05], ["transport Plastic - CONSQ", 0.0006302261652615024], ["PE incineration no Energy Recovery - CONSQ", 4.926923049878476e-06], ["PP incineration no Energy Recovery - CONSQ", 3.618208230836772e-05], ["marginal heating grid projection updated - CONSQ", -0.0002938144434138714]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0005273455625662271], ["autoclave - CONSQ", 0.0010409637092836518], ["market for corrugated board box", 1.992769356693832e-05], ["packaging film production, low density polyethylene", 5.9443267000911506e-05], ["market for polypropylene, granulate", 0.00035807878978268956], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -2.413578050392533e-05], ["market for polypropylene, granulate", -0.00019336254648702426], ["market for electricity, high voltage", -3.398161607526445e-05], ["transport Plastic - CONSQ", 0.0006302261652615024], ["PE incineration no Energy Recovery - CONSQ", 2.2663846029159648e-06], ["PP incineration no Energy Recovery - CONSQ", 1.6643757863047444e-05], ["marginal heating grid projection updated - CONSQ", -0.00013515464396732214]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.0004174314215672984], ["alubox production - CONSQ", 4.455709483824816e-05], ["autoclave - CONSQ", 0.0010810568688617995], ["Handwash - CONSQ", 6.0111120837377276e-05], ["alubox EoL melting - CONSQ", 0.0003572829696987736], ["alubox EoL mixed sorting - CONSQ", 9.19609131640861e-06], ["transport Alu - CONSQ", 4.469502235457776e-06], ["avoided alubox raw materials - CONSQ", -0.00038880630329081315]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0005618338162167878], ["autoclave - CONSQ", 0.0010810568688617995], ["market for corrugated board box", 2.0791114125169064e-05], ["packaging film production, low density polyethylene", 6.631010854578887e-05], ["market for polypropylene, granulate", 0.0003874341887574365], ["market for electricity, high voltage", -7.549524825901237e-05], ["transport Plastic - CONSQ", 0.0006448392063673025], ["PE incineration no Energy Recovery - CONSQ", 4.978085137060835e-06], ["PP incineration no Energy Recovery - CONSQ", 3.657478512948533e-05], ["marginal heating grid projection updated - CONSQ", -0.00031050560622047045]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0005618338162167878], ["autoclave - CONSQ", 0.0010810568688617995], ["market for corrugated board box", 2.0791114125169064e-05], ["packaging film production, low density polyethylene", 6.631010854578887e-05], ["market for polypropylene, granulate", 0.0003874341887574365], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -2.626816623045106e-05], ["market for polypropylene, granulate", -0.00020921446193377323], ["market for electricity, high voltage", -3.472781419914618e-05], ["transport Plastic - CONSQ", 0.0006448392063673025], ["PE incineration no Energy Recovery - CONSQ", 2.289919163020383e-06], ["PP incineration no Energy Recovery - CONSQ", 1.682440116081574e-05], ["marginal heating grid projection updated - CONSQ", -0.00014283257885826928]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.0008992513694695894], ["alubox production - CONSQ", 0.0005956497772618558], ["autoclave - CONSQ", 0.0010491539253294014], ["Handwash - CONSQ", 0.0012331033794999353], ["alubox EoL melting - CONSQ", 0.0007991235636674024], ["alubox EoL mixed sorting - CONSQ", 1.5581023494370883e-05], ["transport Alu - CONSQ", 3.2068979028450636e-06], ["avoided alubox raw materials - CONSQ", -0.0008368257603027835]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0017577048268882362], ["autoclave - CONSQ", 0.0010491539253294014], ["market for corrugated board box", 4.452670480938243e-05], ["packaging film production, low density polyethylene", 0.0004453940631154319], ["market for polypropylene, granulate", 0.0013656742270238083], ["market for electricity, high voltage", -6.571613819584125e-05], ["transport Plastic - CONSQ", 0.0001399901368854677], ["PE incineration no Energy Recovery - CONSQ", 1.2995259348425692e-05], ["PP incineration no Energy Recovery - CONSQ", 0.00010886201777810881], ["marginal heating grid projection updated - CONSQ", -0.0003887749564590118]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0017577048268882362], ["autoclave - CONSQ", 0.0010491539253294014], ["market for corrugated board box", 4.452670480938243e-05], ["packaging film production, low density polyethylene", 0.0004453940631154319], ["market for polypropylene, granulate", 0.0013656742270238083], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -9.681672037336444e-05], ["market for polypropylene, granulate", -0.0007374640825936914], ["market for electricity, high voltage", -3.022942357008819e-05], ["transport Plastic - CONSQ", 0.0001399901368854677], ["PE incineration no Energy Recovery - CONSQ", 5.977819300256769e-06], ["PP incineration no Energy Recovery - CONSQ", 5.0076528179147716e-05], ["marginal heating grid projection updated - CONSQ", -0.00017883647996782967]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 7.145511606017238e-10], ["alubox production - CONSQ", 1.3869501200915352e-10], ["autoclave - CONSQ", 6.359176888816591e-09], ["Handwash - CONSQ", 4.578694169887924e-10], ["alubox EoL melting - CONSQ", 5.905331620351393e-10], ["alubox EoL mixed sorting - CONSQ", 1.5417827147409675e-11], ["transport Alu - CONSQ", 8.901644163947479e-12], ["avoided alubox raw materials - CONSQ", -6.603331676291806e-10]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 9.779412202518208e-10], ["autoclave - CONSQ", 6.359176888816591e-09], ["market for corrugated board box", 1.1794556259477375e-10], ["packaging film production, low density polyethylene", 1.170938746744889e-10], ["market for polypropylene, granulate", 7.022637416929262e-10], ["market for electricity, high voltage", -4.908234227492671e-10], ["transport Plastic - CONSQ", 3.654842686388018e-10], ["PE incineration no Energy Recovery - CONSQ", 8.847708585680705e-11], ["PP incineration no Energy Recovery - CONSQ", 6.472481534959679e-10], ["marginal heating grid projection updated - CONSQ", -1.2507461984615217e-09]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 9.779412202518208e-10], ["autoclave - CONSQ", 6.359176888816591e-09], ["market for corrugated board box", 1.1794556259477375e-10], ["packaging film production, low density polyethylene", 1.170938746744889e-10], ["market for polypropylene, granulate", 7.022637416929262e-10], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -4.504933857243854e-11], ["market for polypropylene, granulate", -3.7922242051256395e-10], ["market for electricity, high voltage", -2.257787744646651e-10], ["transport Plastic - CONSQ", 3.654842686388018e-10], ["PE incineration no Energy Recovery - CONSQ", 4.069945949406622e-11], ["PP incineration no Energy Recovery - CONSQ", 2.977341506106811e-10], ["marginal heating grid projection updated - CONSQ", -5.75343251279769e-10]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 5.130522229115747e-07], ["alubox production - CONSQ", 7.093019284325974e-08], ["autoclave - CONSQ", 1.194075047433503e-06], ["Handwash - CONSQ", 1.0084812172960556e-07], ["alubox EoL melting - CONSQ", 3.9911264677716495e-07], ["alubox EoL mixed sorting - CONSQ", -2.3126096513853413e-08], ["transport Alu - CONSQ", 3.7184982526857473e-09], ["avoided alubox raw materials - CONSQ", -4.677134627961323e-07]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 4.776176836426269e-07], ["autoclave - CONSQ", 1.194075047433503e-06], ["market for corrugated board box", 2.817720799829456e-08], ["packaging film production, low density polyethylene", 5.4114387208721576e-08], ["market for polypropylene, granulate", 3.1711419718869685e-07], ["market for electricity, high voltage", -8.98781834307783e-08], ["transport Plastic - CONSQ", 1.5684385091232697e-07], ["PE incineration no Energy Recovery - CONSQ", 3.3270721500014945e-08], ["PP incineration no Energy Recovery - CONSQ", 2.435057792429553e-07], ["marginal heating grid projection updated - CONSQ", -3.6179419004034245e-07]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 4.776176836426269e-07], ["autoclave - CONSQ", 1.194075047433503e-06], ["market for corrugated board box", 2.817720799829456e-08], ["packaging film production, low density polyethylene", 5.4114387208721576e-08], ["market for polypropylene, granulate", 3.1711419718869685e-07], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -2.078429016806353e-08], ["market for polypropylene, granulate", -1.7124166648320043e-07], ["market for electricity, high voltage", -4.1343964378157976e-08], ["transport Plastic - CONSQ", 1.5684385091232697e-07], ["PE incineration no Energy Recovery - CONSQ", 1.5304531889941912e-08], ["PP incineration no Energy Recovery - CONSQ", 1.1201265845323309e-07], ["marginal heating grid projection updated - CONSQ", -1.6642532741375974e-07]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.006562198476923313], ["alubox production - CONSQ", 0.0019874487680275146], ["autoclave - CONSQ", 0.022816718689192224], ["Handwash - CONSQ", 0.0012265531905278374], ["alubox EoL melting - CONSQ", 0.004906635595617432], ["alubox EoL mixed sorting - CONSQ", 0.00018111150871818652], ["transport Alu - CONSQ", 0.00029171235845180504], ["avoided alubox raw materials - CONSQ", -0.00600187868824489]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.06208002195669975], ["autoclave - CONSQ", 0.022816718689192224], ["market for corrugated board box", 0.00034641083188185725], ["packaging film production, low density polyethylene", 0.0069955286848791725], ["market for polypropylene, granulate", 0.05843815230566258], ["market for electricity, high voltage", -0.0004919641621372878], ["transport Plastic - CONSQ", 0.006809478292203344], ["PE incineration no Energy Recovery - CONSQ", 3.8003274428101495e-05], ["PP incineration no Energy Recovery - CONSQ", 0.0002823387264368425], ["marginal heating grid projection updated - CONSQ", -0.0137675922069433]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.06208002195669975], ["autoclave - CONSQ", 0.022816718689192224], ["market for corrugated board box", 0.00034641083188185725], ["packaging film production, low density polyethylene", 0.0069955286848791725], ["market for polypropylene, granulate", 0.05843815230566258], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.0035487768262253317], ["market for polypropylene, granulate", -0.03155660224543658], ["market for electricity, high voltage", -0.00022630351458306547], ["transport Plastic - CONSQ", 0.006809478292203344], ["PE incineration no Energy Recovery - CONSQ", 1.7481506237108085e-05], ["PP incineration no Energy Recovery - CONSQ", 0.0001298758141807338], ["marginal heating grid projection updated - CONSQ", -0.006333092415158893]]</t>
+    <t>[["alubox raw materials - CONSQ", 0.0006775653291065658], ["alubox production - CONSQ", 6.629550605703986e-05], ["autoclave - CONSQ", 0.0008168335310893735], ["Handwash - CONSQ", 8.905836307234447e-05], ["alubox EoL melting - CONSQ", 0.0005884192389845013], ["alubox EoL mixed sorting - CONSQ", 8.562634890094533e-06], ["transport Alu - CONSQ", 3.2287762067324436e-06], ["avoided alubox raw materials - CONSQ", -0.0006339914261712349]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0005945666947861479], ["autoclave - CONSQ", 0.0008168335310893735], ["market for corrugated board box", 2.5837221571970654e-05], ["packaging film production, low density polyethylene", 6.376674759785153e-05], ["market for polypropylene, granulate", 0.0004018382259604529], ["transport Plastic - CONSQ", 0.0002956106906493175], ["PE incineration no Energy Recovery - CONSQ", 2.0365809447114344e-06], ["PP incineration no Energy Recovery - CONSQ", 1.5021306205522168e-05], ["marginal heating grid projection updated - CONSQ", -0.0002201749276808098], ["energy avoided electricity from energy recovery - CONSQ", -6.503997452470033e-05]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0005945666947861479], ["autoclave - CONSQ", 0.0008168335310893735], ["market for corrugated board box", 2.5837221571970654e-05], ["packaging film production, low density polyethylene", 6.376674759785153e-05], ["market for polypropylene, granulate", 0.0004018382259604529], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -2.5817207918465817e-05], ["market for polypropylene, granulate", -0.00021699264202029305], ["transport Plastic - CONSQ", 0.0002956106906493175], ["PE incineration no Energy Recovery - CONSQ", 9.368272344186168e-07], ["PP incineration no Energy Recovery - CONSQ", 6.9098008584871945e-06], ["marginal heating grid projection updated - CONSQ", -0.00010128046672699861], ["energy avoided electricity from energy recovery - CONSQ", -2.9918388278524232e-05]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.1606541147279832], ["alubox production - CONSQ", 0.028319177385852747], ["autoclave - CONSQ", 0.951491752712585], ["Handwash - CONSQ", 0.05319504805443418], ["alubox EoL melting - CONSQ", 0.13518326770711395], ["alubox EoL mixed sorting - CONSQ", 0.0033103760097333134], ["transport Alu - CONSQ", 0.002207018918299616], ["avoided alubox raw materials - CONSQ", -0.1489866020639352]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.24557815914822093], ["autoclave - CONSQ", 0.951491752712585], ["market for corrugated board box", 0.013204980950018264], ["packaging film production, low density polyethylene", 0.028359676338399035], ["market for polypropylene, granulate", 0.18813136805414704], ["transport Plastic - CONSQ", 0.06422041919175978], ["PE incineration no Energy Recovery - CONSQ", 0.030386037915928737], ["PP incineration no Energy Recovery - CONSQ", 0.22226110454865183], ["marginal heating grid projection updated - CONSQ", -0.26715655420230033], ["energy avoided electricity from energy recovery - CONSQ", -0.046891313255269886]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.24557815914822093], ["autoclave - CONSQ", 0.951491752712585], ["market for corrugated board box", 0.013204980950018264], ["packaging film production, low density polyethylene", 0.028359676338399035], ["market for polypropylene, granulate", 0.18813136805414704], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.011961150087913522], ["market for polypropylene, granulate", -0.10159093874999724], ["transport Plastic - CONSQ", 0.06422041919175978], ["PE incineration no Energy Recovery - CONSQ", 0.013977577441317958], ["PP incineration no Energy Recovery - CONSQ", 0.10224010809278757], ["marginal heating grid projection updated - CONSQ", -0.12289201493247397], ["energy avoided electricity from energy recovery - CONSQ", -0.021570004097008932]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.004857366127607231], ["alubox production - CONSQ", 0.0017893668035763928], ["autoclave - CONSQ", 0.04265337205533771], ["Handwash - CONSQ", 0.0015115580587554038], ["alubox EoL melting - CONSQ", 0.0017729271055850976], ["alubox EoL mixed sorting - CONSQ", 0.0008989760159071156], ["transport Alu - CONSQ", 5.9933956949511586e-05], ["avoided alubox raw materials - CONSQ", -0.004217495270216258]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.006412384202480646], ["autoclave - CONSQ", 0.04265337205533771], ["market for corrugated board box", 0.0002611840476741577], ["packaging film production, low density polyethylene", 0.0006539456792695441], ["market for polypropylene, granulate", 0.0031418480748664867], ["transport Plastic - CONSQ", 0.0022784241061617775], ["PE incineration no Energy Recovery - CONSQ", 0.0015856286240025085], ["PP incineration no Energy Recovery - CONSQ", 0.01160246020836475], ["marginal heating grid projection updated - CONSQ", -0.005950773213116322], ["energy avoided electricity from energy recovery - CONSQ", -0.0020057900262043286]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.006412384202480646], ["autoclave - CONSQ", 0.04265337205533771], ["market for corrugated board box", 0.0002611840476741577], ["packaging film production, low density polyethylene", 0.0006539456792695441], ["market for polypropylene, granulate", 0.0031418480748664867], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.00020579922897293133], ["market for polypropylene, granulate", -0.0016965979604118935], ["transport Plastic - CONSQ", 0.0022784241061617775], ["PE incineration no Energy Recovery - CONSQ", 0.000729389167037291], ["PP incineration no Energy Recovery - CONSQ", 0.005337131695939611], ["marginal heating grid projection updated - CONSQ", -0.0027373556778708856], ["energy avoided electricity from energy recovery - CONSQ", -0.00092266341199534]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.006751992919021646], ["alubox production - CONSQ", 0.002350846866942384], ["autoclave - CONSQ", 0.05250688721886437], ["Handwash - CONSQ", 0.0017407759897446976], ["alubox EoL melting - CONSQ", 0.00250038866506771], ["alubox EoL mixed sorting - CONSQ", 0.0011115381053412958], ["transport Alu - CONSQ", 0.00010128822661857403], ["avoided alubox raw materials - CONSQ", -0.005873426730001119]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.008523811730064883], ["autoclave - CONSQ", 0.05250688721886437], ["market for corrugated board box", 0.0003621664954644836], ["packaging film production, low density polyethylene", 0.0008697010162811554], ["market for polypropylene, granulate", 0.0042630945982127105], ["transport Plastic - CONSQ", 0.003058344480539131], ["PE incineration no Energy Recovery - CONSQ", 0.002295784818493442], ["PP incineration no Energy Recovery - CONSQ", 0.016797606943600895], ["marginal heating grid projection updated - CONSQ", -0.0076281740416686665], ["energy avoided electricity from energy recovery - CONSQ", -0.002542831428074748]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.008523811730064883], ["autoclave - CONSQ", 0.05250688721886437], ["market for corrugated board box", 0.0003621664954644836], ["packaging film production, low density polyethylene", 0.0008697010162811554], ["market for polypropylene, granulate", 0.0042630945982127105], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.00027891919263887786], ["market for polypropylene, granulate", -0.0023020710830179395], ["transport Plastic - CONSQ", 0.003058344480539131], ["PE incineration no Energy Recovery - CONSQ", 0.001056061016501626], ["PP incineration no Energy Recovery - CONSQ", 0.007726899194182712], ["marginal heating grid projection updated - CONSQ", -0.0035089600589448613], ["energy avoided electricity from energy recovery - CONSQ", -0.0011697024568341412]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.37590231532980395], ["alubox production - CONSQ", 0.12963524353325898], ["autoclave - CONSQ", 2.7968043187588876], ["Handwash - CONSQ", 0.11127611691466276], ["alubox EoL melting - CONSQ", -0.09392069856090877], ["alubox EoL mixed sorting - CONSQ", 0.020102297426764334], ["transport Alu - CONSQ", 0.0414482092699488], ["avoided alubox raw materials - CONSQ", -0.2819864416918137]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.8401285404878711], ["autoclave - CONSQ", 2.7968043187588876], ["market for corrugated board box", 0.03017058176478913], ["packaging film production, low density polyethylene", 0.07006761610492501], ["market for polypropylene, granulate", 0.5179952808941972], ["transport Plastic - CONSQ", 0.2440501915808282], ["PE incineration no Energy Recovery - CONSQ", 0.08828092784937608], ["PP incineration no Energy Recovery - CONSQ", 0.645791444449976], ["marginal heating grid projection updated - CONSQ", -0.5986092475406855], ["energy avoided electricity from energy recovery - CONSQ", -0.07220570855774466]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.8401285404878711], ["autoclave - CONSQ", 2.7968043187588876], ["market for corrugated board box", 0.03017058176478913], ["packaging film production, low density polyethylene", 0.07006761610492501], ["market for polypropylene, granulate", 0.5179952808941972], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.034323148728948046], ["market for polypropylene, granulate", -0.27971745168817114], ["transport Plastic - CONSQ", 0.2440501915808282], ["PE incineration no Energy Recovery - CONSQ", 0.040609226809388936], ["PP incineration no Energy Recovery - CONSQ", 0.29706406447184264], ["marginal heating grid projection updated - CONSQ", -0.275360253824699], ["energy avoided electricity from energy recovery - CONSQ", -0.03321462592344643]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.03486045202148191], ["alubox production - CONSQ", 0.00691237484230511], ["autoclave - CONSQ", 0.06318683131251852], ["Handwash - CONSQ", 0.003951347006992205], ["alubox EoL melting - CONSQ", 0.028782771938786065], ["alubox EoL mixed sorting - CONSQ", 0.0008417001437573078], ["transport Alu - CONSQ", 0.0006922450866505672], ["avoided alubox raw materials - CONSQ", -0.03229125436570311]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.15748810249852832], ["autoclave - CONSQ", 0.06318683131251852], ["market for corrugated board box", 0.0014061075334226376], ["packaging film production, low density polyethylene", 0.017987128602816135], ["market for polypropylene, granulate", 0.14340516514392737], ["transport Plastic - CONSQ", 0.017610524731499436], ["PE incineration no Energy Recovery - CONSQ", 0.00011028712725592124], ["PP incineration no Energy Recovery - CONSQ", 0.0008223426079052385], ["marginal heating grid projection updated - CONSQ", -0.0403447055322068], ["energy avoided electricity from energy recovery - CONSQ", -0.011123241862946782]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.15748810249852832], ["autoclave - CONSQ", 0.06318683131251852], ["market for corrugated board box", 0.0014061075334226376], ["packaging film production, low density polyethylene", 0.017987128602816135], ["market for polypropylene, granulate", 0.14340516514392737], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.008778008074957903], ["market for polypropylene, granulate", -0.07743878917855443], ["transport Plastic - CONSQ", 0.017610524731499436], ["PE incineration no Energy Recovery - CONSQ", 5.0732078535285136e-05], ["PP incineration no Energy Recovery - CONSQ", 0.00037827759972380403], ["marginal heating grid projection updated - CONSQ", -0.01855856454469089], ["energy avoided electricity from energy recovery - CONSQ", -0.005116691256838774]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 5.674689072285325e-05], ["alubox production - CONSQ", 1.3998613324046819e-05], ["autoclave - CONSQ", 3.532670383594245e-05], ["Handwash - CONSQ", 0.0001876352812167408], ["alubox EoL melting - CONSQ", 4.490172565453172e-05], ["alubox EoL mixed sorting - CONSQ", 2.9158068823253486e-06], ["transport Alu - CONSQ", 2.1648705354488862e-07], ["avoided alubox raw materials - CONSQ", -5.145723028021371e-05]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 4.645599491009539e-05], ["autoclave - CONSQ", 3.532670383594245e-05], ["market for corrugated board box", 6.06066020511809e-06], ["packaging film production, low density polyethylene", 6.4122449313985585e-06], ["market for polypropylene, granulate", 1.964683665613263e-05], ["transport Plastic - CONSQ", 1.366601800400479e-05], ["PE incineration no Energy Recovery - CONSQ", 4.700623402183256e-08], ["PP incineration no Energy Recovery - CONSQ", 3.7261413267369015e-07], ["marginal heating grid projection updated - CONSQ", -2.316923707377802e-05], ["energy avoided electricity from energy recovery - CONSQ", -1.5548089004116344e-05]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 4.645599491009539e-05], ["autoclave - CONSQ", 3.532670383594245e-05], ["market for corrugated board box", 6.06066020511809e-06], ["packaging film production, low density polyethylene", 6.4122449313985585e-06], ["market for polypropylene, granulate", 1.964683665613263e-05], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -1.3837296222243698e-06], ["market for polypropylene, granulate", -1.060929179428487e-05], ["transport Plastic - CONSQ", 1.366601800400479e-05], ["PE incineration no Energy Recovery - CONSQ", 2.162286764289093e-08], ["PP incineration no Energy Recovery - CONSQ", 1.714025012280218e-07], ["marginal heating grid projection updated - CONSQ", -1.0657849053595463e-05], ["energy avoided electricity from energy recovery - CONSQ", -7.152120941739769e-06]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 3.8073056985077197e-06], ["alubox production - CONSQ", 2.2529251969022175e-06], ["autoclave - CONSQ", 4.150004783270754e-05], ["Handwash - CONSQ", 9.585919244733559e-05], ["alubox EoL melting - CONSQ", 3.2952848522127418e-06], ["alubox EoL mixed sorting - CONSQ", 1.277667644041824e-07], ["transport Alu - CONSQ", 5.890105739136465e-08], ["avoided alubox raw materials - CONSQ", -3.5259461573087766e-06]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 5.488323122627126e-06], ["autoclave - CONSQ", 4.150004783270754e-05], ["market for corrugated board box", 3.8612259228844765e-07], ["packaging film production, low density polyethylene", 8.931098200818854e-07], ["market for polypropylene, granulate", 2.3047807636825643e-06], ["transport Plastic - CONSQ", 1.5857185356624875e-06], ["PE incineration no Energy Recovery - CONSQ", 4.725445040985872e-08], ["PP incineration no Energy Recovery - CONSQ", 3.4690323686799765e-07], ["marginal heating grid projection updated - CONSQ", -2.0408849538946707e-06], ["energy avoided electricity from energy recovery - CONSQ", -1.113048716267988e-06]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 5.488323122627126e-06], ["autoclave - CONSQ", 4.150004783270754e-05], ["market for corrugated board box", 3.8612259228844765e-07], ["packaging film production, low density polyethylene", 8.931098200818854e-07], ["market for polypropylene, granulate", 2.3047807636825643e-06], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -1.536964550964375e-07], ["market for polypropylene, granulate", -1.2445816124297446e-06], ["transport Plastic - CONSQ", 1.5857185356624875e-06], ["PE incineration no Energy Recovery - CONSQ", 2.173704718861357e-08], ["PP incineration no Energy Recovery - CONSQ", 1.5957548897553483e-07], ["marginal heating grid projection updated - CONSQ", -9.388070787757505e-07], ["energy avoided electricity from energy recovery - CONSQ", -5.120024094613718e-07]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.03618091952126559], ["alubox production - CONSQ", 0.0028029186315702923], ["autoclave - CONSQ", 0.012800098451075], ["Handwash - CONSQ", 0.0032059514159326285], ["alubox EoL melting - CONSQ", 0.026681396735130477], ["alubox EoL mixed sorting - CONSQ", -0.010000873466737073], ["transport Alu - CONSQ", 2.893699126617276e-05], ["avoided alubox raw materials - CONSQ", -0.03219876077542022]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0064594240812074245], ["autoclave - CONSQ", 0.012800098451075], ["market for corrugated board box", 0.0003079234064602862], ["packaging film production, low density polyethylene", 0.0007490979899267339], ["market for polypropylene, granulate", 0.004290057233679009], ["transport Plastic - CONSQ", 0.001352133426883247], ["PE incineration no Energy Recovery - CONSQ", 7.043862153350928e-05], ["PP incineration no Energy Recovery - CONSQ", 0.0005141072547452981], ["marginal heating grid projection updated - CONSQ", -0.0022590076585288854], ["energy avoided electricity from energy recovery - CONSQ", -0.0014347985237476446]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0064594240812074245], ["autoclave - CONSQ", 0.012800098451075], ["market for corrugated board box", 0.0003079234064602862], ["packaging film production, low density polyethylene", 0.0007490979899267339], ["market for polypropylene, granulate", 0.004290057233679009], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.0003578493652562967], ["market for polypropylene, granulate", -0.0023166309062040437], ["transport Plastic - CONSQ", 0.001352133426883247], ["PE incineration no Energy Recovery - CONSQ", 3.240176590339967e-05], ["PP incineration no Energy Recovery - CONSQ", 0.0002364893372302118], ["marginal heating grid projection updated - CONSQ", -0.0010391435228385947], ["energy avoided electricity from energy recovery - CONSQ", -0.000660007320896239]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.14399189342316263], ["alubox production - CONSQ", 0.03422369552688528], ["autoclave - CONSQ", 0.4323705765596624], ["Handwash - CONSQ", 0.05715192797802266], ["alubox EoL melting - CONSQ", 0.06007316862662303], ["alubox EoL mixed sorting - CONSQ", 0.010255781168013862], ["transport Alu - CONSQ", 0.0018208619430123908], ["avoided alubox raw materials - CONSQ", -0.13069794728819595]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.13081523573786313], ["autoclave - CONSQ", 0.4323705765596624], ["market for corrugated board box", 0.00997482064110965], ["packaging film production, low density polyethylene", 0.0150342046587877], ["market for polypropylene, granulate", 0.07156715003699723], ["transport Plastic - CONSQ", 0.03911631107193289], ["PE incineration no Energy Recovery - CONSQ", 0.019130751398476024], ["PP incineration no Energy Recovery - CONSQ", 0.13997609610997214], ["marginal heating grid projection updated - CONSQ", -0.08974728055050814], ["energy avoided electricity from energy recovery - CONSQ", -0.03328575843243604]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.13081523573786313], ["autoclave - CONSQ", 0.4323705765596624], ["market for corrugated board box", 0.00997482064110965], ["packaging film production, low density polyethylene", 0.0150342046587877], ["market for polypropylene, granulate", 0.07156715003699723], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.0047580063349078935], ["market for polypropylene, granulate", -0.038646261019972594], ["transport Plastic - CONSQ", 0.03911631107193289], ["PE incineration no Energy Recovery - CONSQ", 0.008800145643187277], ["PP incineration no Energy Recovery - CONSQ", 0.06438900421316206], ["marginal heating grid projection updated - CONSQ", -0.04128374904888525], ["energy avoided electricity from energy recovery - CONSQ", -0.01531144887736553]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.000506292862798092], ["alubox production - CONSQ", 0.0018303628175715477], ["autoclave - CONSQ", -0.005033701645044582], ["Handwash - CONSQ", 0.001604099655210045], ["alubox EoL melting - CONSQ", 0.001078928618394637], ["alubox EoL mixed sorting - CONSQ", -0.00014209540003861791], ["transport Alu - CONSQ", 9.39356990358891e-06], ["avoided alubox raw materials - CONSQ", -0.000564655330090803]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.008168603514405631], ["autoclave - CONSQ", -0.005033701645044582], ["market for corrugated board box", -0.00019329161513200805], ["packaging film production, low density polyethylene", 0.0012730945337941888], ["market for polypropylene, granulate", 0.002750892066170575], ["transport Plastic - CONSQ", 0.00023580918818004765], ["PE incineration no Energy Recovery - CONSQ", 2.863318231305701e-07], ["PP incineration no Energy Recovery - CONSQ", 1.57012553059987e-06], ["marginal heating grid projection updated - CONSQ", -0.009154251912576522], ["energy avoided electricity from energy recovery - CONSQ", -0.0001198218696774197]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.008168603514405631], ["autoclave - CONSQ", -0.005033701645044582], ["market for corrugated board box", -0.00019329161513200805], ["packaging film production, low density polyethylene", 0.0012730945337941888], ["market for polypropylene, granulate", 0.002750892066170575], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.00021279553450212322], ["market for polypropylene, granulate", -0.0014854817157459717], ["transport Plastic - CONSQ", 0.00023580918818004765], ["PE incineration no Energy Recovery - CONSQ", 1.3171263840340642e-07], ["PP incineration no Energy Recovery - CONSQ", 7.222577478423296e-07], ["marginal heating grid projection updated - CONSQ", -0.004210955879782235], ["energy avoided electricity from energy recovery - CONSQ", -5.511806004607783e-05]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0023347146882327493], ["alubox production - CONSQ", 0.0030717404189460357], ["autoclave - CONSQ", 0.37121000470614174], ["Handwash - CONSQ", 0.017318123631340672], ["alubox EoL melting - CONSQ", 0.0011909714409841466], ["alubox EoL mixed sorting - CONSQ", 2.520138302956028e-05], ["transport Alu - CONSQ", 8.89824641790565e-05], ["avoided alubox raw materials - CONSQ", -0.0019446684301437586]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.005127791514639285], ["autoclave - CONSQ", 0.37121000470614174], ["market for corrugated board box", 0.00769024222237969], ["packaging film production, low density polyethylene", 0.0011214908538673086], ["market for polypropylene, granulate", 0.0020736297474166663], ["transport Plastic - CONSQ", 0.0029247857466888367], ["PE incineration no Energy Recovery - CONSQ", -6.926485452912442e-06], ["PP incineration no Energy Recovery - CONSQ", -5.0135132081062274e-05], ["marginal heating grid projection updated - CONSQ", -0.04382531537327047], ["energy avoided electricity from energy recovery - CONSQ", -0.0032705765199335293]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.005127791514639285], ["autoclave - CONSQ", 0.37121000470614174], ["market for corrugated board box", 0.00769024222237969], ["packaging film production, low density polyethylene", 0.0011214908538673086], ["market for polypropylene, granulate", 0.0020736297474166663], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.00013435578904063823], ["market for polypropylene, granulate", -0.0011197600630719088], ["transport Plastic - CONSQ", 0.0029247857466888367], ["PE incineration no Energy Recovery - CONSQ", -3.18618331925689e-06], ["PP incineration no Energy Recovery - CONSQ", -2.3062160665635066e-05], ["marginal heating grid projection updated - CONSQ", -0.020159645075861914], ["energy avoided electricity from energy recovery - CONSQ", -0.0015044651989975372]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0027012479429851044], ["alubox production - CONSQ", 0.0002572924703668961], ["autoclave - CONSQ", 0.0012409999221925491], ["Handwash - CONSQ", 0.00037346315266956057], ["alubox EoL melting - CONSQ", 0.0016443236329909312], ["alubox EoL mixed sorting - CONSQ", 0.00024798070199126695], ["transport Alu - CONSQ", 9.387436923989773e-06], ["avoided alubox raw materials - CONSQ", -0.0022995533822968966]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0002785208061929546], ["autoclave - CONSQ", 0.0012409999221925491], ["market for corrugated board box", 1.4358495269997662e-05], ["packaging film production, low density polyethylene", 3.0265462195767782e-05], ["market for polypropylene, granulate", 0.0001883616490990964], ["transport Plastic - CONSQ", 0.000535135166177872], ["PE incineration no Energy Recovery - CONSQ", 2.8330989959435073e-06], ["PP incineration no Energy Recovery - CONSQ", 2.3064747773393e-05], ["marginal heating grid projection updated - CONSQ", -0.0001424373547087525], ["energy avoided electricity from energy recovery - CONSQ", -9.766874498035461e-05]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0002785208061929546], ["autoclave - CONSQ", 0.0012409999221925491], ["market for corrugated board box", 1.4358495269997662e-05], ["packaging film production, low density polyethylene", 3.0265462195767782e-05], ["market for polypropylene, granulate", 0.0001883616490990964], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -9.1367656341591e-06], ["market for polypropylene, granulate", -0.00010171529052578622], ["transport Plastic - CONSQ", 0.000535135166177872], ["PE incineration no Energy Recovery - CONSQ", 1.3032255387669824e-06], ["PP incineration no Energy Recovery - CONSQ", 1.0609783975463249e-05], ["marginal heating grid projection updated - CONSQ", -6.552118317382946e-05], ["energy avoided electricity from energy recovery - CONSQ", -4.4927622642964245e-05]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 3.005247744141417e-08], ["alubox production - CONSQ", 6.7557037336857965e-09], ["autoclave - CONSQ", 3.797794667029101e-07], ["Handwash - CONSQ", 8.840768881625287e-08], ["alubox EoL melting - CONSQ", 2.3096257063345617e-08], ["alubox EoL mixed sorting - CONSQ", 2.982620528658935e-10], ["transport Alu - CONSQ", 9.717378819988433e-10], ["avoided alubox raw materials - CONSQ", -2.791171977130472e-08]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 3.263534094603485e-08], ["autoclave - CONSQ", 3.797794667029101e-07], ["market for corrugated board box", 2.7834470776847915e-09], ["packaging film production, low density polyethylene", 4.2284699991133815e-09], ["market for polypropylene, granulate", 1.3893127747635222e-08], ["transport Plastic - CONSQ", 1.8481047712101694e-08], ["PE incineration no Energy Recovery - CONSQ", 2.3586924744483617e-09], ["PP incineration no Energy Recovery - CONSQ", 1.7256545690238117e-08], ["marginal heating grid projection updated - CONSQ", -7.096087531493722e-08], ["energy avoided electricity from energy recovery - CONSQ", -1.9373846264074528e-08]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 3.263534094603485e-08], ["autoclave - CONSQ", 3.797794667029101e-07], ["market for corrugated board box", 2.7834470776847915e-09], ["packaging film production, low density polyethylene", 4.2284699991133815e-09], ["market for polypropylene, granulate", 1.3893127747635222e-08], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -1.767432103351432e-09], ["market for polypropylene, granulate", -7.502288983978914e-09], ["transport Plastic - CONSQ", 1.8481047712101694e-08], ["PE incineration no Energy Recovery - CONSQ", 1.0849985382408151e-09], ["PP incineration no Energy Recovery - CONSQ", 7.938011017648697e-09], ["marginal heating grid projection updated - CONSQ", -3.264200264465228e-08], ["energy avoided electricity from energy recovery - CONSQ", -8.911969281356175e-09]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0003320543296807067], ["alubox production - CONSQ", 4.162180472246632e-05], ["autoclave - CONSQ", 0.0002649056683111777], ["Handwash - CONSQ", 3.968346390530431e-05], ["alubox EoL melting - CONSQ", 0.00026944375020867444], ["alubox EoL mixed sorting - CONSQ", 7.353934229343672e-06], ["transport Alu - CONSQ", 1.8259531689458998e-06], ["avoided alubox raw materials - CONSQ", -0.00030326437196262165]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.00030867321509145385], ["autoclave - CONSQ", 0.0002649056683111777], ["market for corrugated board box", 1.9898656197765445e-05], ["packaging film production, low density polyethylene", 3.3140475682123626e-05], ["market for polypropylene, granulate", 0.00017282185237223164], ["transport Plastic - CONSQ", 0.0001319042151189609], ["PE incineration no Energy Recovery - CONSQ", 7.002033472130834e-07], ["PP incineration no Energy Recovery - CONSQ", 5.29286539079212e-06], ["marginal heating grid projection updated - CONSQ", -0.00013466525500775844], ["energy avoided electricity from energy recovery - CONSQ", -2.4808563489243707e-05]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.00030867321509145385], ["autoclave - CONSQ", 0.0002649056683111777], ["market for corrugated board box", 1.9898656197765445e-05], ["packaging film production, low density polyethylene", 3.3140475682123626e-05], ["market for polypropylene, granulate", 0.00017282185237223164], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -1.1414481711249861e-05], ["market for polypropylene, granulate", -9.332380028186167e-05], ["transport Plastic - CONSQ", 0.0001319042151189609], ["PE incineration no Energy Recovery - CONSQ", 3.220935396690695e-07], ["PP incineration no Energy Recovery - CONSQ", 2.4347180810882727e-06], ["marginal heating grid projection updated - CONSQ", -6.194601730055737e-05], ["energy avoided electricity from energy recovery - CONSQ", -1.1411939204017445e-05]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.00040633976653621723], ["alubox production - CONSQ", 4.140675327984576e-05], ["autoclave - CONSQ", 0.0010409637066292495], ["Handwash - CONSQ", 5.654824487875126e-05], ["alubox EoL melting - CONSQ", 0.00034924729507403813], ["alubox EoL mixed sorting - CONSQ", 8.319698834302502e-06], ["transport Alu - CONSQ", 4.0007846530023785e-06], ["avoided alubox raw materials - CONSQ", -0.00037876832207002395]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0005273455624694649], ["autoclave - CONSQ", 0.0010409637066292495], ["market for corrugated board box", 1.992769356693832e-05], ["packaging film production, low density polyethylene", 5.9443267000911506e-05], ["market for polypropylene, granulate", 0.00035807878978268956], ["transport Plastic - CONSQ", 0.0006302261652680697], ["PE incineration no Energy Recovery - CONSQ", 4.926923049985816e-06], ["PP incineration no Energy Recovery - CONSQ", 3.6182082308653207e-05], ["marginal heating grid projection updated - CONSQ", -0.0002938144434229266], ["energy avoided electricity from energy recovery - CONSQ", -5.947311356692644e-05]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0005273455624694649], ["autoclave - CONSQ", 0.0010409637066292495], ["market for corrugated board box", 1.992769356693832e-05], ["packaging film production, low density polyethylene", 5.9443267000911506e-05], ["market for polypropylene, granulate", 0.00035807878978268956], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -2.413578050392533e-05], ["market for polypropylene, granulate", -0.00019336254648702426], ["transport Plastic - CONSQ", 0.0006302261652680697], ["PE incineration no Energy Recovery - CONSQ", 2.2663846029444954e-06], ["PP incineration no Energy Recovery - CONSQ", 1.6643757863469158e-05], ["marginal heating grid projection updated - CONSQ", -0.0001351546439723567], ["energy avoided electricity from energy recovery - CONSQ", -2.735763223914729e-05]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.00041743142154986496], ["alubox production - CONSQ", 4.455709485172259e-05], ["autoclave - CONSQ", 0.0010810568661097698], ["Handwash - CONSQ", 6.0111317114538656e-05], ["alubox EoL melting - CONSQ", 0.00035728296967379975], ["alubox EoL mixed sorting - CONSQ", 9.196091315614561e-06], ["transport Alu - CONSQ", 4.469502235853217e-06], ["avoided alubox raw materials - CONSQ", -0.00038880630327067035]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0005618338161144837], ["autoclave - CONSQ", 0.0010810568661097698], ["market for corrugated board box", 2.0791114125169064e-05], ["packaging film production, low density polyethylene", 6.631010854578887e-05], ["market for polypropylene, granulate", 0.0003874341887574365], ["transport Plastic - CONSQ", 0.0006448392063739959], ["PE incineration no Energy Recovery - CONSQ", 4.978085137171641e-06], ["PP incineration no Energy Recovery - CONSQ", 3.657478512976802e-05], ["marginal heating grid projection updated - CONSQ", -0.0003105056062297907], ["energy avoided electricity from energy recovery - CONSQ", -6.125043464493624e-05]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0005618338161144837], ["autoclave - CONSQ", 0.0010810568661097698], ["market for corrugated board box", 2.0791114125169064e-05], ["packaging film production, low density polyethylene", 6.631010854578887e-05], ["market for polypropylene, granulate", 0.0003874341887574365], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -2.626816623045106e-05], ["market for polypropylene, granulate", -0.00020921446193377323], ["transport Plastic - CONSQ", 0.0006448392063739959], ["PE incineration no Energy Recovery - CONSQ", 2.2899191630480137e-06], ["PP incineration no Energy Recovery - CONSQ", 1.6824401161239685e-05], ["marginal heating grid projection updated - CONSQ", -0.0001428325788634346], ["energy avoided electricity from energy recovery - CONSQ", -2.817519993492104e-05]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0008992513694317904], ["alubox production - CONSQ", 0.0005956497772846476], ["autoclave - CONSQ", 0.0010491539223125314], ["Handwash - CONSQ", 0.0012331036187721658], ["alubox EoL melting - CONSQ", 0.0007991235636232352], ["alubox EoL mixed sorting - CONSQ", 1.558102349115015e-05], ["transport Alu - CONSQ", 3.206897903186722e-06], ["avoided alubox raw materials - CONSQ", -0.0008368257602620459]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0017577048267277756], ["autoclave - CONSQ", 0.0010491539223125314], ["market for corrugated board box", 4.452670480938243e-05], ["packaging film production, low density polyethylene", 0.0004453940631154319], ["market for polypropylene, granulate", 0.0013656742270238083], ["transport Plastic - CONSQ", 0.00013999013688847947], ["PE incineration no Energy Recovery - CONSQ", 1.2995259348525339e-05], ["PP incineration no Energy Recovery - CONSQ", 0.00010886201777815281], ["marginal heating grid projection updated - CONSQ", -0.00038877495646860363], ["energy avoided electricity from energy recovery - CONSQ", -8.563263478252755e-05]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.0017577048267277756], ["autoclave - CONSQ", 0.0010491539223125314], ["market for corrugated board box", 4.452670480938243e-05], ["packaging film production, low density polyethylene", 0.0004453940631154319], ["market for polypropylene, granulate", 0.0013656742270238083], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -9.681672037336444e-05], ["market for polypropylene, granulate", -0.0007374640825936914], ["transport Plastic - CONSQ", 0.00013999013688847947], ["PE incineration no Energy Recovery - CONSQ", 5.977819300287237e-06], ["PP incineration no Energy Recovery - CONSQ", 5.00765281795766e-05], ["marginal heating grid projection updated - CONSQ", -0.0001788364799730058], ["energy avoided electricity from energy recovery - CONSQ", -3.939101199813133e-05]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 7.145511605928252e-10], ["alubox production - CONSQ", 1.3869501194519183e-10], ["autoclave - CONSQ", 6.359176882956889e-09], ["Handwash - CONSQ", 4.5786969314653276e-10], ["alubox EoL melting - CONSQ", 5.905331620176393e-10], ["alubox EoL mixed sorting - CONSQ", 1.5417827140968123e-11], ["transport Alu - CONSQ", 8.901644164889872e-12], ["avoided alubox raw materials - CONSQ", -6.603331676990763e-10]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 9.779412196160193e-10], ["autoclave - CONSQ", 6.359176882956889e-09], ["market for corrugated board box", 1.1794556259477375e-10], ["packaging film production, low density polyethylene", 1.170938746744889e-10], ["market for polypropylene, granulate", 7.022637416929262e-10], ["transport Plastic - CONSQ", 3.654842686466822e-10], ["PE incineration no Energy Recovery - CONSQ", 8.847708585728578e-11], ["PP incineration no Energy Recovery - CONSQ", 6.472481534960111e-10], ["marginal heating grid projection updated - CONSQ", -1.2507461984480972e-09], ["energy avoided electricity from energy recovery - CONSQ", -1.9490446672639282e-10]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 9.779412196160193e-10], ["autoclave - CONSQ", 6.359176882956889e-09], ["market for corrugated board box", 1.1794556259477375e-10], ["packaging film production, low density polyethylene", 1.170938746744889e-10], ["market for polypropylene, granulate", 7.022637416929262e-10], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -4.504933857243854e-11], ["market for polypropylene, granulate", -3.7922242051256395e-10], ["transport Plastic - CONSQ", 3.654842686466822e-10], ["PE incineration no Energy Recovery - CONSQ", 4.069945949416738e-11], ["PP incineration no Energy Recovery - CONSQ", 2.9773415061165006e-10], ["marginal heating grid projection updated - CONSQ", -5.753432513189246e-10], ["energy avoided electricity from energy recovery - CONSQ", -8.965605469032296e-11]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 5.130522228988051e-07], ["alubox production - CONSQ", 7.093019286187184e-08], ["autoclave - CONSQ", 1.1940750438112246e-06], ["Handwash - CONSQ", 1.008483100123822e-07], ["alubox EoL melting - CONSQ", 3.9911264675527085e-07], ["alubox EoL mixed sorting - CONSQ", -2.3126096514517695e-08], ["transport Alu - CONSQ", 3.7184982531464856e-09], ["avoided alubox raw materials - CONSQ", -4.677134627791185e-07]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 4.776176835497813e-07], ["autoclave - CONSQ", 1.1940750438112246e-06], ["market for corrugated board box", 2.817720799829456e-08], ["packaging film production, low density polyethylene", 5.4114387208721576e-08], ["market for polypropylene, granulate", 3.1711419718869685e-07], ["transport Plastic - CONSQ", 1.5684385092005196e-07], ["PE incineration no Energy Recovery - CONSQ", 3.327072150015725e-08], ["PP incineration no Energy Recovery - CONSQ", 2.435057792434667e-07], ["marginal heating grid projection updated - CONSQ", -3.6179419004955235e-07], ["energy avoided electricity from energy recovery - CONSQ", -7.171018951458978e-08]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 4.776176835497813e-07], ["autoclave - CONSQ", 1.1940750438112246e-06], ["market for corrugated board box", 2.817720799829456e-08], ["packaging film production, low density polyethylene", 5.4114387208721576e-08], ["market for polypropylene, granulate", 3.1711419718869685e-07], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -2.078429016806353e-08], ["market for polypropylene, granulate", -1.7124166648320043e-07], ["transport Plastic - CONSQ", 1.5684385092005196e-07], ["PE incineration no Energy Recovery - CONSQ", 1.530453189000074e-08], ["PP incineration no Energy Recovery - CONSQ", 1.120126584539537e-07], ["marginal heating grid projection updated - CONSQ", -1.6642532741907996e-07], ["energy avoided electricity from energy recovery - CONSQ", -3.2986687175223885e-08]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.006562198476463859], ["alubox production - CONSQ", 0.0019874487681881105], ["autoclave - CONSQ", 0.022816718652521273], ["Handwash - CONSQ", 0.0012265568040732602], ["alubox EoL melting - CONSQ", 0.004906635595038445], ["alubox EoL mixed sorting - CONSQ", 0.00018111150869155272], ["transport Alu - CONSQ", 0.00029171235845780854], ["avoided alubox raw materials - CONSQ", -0.006001878687753108]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.06208002195471321], ["autoclave - CONSQ", 0.022816718652521273], ["market for corrugated board box", 0.00034641083188185725], ["packaging film production, low density polyethylene", 0.0069955286848791725], ["market for polypropylene, granulate", 0.05843815230566258], ["transport Plastic - CONSQ", 0.006809478292298527], ["PE incineration no Energy Recovery - CONSQ", 3.8003274429607946e-05], ["PP incineration no Energy Recovery - CONSQ", 0.00028233872643720486], ["marginal heating grid projection updated - CONSQ", -0.01376759220708353], ["energy avoided electricity from energy recovery - CONSQ", -0.0022377285914058245]]</t>
+  </si>
+  <si>
+    <t>[["pp production - CONSQ", 0.06208002195471321], ["autoclave - CONSQ", 0.022816718652521273], ["market for corrugated board box", 0.00034641083188185725], ["packaging film production, low density polyethylene", 0.0069955286848791725], ["market for polypropylene, granulate", 0.05843815230566258], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.0035487768262253317], ["market for polypropylene, granulate", -0.03155660224543658], ["transport Plastic - CONSQ", 0.006809478292298527], ["PE incineration no Energy Recovery - CONSQ", 1.7481506237070754e-05], ["PP incineration no Energy Recovery - CONSQ", 0.00012987581418344327], ["marginal heating grid projection updated - CONSQ", -0.006333092415231067], ["energy avoided electricity from energy recovery - CONSQ", -0.0010293551519985013]]</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
modified:   Brighway/LCA_plots.py 	modified:   Brighway/Ofir.ipynb 	modified:   Brighway/Results/Ananas - CONSQ_recipe.xlsx 	modified:   Brighway/Single-use-vs-multi-use-in-health-care/Results/GWP_life_stage_CONSQ.jpg 	new file:   Brighway/Single-use-vs-multi-use-in-health-care/Results/_GWP_life_stage_pr_scenario_CONSQ.jpg 	modified:   Brighway/Single-use-vs-multi-use-in-health-care/Results/scaled_impact_score_multi_CONSQ_ReCiPe 2016 v1.03, endpoint (H).jpg 	modified:   Brighway/Single-use-vs-multi-use-in-health-care/Results/scaled_impact_score_multi_CONSQ_ReCiPe 2016 v1.03, midpoint (H).jpg 	modified:   Brighway/Stine.ipynb 	modified:   Brighway/__pycache__/LCA_plots.cpython-311.pyc 	modified:   Brighway/__pycache__/life_cycle_assessment.cpython-311.pyc 	modified:   Brighway/df_idx_ofir_CONSQ 	modified:   Brighway/life_cycle_assessment.py 	new file:   Brighway/process.ipynb
</commit_message>
<xml_diff>
--- a/Brighway/Results/Ananas - CONSQ_recipe.xlsx
+++ b/Brighway/Results/Ananas - CONSQ_recipe.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="189">
   <si>
     <t>('ReCiPe 2016 v1.03, midpoint (H)', 'acidification: terrestrial', 'terrestrial acidification potential (TAP)')</t>
   </si>
@@ -79,193 +79,508 @@
     <t>('ReCiPe 2016 v1.03, endpoint (H)', 'total: natural resources', 'natural resources')</t>
   </si>
   <si>
-    <t>[["alubox raw materials - CONSQ", 0.0006775653291065658], ["alubox production - CONSQ", 6.629550605703986e-05], ["autoclave - CONSQ", 0.0008168335310893735], ["Handwash - CONSQ", 8.905836307234447e-05], ["alubox EoL melting - CONSQ", 0.0005884192389845013], ["alubox EoL mixed sorting - CONSQ", 8.562634890094533e-06], ["transport Alu - CONSQ", 3.2287762067324436e-06], ["avoided alubox raw materials - CONSQ", -0.0006339914261712349]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0005945666947861479], ["autoclave - CONSQ", 0.0008168335310893735], ["market for corrugated board box", 2.5837221571970654e-05], ["packaging film production, low density polyethylene", 6.376674759785153e-05], ["market for polypropylene, granulate", 0.0004018382259604529], ["transport Plastic - CONSQ", 0.0002956106906493175], ["PE incineration no Energy Recovery - CONSQ", 2.0365809447114344e-06], ["PP incineration no Energy Recovery - CONSQ", 1.5021306205522168e-05], ["marginal heating grid projection updated - CONSQ", -0.0002201749276808098], ["energy avoided electricity from energy recovery - CONSQ", -6.503997452470033e-05]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0005945666947861479], ["autoclave - CONSQ", 0.0008168335310893735], ["market for corrugated board box", 2.5837221571970654e-05], ["packaging film production, low density polyethylene", 6.376674759785153e-05], ["market for polypropylene, granulate", 0.0004018382259604529], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -2.5817207918465817e-05], ["market for polypropylene, granulate", -0.00021699264202029305], ["transport Plastic - CONSQ", 0.0002956106906493175], ["PE incineration no Energy Recovery - CONSQ", 9.368272344186168e-07], ["PP incineration no Energy Recovery - CONSQ", 6.9098008584871945e-06], ["marginal heating grid projection updated - CONSQ", -0.00010128046672699861], ["energy avoided electricity from energy recovery - CONSQ", -2.9918388278524232e-05]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.1606541147279832], ["alubox production - CONSQ", 0.028319177385852747], ["autoclave - CONSQ", 0.951491752712585], ["Handwash - CONSQ", 0.05319504805443418], ["alubox EoL melting - CONSQ", 0.13518326770711395], ["alubox EoL mixed sorting - CONSQ", 0.0033103760097333134], ["transport Alu - CONSQ", 0.002207018918299616], ["avoided alubox raw materials - CONSQ", -0.1489866020639352]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.24557815914822093], ["autoclave - CONSQ", 0.951491752712585], ["market for corrugated board box", 0.013204980950018264], ["packaging film production, low density polyethylene", 0.028359676338399035], ["market for polypropylene, granulate", 0.18813136805414704], ["transport Plastic - CONSQ", 0.06422041919175978], ["PE incineration no Energy Recovery - CONSQ", 0.030386037915928737], ["PP incineration no Energy Recovery - CONSQ", 0.22226110454865183], ["marginal heating grid projection updated - CONSQ", -0.26715655420230033], ["energy avoided electricity from energy recovery - CONSQ", -0.046891313255269886]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.24557815914822093], ["autoclave - CONSQ", 0.951491752712585], ["market for corrugated board box", 0.013204980950018264], ["packaging film production, low density polyethylene", 0.028359676338399035], ["market for polypropylene, granulate", 0.18813136805414704], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.011961150087913522], ["market for polypropylene, granulate", -0.10159093874999724], ["transport Plastic - CONSQ", 0.06422041919175978], ["PE incineration no Energy Recovery - CONSQ", 0.013977577441317958], ["PP incineration no Energy Recovery - CONSQ", 0.10224010809278757], ["marginal heating grid projection updated - CONSQ", -0.12289201493247397], ["energy avoided electricity from energy recovery - CONSQ", -0.021570004097008932]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.004857366127607231], ["alubox production - CONSQ", 0.0017893668035763928], ["autoclave - CONSQ", 0.04265337205533771], ["Handwash - CONSQ", 0.0015115580587554038], ["alubox EoL melting - CONSQ", 0.0017729271055850976], ["alubox EoL mixed sorting - CONSQ", 0.0008989760159071156], ["transport Alu - CONSQ", 5.9933956949511586e-05], ["avoided alubox raw materials - CONSQ", -0.004217495270216258]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.006412384202480646], ["autoclave - CONSQ", 0.04265337205533771], ["market for corrugated board box", 0.0002611840476741577], ["packaging film production, low density polyethylene", 0.0006539456792695441], ["market for polypropylene, granulate", 0.0031418480748664867], ["transport Plastic - CONSQ", 0.0022784241061617775], ["PE incineration no Energy Recovery - CONSQ", 0.0015856286240025085], ["PP incineration no Energy Recovery - CONSQ", 0.01160246020836475], ["marginal heating grid projection updated - CONSQ", -0.005950773213116322], ["energy avoided electricity from energy recovery - CONSQ", -0.0020057900262043286]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.006412384202480646], ["autoclave - CONSQ", 0.04265337205533771], ["market for corrugated board box", 0.0002611840476741577], ["packaging film production, low density polyethylene", 0.0006539456792695441], ["market for polypropylene, granulate", 0.0031418480748664867], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.00020579922897293133], ["market for polypropylene, granulate", -0.0016965979604118935], ["transport Plastic - CONSQ", 0.0022784241061617775], ["PE incineration no Energy Recovery - CONSQ", 0.000729389167037291], ["PP incineration no Energy Recovery - CONSQ", 0.005337131695939611], ["marginal heating grid projection updated - CONSQ", -0.0027373556778708856], ["energy avoided electricity from energy recovery - CONSQ", -0.00092266341199534]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.006751992919021646], ["alubox production - CONSQ", 0.002350846866942384], ["autoclave - CONSQ", 0.05250688721886437], ["Handwash - CONSQ", 0.0017407759897446976], ["alubox EoL melting - CONSQ", 0.00250038866506771], ["alubox EoL mixed sorting - CONSQ", 0.0011115381053412958], ["transport Alu - CONSQ", 0.00010128822661857403], ["avoided alubox raw materials - CONSQ", -0.005873426730001119]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.008523811730064883], ["autoclave - CONSQ", 0.05250688721886437], ["market for corrugated board box", 0.0003621664954644836], ["packaging film production, low density polyethylene", 0.0008697010162811554], ["market for polypropylene, granulate", 0.0042630945982127105], ["transport Plastic - CONSQ", 0.003058344480539131], ["PE incineration no Energy Recovery - CONSQ", 0.002295784818493442], ["PP incineration no Energy Recovery - CONSQ", 0.016797606943600895], ["marginal heating grid projection updated - CONSQ", -0.0076281740416686665], ["energy avoided electricity from energy recovery - CONSQ", -0.002542831428074748]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.008523811730064883], ["autoclave - CONSQ", 0.05250688721886437], ["market for corrugated board box", 0.0003621664954644836], ["packaging film production, low density polyethylene", 0.0008697010162811554], ["market for polypropylene, granulate", 0.0042630945982127105], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.00027891919263887786], ["market for polypropylene, granulate", -0.0023020710830179395], ["transport Plastic - CONSQ", 0.003058344480539131], ["PE incineration no Energy Recovery - CONSQ", 0.001056061016501626], ["PP incineration no Energy Recovery - CONSQ", 0.007726899194182712], ["marginal heating grid projection updated - CONSQ", -0.0035089600589448613], ["energy avoided electricity from energy recovery - CONSQ", -0.0011697024568341412]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.37590231532980395], ["alubox production - CONSQ", 0.12963524353325898], ["autoclave - CONSQ", 2.7968043187588876], ["Handwash - CONSQ", 0.11127611691466276], ["alubox EoL melting - CONSQ", -0.09392069856090877], ["alubox EoL mixed sorting - CONSQ", 0.020102297426764334], ["transport Alu - CONSQ", 0.0414482092699488], ["avoided alubox raw materials - CONSQ", -0.2819864416918137]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.8401285404878711], ["autoclave - CONSQ", 2.7968043187588876], ["market for corrugated board box", 0.03017058176478913], ["packaging film production, low density polyethylene", 0.07006761610492501], ["market for polypropylene, granulate", 0.5179952808941972], ["transport Plastic - CONSQ", 0.2440501915808282], ["PE incineration no Energy Recovery - CONSQ", 0.08828092784937608], ["PP incineration no Energy Recovery - CONSQ", 0.645791444449976], ["marginal heating grid projection updated - CONSQ", -0.5986092475406855], ["energy avoided electricity from energy recovery - CONSQ", -0.07220570855774466]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.8401285404878711], ["autoclave - CONSQ", 2.7968043187588876], ["market for corrugated board box", 0.03017058176478913], ["packaging film production, low density polyethylene", 0.07006761610492501], ["market for polypropylene, granulate", 0.5179952808941972], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.034323148728948046], ["market for polypropylene, granulate", -0.27971745168817114], ["transport Plastic - CONSQ", 0.2440501915808282], ["PE incineration no Energy Recovery - CONSQ", 0.040609226809388936], ["PP incineration no Energy Recovery - CONSQ", 0.29706406447184264], ["marginal heating grid projection updated - CONSQ", -0.275360253824699], ["energy avoided electricity from energy recovery - CONSQ", -0.03321462592344643]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.03486045202148191], ["alubox production - CONSQ", 0.00691237484230511], ["autoclave - CONSQ", 0.06318683131251852], ["Handwash - CONSQ", 0.003951347006992205], ["alubox EoL melting - CONSQ", 0.028782771938786065], ["alubox EoL mixed sorting - CONSQ", 0.0008417001437573078], ["transport Alu - CONSQ", 0.0006922450866505672], ["avoided alubox raw materials - CONSQ", -0.03229125436570311]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.15748810249852832], ["autoclave - CONSQ", 0.06318683131251852], ["market for corrugated board box", 0.0014061075334226376], ["packaging film production, low density polyethylene", 0.017987128602816135], ["market for polypropylene, granulate", 0.14340516514392737], ["transport Plastic - CONSQ", 0.017610524731499436], ["PE incineration no Energy Recovery - CONSQ", 0.00011028712725592124], ["PP incineration no Energy Recovery - CONSQ", 0.0008223426079052385], ["marginal heating grid projection updated - CONSQ", -0.0403447055322068], ["energy avoided electricity from energy recovery - CONSQ", -0.011123241862946782]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.15748810249852832], ["autoclave - CONSQ", 0.06318683131251852], ["market for corrugated board box", 0.0014061075334226376], ["packaging film production, low density polyethylene", 0.017987128602816135], ["market for polypropylene, granulate", 0.14340516514392737], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.008778008074957903], ["market for polypropylene, granulate", -0.07743878917855443], ["transport Plastic - CONSQ", 0.017610524731499436], ["PE incineration no Energy Recovery - CONSQ", 5.0732078535285136e-05], ["PP incineration no Energy Recovery - CONSQ", 0.00037827759972380403], ["marginal heating grid projection updated - CONSQ", -0.01855856454469089], ["energy avoided electricity from energy recovery - CONSQ", -0.005116691256838774]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 5.674689072285325e-05], ["alubox production - CONSQ", 1.3998613324046819e-05], ["autoclave - CONSQ", 3.532670383594245e-05], ["Handwash - CONSQ", 0.0001876352812167408], ["alubox EoL melting - CONSQ", 4.490172565453172e-05], ["alubox EoL mixed sorting - CONSQ", 2.9158068823253486e-06], ["transport Alu - CONSQ", 2.1648705354488862e-07], ["avoided alubox raw materials - CONSQ", -5.145723028021371e-05]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 4.645599491009539e-05], ["autoclave - CONSQ", 3.532670383594245e-05], ["market for corrugated board box", 6.06066020511809e-06], ["packaging film production, low density polyethylene", 6.4122449313985585e-06], ["market for polypropylene, granulate", 1.964683665613263e-05], ["transport Plastic - CONSQ", 1.366601800400479e-05], ["PE incineration no Energy Recovery - CONSQ", 4.700623402183256e-08], ["PP incineration no Energy Recovery - CONSQ", 3.7261413267369015e-07], ["marginal heating grid projection updated - CONSQ", -2.316923707377802e-05], ["energy avoided electricity from energy recovery - CONSQ", -1.5548089004116344e-05]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 4.645599491009539e-05], ["autoclave - CONSQ", 3.532670383594245e-05], ["market for corrugated board box", 6.06066020511809e-06], ["packaging film production, low density polyethylene", 6.4122449313985585e-06], ["market for polypropylene, granulate", 1.964683665613263e-05], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -1.3837296222243698e-06], ["market for polypropylene, granulate", -1.060929179428487e-05], ["transport Plastic - CONSQ", 1.366601800400479e-05], ["PE incineration no Energy Recovery - CONSQ", 2.162286764289093e-08], ["PP incineration no Energy Recovery - CONSQ", 1.714025012280218e-07], ["marginal heating grid projection updated - CONSQ", -1.0657849053595463e-05], ["energy avoided electricity from energy recovery - CONSQ", -7.152120941739769e-06]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 3.8073056985077197e-06], ["alubox production - CONSQ", 2.2529251969022175e-06], ["autoclave - CONSQ", 4.150004783270754e-05], ["Handwash - CONSQ", 9.585919244733559e-05], ["alubox EoL melting - CONSQ", 3.2952848522127418e-06], ["alubox EoL mixed sorting - CONSQ", 1.277667644041824e-07], ["transport Alu - CONSQ", 5.890105739136465e-08], ["avoided alubox raw materials - CONSQ", -3.5259461573087766e-06]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 5.488323122627126e-06], ["autoclave - CONSQ", 4.150004783270754e-05], ["market for corrugated board box", 3.8612259228844765e-07], ["packaging film production, low density polyethylene", 8.931098200818854e-07], ["market for polypropylene, granulate", 2.3047807636825643e-06], ["transport Plastic - CONSQ", 1.5857185356624875e-06], ["PE incineration no Energy Recovery - CONSQ", 4.725445040985872e-08], ["PP incineration no Energy Recovery - CONSQ", 3.4690323686799765e-07], ["marginal heating grid projection updated - CONSQ", -2.0408849538946707e-06], ["energy avoided electricity from energy recovery - CONSQ", -1.113048716267988e-06]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 5.488323122627126e-06], ["autoclave - CONSQ", 4.150004783270754e-05], ["market for corrugated board box", 3.8612259228844765e-07], ["packaging film production, low density polyethylene", 8.931098200818854e-07], ["market for polypropylene, granulate", 2.3047807636825643e-06], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -1.536964550964375e-07], ["market for polypropylene, granulate", -1.2445816124297446e-06], ["transport Plastic - CONSQ", 1.5857185356624875e-06], ["PE incineration no Energy Recovery - CONSQ", 2.173704718861357e-08], ["PP incineration no Energy Recovery - CONSQ", 1.5957548897553483e-07], ["marginal heating grid projection updated - CONSQ", -9.388070787757505e-07], ["energy avoided electricity from energy recovery - CONSQ", -5.120024094613718e-07]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.03618091952126559], ["alubox production - CONSQ", 0.0028029186315702923], ["autoclave - CONSQ", 0.012800098451075], ["Handwash - CONSQ", 0.0032059514159326285], ["alubox EoL melting - CONSQ", 0.026681396735130477], ["alubox EoL mixed sorting - CONSQ", -0.010000873466737073], ["transport Alu - CONSQ", 2.893699126617276e-05], ["avoided alubox raw materials - CONSQ", -0.03219876077542022]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0064594240812074245], ["autoclave - CONSQ", 0.012800098451075], ["market for corrugated board box", 0.0003079234064602862], ["packaging film production, low density polyethylene", 0.0007490979899267339], ["market for polypropylene, granulate", 0.004290057233679009], ["transport Plastic - CONSQ", 0.001352133426883247], ["PE incineration no Energy Recovery - CONSQ", 7.043862153350928e-05], ["PP incineration no Energy Recovery - CONSQ", 0.0005141072547452981], ["marginal heating grid projection updated - CONSQ", -0.0022590076585288854], ["energy avoided electricity from energy recovery - CONSQ", -0.0014347985237476446]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0064594240812074245], ["autoclave - CONSQ", 0.012800098451075], ["market for corrugated board box", 0.0003079234064602862], ["packaging film production, low density polyethylene", 0.0007490979899267339], ["market for polypropylene, granulate", 0.004290057233679009], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.0003578493652562967], ["market for polypropylene, granulate", -0.0023166309062040437], ["transport Plastic - CONSQ", 0.001352133426883247], ["PE incineration no Energy Recovery - CONSQ", 3.240176590339967e-05], ["PP incineration no Energy Recovery - CONSQ", 0.0002364893372302118], ["marginal heating grid projection updated - CONSQ", -0.0010391435228385947], ["energy avoided electricity from energy recovery - CONSQ", -0.000660007320896239]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.14399189342316263], ["alubox production - CONSQ", 0.03422369552688528], ["autoclave - CONSQ", 0.4323705765596624], ["Handwash - CONSQ", 0.05715192797802266], ["alubox EoL melting - CONSQ", 0.06007316862662303], ["alubox EoL mixed sorting - CONSQ", 0.010255781168013862], ["transport Alu - CONSQ", 0.0018208619430123908], ["avoided alubox raw materials - CONSQ", -0.13069794728819595]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.13081523573786313], ["autoclave - CONSQ", 0.4323705765596624], ["market for corrugated board box", 0.00997482064110965], ["packaging film production, low density polyethylene", 0.0150342046587877], ["market for polypropylene, granulate", 0.07156715003699723], ["transport Plastic - CONSQ", 0.03911631107193289], ["PE incineration no Energy Recovery - CONSQ", 0.019130751398476024], ["PP incineration no Energy Recovery - CONSQ", 0.13997609610997214], ["marginal heating grid projection updated - CONSQ", -0.08974728055050814], ["energy avoided electricity from energy recovery - CONSQ", -0.03328575843243604]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.13081523573786313], ["autoclave - CONSQ", 0.4323705765596624], ["market for corrugated board box", 0.00997482064110965], ["packaging film production, low density polyethylene", 0.0150342046587877], ["market for polypropylene, granulate", 0.07156715003699723], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.0047580063349078935], ["market for polypropylene, granulate", -0.038646261019972594], ["transport Plastic - CONSQ", 0.03911631107193289], ["PE incineration no Energy Recovery - CONSQ", 0.008800145643187277], ["PP incineration no Energy Recovery - CONSQ", 0.06438900421316206], ["marginal heating grid projection updated - CONSQ", -0.04128374904888525], ["energy avoided electricity from energy recovery - CONSQ", -0.01531144887736553]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.000506292862798092], ["alubox production - CONSQ", 0.0018303628175715477], ["autoclave - CONSQ", -0.005033701645044582], ["Handwash - CONSQ", 0.001604099655210045], ["alubox EoL melting - CONSQ", 0.001078928618394637], ["alubox EoL mixed sorting - CONSQ", -0.00014209540003861791], ["transport Alu - CONSQ", 9.39356990358891e-06], ["avoided alubox raw materials - CONSQ", -0.000564655330090803]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.008168603514405631], ["autoclave - CONSQ", -0.005033701645044582], ["market for corrugated board box", -0.00019329161513200805], ["packaging film production, low density polyethylene", 0.0012730945337941888], ["market for polypropylene, granulate", 0.002750892066170575], ["transport Plastic - CONSQ", 0.00023580918818004765], ["PE incineration no Energy Recovery - CONSQ", 2.863318231305701e-07], ["PP incineration no Energy Recovery - CONSQ", 1.57012553059987e-06], ["marginal heating grid projection updated - CONSQ", -0.009154251912576522], ["energy avoided electricity from energy recovery - CONSQ", -0.0001198218696774197]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.008168603514405631], ["autoclave - CONSQ", -0.005033701645044582], ["market for corrugated board box", -0.00019329161513200805], ["packaging film production, low density polyethylene", 0.0012730945337941888], ["market for polypropylene, granulate", 0.002750892066170575], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.00021279553450212322], ["market for polypropylene, granulate", -0.0014854817157459717], ["transport Plastic - CONSQ", 0.00023580918818004765], ["PE incineration no Energy Recovery - CONSQ", 1.3171263840340642e-07], ["PP incineration no Energy Recovery - CONSQ", 7.222577478423296e-07], ["marginal heating grid projection updated - CONSQ", -0.004210955879782235], ["energy avoided electricity from energy recovery - CONSQ", -5.511806004607783e-05]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.0023347146882327493], ["alubox production - CONSQ", 0.0030717404189460357], ["autoclave - CONSQ", 0.37121000470614174], ["Handwash - CONSQ", 0.017318123631340672], ["alubox EoL melting - CONSQ", 0.0011909714409841466], ["alubox EoL mixed sorting - CONSQ", 2.520138302956028e-05], ["transport Alu - CONSQ", 8.89824641790565e-05], ["avoided alubox raw materials - CONSQ", -0.0019446684301437586]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.005127791514639285], ["autoclave - CONSQ", 0.37121000470614174], ["market for corrugated board box", 0.00769024222237969], ["packaging film production, low density polyethylene", 0.0011214908538673086], ["market for polypropylene, granulate", 0.0020736297474166663], ["transport Plastic - CONSQ", 0.0029247857466888367], ["PE incineration no Energy Recovery - CONSQ", -6.926485452912442e-06], ["PP incineration no Energy Recovery - CONSQ", -5.0135132081062274e-05], ["marginal heating grid projection updated - CONSQ", -0.04382531537327047], ["energy avoided electricity from energy recovery - CONSQ", -0.0032705765199335293]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.005127791514639285], ["autoclave - CONSQ", 0.37121000470614174], ["market for corrugated board box", 0.00769024222237969], ["packaging film production, low density polyethylene", 0.0011214908538673086], ["market for polypropylene, granulate", 0.0020736297474166663], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.00013435578904063823], ["market for polypropylene, granulate", -0.0011197600630719088], ["transport Plastic - CONSQ", 0.0029247857466888367], ["PE incineration no Energy Recovery - CONSQ", -3.18618331925689e-06], ["PP incineration no Energy Recovery - CONSQ", -2.3062160665635066e-05], ["marginal heating grid projection updated - CONSQ", -0.020159645075861914], ["energy avoided electricity from energy recovery - CONSQ", -0.0015044651989975372]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.0027012479429851044], ["alubox production - CONSQ", 0.0002572924703668961], ["autoclave - CONSQ", 0.0012409999221925491], ["Handwash - CONSQ", 0.00037346315266956057], ["alubox EoL melting - CONSQ", 0.0016443236329909312], ["alubox EoL mixed sorting - CONSQ", 0.00024798070199126695], ["transport Alu - CONSQ", 9.387436923989773e-06], ["avoided alubox raw materials - CONSQ", -0.0022995533822968966]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0002785208061929546], ["autoclave - CONSQ", 0.0012409999221925491], ["market for corrugated board box", 1.4358495269997662e-05], ["packaging film production, low density polyethylene", 3.0265462195767782e-05], ["market for polypropylene, granulate", 0.0001883616490990964], ["transport Plastic - CONSQ", 0.000535135166177872], ["PE incineration no Energy Recovery - CONSQ", 2.8330989959435073e-06], ["PP incineration no Energy Recovery - CONSQ", 2.3064747773393e-05], ["marginal heating grid projection updated - CONSQ", -0.0001424373547087525], ["energy avoided electricity from energy recovery - CONSQ", -9.766874498035461e-05]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0002785208061929546], ["autoclave - CONSQ", 0.0012409999221925491], ["market for corrugated board box", 1.4358495269997662e-05], ["packaging film production, low density polyethylene", 3.0265462195767782e-05], ["market for polypropylene, granulate", 0.0001883616490990964], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -9.1367656341591e-06], ["market for polypropylene, granulate", -0.00010171529052578622], ["transport Plastic - CONSQ", 0.000535135166177872], ["PE incineration no Energy Recovery - CONSQ", 1.3032255387669824e-06], ["PP incineration no Energy Recovery - CONSQ", 1.0609783975463249e-05], ["marginal heating grid projection updated - CONSQ", -6.552118317382946e-05], ["energy avoided electricity from energy recovery - CONSQ", -4.4927622642964245e-05]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 3.005247744141417e-08], ["alubox production - CONSQ", 6.7557037336857965e-09], ["autoclave - CONSQ", 3.797794667029101e-07], ["Handwash - CONSQ", 8.840768881625287e-08], ["alubox EoL melting - CONSQ", 2.3096257063345617e-08], ["alubox EoL mixed sorting - CONSQ", 2.982620528658935e-10], ["transport Alu - CONSQ", 9.717378819988433e-10], ["avoided alubox raw materials - CONSQ", -2.791171977130472e-08]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 3.263534094603485e-08], ["autoclave - CONSQ", 3.797794667029101e-07], ["market for corrugated board box", 2.7834470776847915e-09], ["packaging film production, low density polyethylene", 4.2284699991133815e-09], ["market for polypropylene, granulate", 1.3893127747635222e-08], ["transport Plastic - CONSQ", 1.8481047712101694e-08], ["PE incineration no Energy Recovery - CONSQ", 2.3586924744483617e-09], ["PP incineration no Energy Recovery - CONSQ", 1.7256545690238117e-08], ["marginal heating grid projection updated - CONSQ", -7.096087531493722e-08], ["energy avoided electricity from energy recovery - CONSQ", -1.9373846264074528e-08]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 3.263534094603485e-08], ["autoclave - CONSQ", 3.797794667029101e-07], ["market for corrugated board box", 2.7834470776847915e-09], ["packaging film production, low density polyethylene", 4.2284699991133815e-09], ["market for polypropylene, granulate", 1.3893127747635222e-08], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -1.767432103351432e-09], ["market for polypropylene, granulate", -7.502288983978914e-09], ["transport Plastic - CONSQ", 1.8481047712101694e-08], ["PE incineration no Energy Recovery - CONSQ", 1.0849985382408151e-09], ["PP incineration no Energy Recovery - CONSQ", 7.938011017648697e-09], ["marginal heating grid projection updated - CONSQ", -3.264200264465228e-08], ["energy avoided electricity from energy recovery - CONSQ", -8.911969281356175e-09]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.0003320543296807067], ["alubox production - CONSQ", 4.162180472246632e-05], ["autoclave - CONSQ", 0.0002649056683111777], ["Handwash - CONSQ", 3.968346390530431e-05], ["alubox EoL melting - CONSQ", 0.00026944375020867444], ["alubox EoL mixed sorting - CONSQ", 7.353934229343672e-06], ["transport Alu - CONSQ", 1.8259531689458998e-06], ["avoided alubox raw materials - CONSQ", -0.00030326437196262165]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.00030867321509145385], ["autoclave - CONSQ", 0.0002649056683111777], ["market for corrugated board box", 1.9898656197765445e-05], ["packaging film production, low density polyethylene", 3.3140475682123626e-05], ["market for polypropylene, granulate", 0.00017282185237223164], ["transport Plastic - CONSQ", 0.0001319042151189609], ["PE incineration no Energy Recovery - CONSQ", 7.002033472130834e-07], ["PP incineration no Energy Recovery - CONSQ", 5.29286539079212e-06], ["marginal heating grid projection updated - CONSQ", -0.00013466525500775844], ["energy avoided electricity from energy recovery - CONSQ", -2.4808563489243707e-05]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.00030867321509145385], ["autoclave - CONSQ", 0.0002649056683111777], ["market for corrugated board box", 1.9898656197765445e-05], ["packaging film production, low density polyethylene", 3.3140475682123626e-05], ["market for polypropylene, granulate", 0.00017282185237223164], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -1.1414481711249861e-05], ["market for polypropylene, granulate", -9.332380028186167e-05], ["transport Plastic - CONSQ", 0.0001319042151189609], ["PE incineration no Energy Recovery - CONSQ", 3.220935396690695e-07], ["PP incineration no Energy Recovery - CONSQ", 2.4347180810882727e-06], ["marginal heating grid projection updated - CONSQ", -6.194601730055737e-05], ["energy avoided electricity from energy recovery - CONSQ", -1.1411939204017445e-05]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.00040633976653621723], ["alubox production - CONSQ", 4.140675327984576e-05], ["autoclave - CONSQ", 0.0010409637066292495], ["Handwash - CONSQ", 5.654824487875126e-05], ["alubox EoL melting - CONSQ", 0.00034924729507403813], ["alubox EoL mixed sorting - CONSQ", 8.319698834302502e-06], ["transport Alu - CONSQ", 4.0007846530023785e-06], ["avoided alubox raw materials - CONSQ", -0.00037876832207002395]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0005273455624694649], ["autoclave - CONSQ", 0.0010409637066292495], ["market for corrugated board box", 1.992769356693832e-05], ["packaging film production, low density polyethylene", 5.9443267000911506e-05], ["market for polypropylene, granulate", 0.00035807878978268956], ["transport Plastic - CONSQ", 0.0006302261652680697], ["PE incineration no Energy Recovery - CONSQ", 4.926923049985816e-06], ["PP incineration no Energy Recovery - CONSQ", 3.6182082308653207e-05], ["marginal heating grid projection updated - CONSQ", -0.0002938144434229266], ["energy avoided electricity from energy recovery - CONSQ", -5.947311356692644e-05]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0005273455624694649], ["autoclave - CONSQ", 0.0010409637066292495], ["market for corrugated board box", 1.992769356693832e-05], ["packaging film production, low density polyethylene", 5.9443267000911506e-05], ["market for polypropylene, granulate", 0.00035807878978268956], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -2.413578050392533e-05], ["market for polypropylene, granulate", -0.00019336254648702426], ["transport Plastic - CONSQ", 0.0006302261652680697], ["PE incineration no Energy Recovery - CONSQ", 2.2663846029444954e-06], ["PP incineration no Energy Recovery - CONSQ", 1.6643757863469158e-05], ["marginal heating grid projection updated - CONSQ", -0.0001351546439723567], ["energy avoided electricity from energy recovery - CONSQ", -2.735763223914729e-05]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.00041743142154986496], ["alubox production - CONSQ", 4.455709485172259e-05], ["autoclave - CONSQ", 0.0010810568661097698], ["Handwash - CONSQ", 6.0111317114538656e-05], ["alubox EoL melting - CONSQ", 0.00035728296967379975], ["alubox EoL mixed sorting - CONSQ", 9.196091315614561e-06], ["transport Alu - CONSQ", 4.469502235853217e-06], ["avoided alubox raw materials - CONSQ", -0.00038880630327067035]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0005618338161144837], ["autoclave - CONSQ", 0.0010810568661097698], ["market for corrugated board box", 2.0791114125169064e-05], ["packaging film production, low density polyethylene", 6.631010854578887e-05], ["market for polypropylene, granulate", 0.0003874341887574365], ["transport Plastic - CONSQ", 0.0006448392063739959], ["PE incineration no Energy Recovery - CONSQ", 4.978085137171641e-06], ["PP incineration no Energy Recovery - CONSQ", 3.657478512976802e-05], ["marginal heating grid projection updated - CONSQ", -0.0003105056062297907], ["energy avoided electricity from energy recovery - CONSQ", -6.125043464493624e-05]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0005618338161144837], ["autoclave - CONSQ", 0.0010810568661097698], ["market for corrugated board box", 2.0791114125169064e-05], ["packaging film production, low density polyethylene", 6.631010854578887e-05], ["market for polypropylene, granulate", 0.0003874341887574365], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -2.626816623045106e-05], ["market for polypropylene, granulate", -0.00020921446193377323], ["transport Plastic - CONSQ", 0.0006448392063739959], ["PE incineration no Energy Recovery - CONSQ", 2.2899191630480137e-06], ["PP incineration no Energy Recovery - CONSQ", 1.6824401161239685e-05], ["marginal heating grid projection updated - CONSQ", -0.0001428325788634346], ["energy avoided electricity from energy recovery - CONSQ", -2.817519993492104e-05]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.0008992513694317904], ["alubox production - CONSQ", 0.0005956497772846476], ["autoclave - CONSQ", 0.0010491539223125314], ["Handwash - CONSQ", 0.0012331036187721658], ["alubox EoL melting - CONSQ", 0.0007991235636232352], ["alubox EoL mixed sorting - CONSQ", 1.558102349115015e-05], ["transport Alu - CONSQ", 3.206897903186722e-06], ["avoided alubox raw materials - CONSQ", -0.0008368257602620459]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0017577048267277756], ["autoclave - CONSQ", 0.0010491539223125314], ["market for corrugated board box", 4.452670480938243e-05], ["packaging film production, low density polyethylene", 0.0004453940631154319], ["market for polypropylene, granulate", 0.0013656742270238083], ["transport Plastic - CONSQ", 0.00013999013688847947], ["PE incineration no Energy Recovery - CONSQ", 1.2995259348525339e-05], ["PP incineration no Energy Recovery - CONSQ", 0.00010886201777815281], ["marginal heating grid projection updated - CONSQ", -0.00038877495646860363], ["energy avoided electricity from energy recovery - CONSQ", -8.563263478252755e-05]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.0017577048267277756], ["autoclave - CONSQ", 0.0010491539223125314], ["market for corrugated board box", 4.452670480938243e-05], ["packaging film production, low density polyethylene", 0.0004453940631154319], ["market for polypropylene, granulate", 0.0013656742270238083], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -9.681672037336444e-05], ["market for polypropylene, granulate", -0.0007374640825936914], ["transport Plastic - CONSQ", 0.00013999013688847947], ["PE incineration no Energy Recovery - CONSQ", 5.977819300287237e-06], ["PP incineration no Energy Recovery - CONSQ", 5.00765281795766e-05], ["marginal heating grid projection updated - CONSQ", -0.0001788364799730058], ["energy avoided electricity from energy recovery - CONSQ", -3.939101199813133e-05]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 7.145511605928252e-10], ["alubox production - CONSQ", 1.3869501194519183e-10], ["autoclave - CONSQ", 6.359176882956889e-09], ["Handwash - CONSQ", 4.5786969314653276e-10], ["alubox EoL melting - CONSQ", 5.905331620176393e-10], ["alubox EoL mixed sorting - CONSQ", 1.5417827140968123e-11], ["transport Alu - CONSQ", 8.901644164889872e-12], ["avoided alubox raw materials - CONSQ", -6.603331676990763e-10]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 9.779412196160193e-10], ["autoclave - CONSQ", 6.359176882956889e-09], ["market for corrugated board box", 1.1794556259477375e-10], ["packaging film production, low density polyethylene", 1.170938746744889e-10], ["market for polypropylene, granulate", 7.022637416929262e-10], ["transport Plastic - CONSQ", 3.654842686466822e-10], ["PE incineration no Energy Recovery - CONSQ", 8.847708585728578e-11], ["PP incineration no Energy Recovery - CONSQ", 6.472481534960111e-10], ["marginal heating grid projection updated - CONSQ", -1.2507461984480972e-09], ["energy avoided electricity from energy recovery - CONSQ", -1.9490446672639282e-10]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 9.779412196160193e-10], ["autoclave - CONSQ", 6.359176882956889e-09], ["market for corrugated board box", 1.1794556259477375e-10], ["packaging film production, low density polyethylene", 1.170938746744889e-10], ["market for polypropylene, granulate", 7.022637416929262e-10], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -4.504933857243854e-11], ["market for polypropylene, granulate", -3.7922242051256395e-10], ["transport Plastic - CONSQ", 3.654842686466822e-10], ["PE incineration no Energy Recovery - CONSQ", 4.069945949416738e-11], ["PP incineration no Energy Recovery - CONSQ", 2.9773415061165006e-10], ["marginal heating grid projection updated - CONSQ", -5.753432513189246e-10], ["energy avoided electricity from energy recovery - CONSQ", -8.965605469032296e-11]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 5.130522228988051e-07], ["alubox production - CONSQ", 7.093019286187184e-08], ["autoclave - CONSQ", 1.1940750438112246e-06], ["Handwash - CONSQ", 1.008483100123822e-07], ["alubox EoL melting - CONSQ", 3.9911264675527085e-07], ["alubox EoL mixed sorting - CONSQ", -2.3126096514517695e-08], ["transport Alu - CONSQ", 3.7184982531464856e-09], ["avoided alubox raw materials - CONSQ", -4.677134627791185e-07]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 4.776176835497813e-07], ["autoclave - CONSQ", 1.1940750438112246e-06], ["market for corrugated board box", 2.817720799829456e-08], ["packaging film production, low density polyethylene", 5.4114387208721576e-08], ["market for polypropylene, granulate", 3.1711419718869685e-07], ["transport Plastic - CONSQ", 1.5684385092005196e-07], ["PE incineration no Energy Recovery - CONSQ", 3.327072150015725e-08], ["PP incineration no Energy Recovery - CONSQ", 2.435057792434667e-07], ["marginal heating grid projection updated - CONSQ", -3.6179419004955235e-07], ["energy avoided electricity from energy recovery - CONSQ", -7.171018951458978e-08]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 4.776176835497813e-07], ["autoclave - CONSQ", 1.1940750438112246e-06], ["market for corrugated board box", 2.817720799829456e-08], ["packaging film production, low density polyethylene", 5.4114387208721576e-08], ["market for polypropylene, granulate", 3.1711419718869685e-07], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -2.078429016806353e-08], ["market for polypropylene, granulate", -1.7124166648320043e-07], ["transport Plastic - CONSQ", 1.5684385092005196e-07], ["PE incineration no Energy Recovery - CONSQ", 1.530453189000074e-08], ["PP incineration no Energy Recovery - CONSQ", 1.120126584539537e-07], ["marginal heating grid projection updated - CONSQ", -1.6642532741907996e-07], ["energy avoided electricity from energy recovery - CONSQ", -3.2986687175223885e-08]]</t>
-  </si>
-  <si>
-    <t>[["alubox raw materials - CONSQ", 0.006562198476463859], ["alubox production - CONSQ", 0.0019874487681881105], ["autoclave - CONSQ", 0.022816718652521273], ["Handwash - CONSQ", 0.0012265568040732602], ["alubox EoL melting - CONSQ", 0.004906635595038445], ["alubox EoL mixed sorting - CONSQ", 0.00018111150869155272], ["transport Alu - CONSQ", 0.00029171235845780854], ["avoided alubox raw materials - CONSQ", -0.006001878687753108]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.06208002195471321], ["autoclave - CONSQ", 0.022816718652521273], ["market for corrugated board box", 0.00034641083188185725], ["packaging film production, low density polyethylene", 0.0069955286848791725], ["market for polypropylene, granulate", 0.05843815230566258], ["transport Plastic - CONSQ", 0.006809478292298527], ["PE incineration no Energy Recovery - CONSQ", 3.8003274429607946e-05], ["PP incineration no Energy Recovery - CONSQ", 0.00028233872643720486], ["marginal heating grid projection updated - CONSQ", -0.01376759220708353], ["energy avoided electricity from energy recovery - CONSQ", -0.0022377285914058245]]</t>
-  </si>
-  <si>
-    <t>[["pp production - CONSQ", 0.06208002195471321], ["autoclave - CONSQ", 0.022816718652521273], ["market for corrugated board box", 0.00034641083188185725], ["packaging film production, low density polyethylene", 0.0069955286848791725], ["market for polypropylene, granulate", 0.05843815230566258], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.0035487768262253317], ["market for polypropylene, granulate", -0.03155660224543658], ["transport Plastic - CONSQ", 0.006809478292298527], ["PE incineration no Energy Recovery - CONSQ", 1.7481506237070754e-05], ["PP incineration no Energy Recovery - CONSQ", 0.00012987581418344327], ["marginal heating grid projection updated - CONSQ", -0.006333092415231067], ["energy avoided electricity from energy recovery - CONSQ", -0.0010293551519985013]]</t>
+    <t>[["market for polypropylene, granulate", 0.0002923303491424216], ["sheet manufacturing - CONSQ", 0.0001402066317925113], ["packaging film production, low density polyethylene", 4.638920570989371e-05], ["market for corrugated board box", 2.0137784910350864e-05], ["autoclave - CONSQ", 0.0004521809809492889], ["transport Plastic - CONSQ", 1.1147787063326353e-06], ["market for polypropylene, granulate", -0.00015785838853400857], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -1.8781572123395753e-05], ["PP incineration no Energy Recovery - CONSQ", 5.026760436038136e-06], ["PE incineration no Energy Recovery - CONSQ", 6.815256058936856e-07], ["marginal electricity mix - CONSQ", -2.1765109391440553e-05], ["marginal heating grid projection updated - CONSQ", -7.367978527447541e-05]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.0002923303491424216], ["sheet manufacturing - CONSQ", 0.0001402066317925113], ["packaging film production, low density polyethylene", 4.638920570989371e-05], ["market for corrugated board box", 2.0137784910350864e-05], ["autoclave - CONSQ", 0.0004521809809492889], ["transport Plastic - CONSQ", 1.1147787063326353e-06], ["PP incineration no Energy Recovery - CONSQ", 1.0927740078167968e-05], ["PE incineration no Energy Recovery - CONSQ", 1.4815774040633578e-06], ["marginal electricity mix - CONSQ", -4.731545487910874e-05], ["marginal heating grid projection updated - CONSQ", -0.00016017344618911826]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.0008816312116942907], ["sheet manufacturing - CONSQ", 0.0004228453974853523], ["packaging film production, low density polyethylene", 0.00013990395090031596], ["market for corrugated board box", 6.073300209966322e-05], ["autoclave - CONSQ", 0.0006029079746154194], ["transport Plastic - CONSQ", 3.3620310193193104e-06], ["market for polypropylene, granulate", -0.00047608085431620495], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -5.6642835413861316e-05], ["PP incineration no Energy Recovery - CONSQ", 1.516007115608494e-05], ["PE incineration no Energy Recovery - CONSQ", 2.412854580603599e-06], ["marginal electricity mix - CONSQ", -6.564080577614083e-05], ["marginal heating grid projection updated - CONSQ", -0.00022220887614899786]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.0008816312116942907], ["sheet manufacturing - CONSQ", 0.0004228453974853523], ["packaging film production, low density polyethylene", 0.00013990395090031596], ["market for corrugated board box", 6.073300209966322e-05], ["autoclave - CONSQ", 0.0006029079746154194], ["transport Plastic - CONSQ", 1.5809710860480947e-05], ["PP incineration no Energy Recovery - CONSQ", 3.295667642766308e-05], ["PE incineration no Energy Recovery - CONSQ", 4.468249223175466e-06], ["marginal electricity mix - CONSQ", -0.0001426974038479957], ["marginal heating grid projection updated - CONSQ", -0.00048306277423123916]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0006976099450750722], ["alubox production - CONSQ", 6.0853003254803214e-05], ["market for polysulfone", 4.123615385169446e-06], ["autoclave - CONSQ", 0.0009043619618985778], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 2.560435613717889e-06], ["alubox EoL melting - CONSQ", 0.0006361709659517855], ["alubox EoL mixed sorting - CONSQ", 0.0], ["alubox raw materials - CONSQ", -0.0006627294478174007]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0006976099450750722], ["alubox production - CONSQ", 6.0853003254803214e-05], ["market for polysulfone", 4.123615385169446e-06], ["autoclave - CONSQ", 0.0009043619618985778], ["wet wipe", 0.0], ["transport Alu - CONSQ", 2.560435613717889e-06], ["alubox EoL melting - CONSQ", 0.0006361709659517855], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.0006627294478174007]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.00041684147741569095], ["alubox production - CONSQ", 3.636137352133111e-05], ["market for polysulfone", 2.061807692584723e-06], ["autoclave - CONSQ", 0.0006029079746154194], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 1.5299319793041158e-06], ["alubox EoL melting - CONSQ", 0.0003801299669089904], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.0003959994035443628]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.00041684147741569095], ["alubox production - CONSQ", 3.636137352133111e-05], ["market for polysulfone", 2.061807692584723e-06], ["autoclave - CONSQ", 0.0006029079746154194], ["wet wipe", 0.0], ["transport Alu - CONSQ", 1.5299319793041158e-06], ["alubox EoL melting - CONSQ", 0.0003801299669089904], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.0003959994035443628]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.13686231163340815], ["sheet manufacturing - CONSQ", 0.04179154922192118], ["packaging film production, low density polyethylene", 0.020631173913479607], ["market for corrugated board box", 0.009064392528037521], ["autoclave - CONSQ", 0.17629230606039337], ["transport Plastic - CONSQ", 0.0002270488086994238], ["market for polypropylene, granulate", -0.073905648281564], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.008701529761049199], ["PP incineration no Energy Recovery - CONSQ", 0.07437790773452976], ["PE incineration no Energy Recovery - CONSQ", 0.010168445776448428], ["marginal electricity mix - CONSQ", -0.015691804464282946], ["marginal heating grid projection updated - CONSQ", -0.08940181227960235]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.13686231163340815], ["sheet manufacturing - CONSQ", 0.04179154922192118], ["packaging film production, low density polyethylene", 0.020631173913479607], ["market for corrugated board box", 0.009064392528037521], ["autoclave - CONSQ", 0.17629230606039337], ["transport Plastic - CONSQ", 0.0002270488086994238], ["PP incineration no Energy Recovery - CONSQ", 0.16169110377063747], ["PE incineration no Energy Recovery - CONSQ", 0.022105316905314514], ["marginal electricity mix - CONSQ", -0.034112618171510414], ["marginal heating grid projection updated - CONSQ", -0.19435176575280427]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.4127593525451117], ["sheet manufacturing - CONSQ", 0.1260380055914172], ["packaging film production, low density polyethylene", 0.06222099943002526], ["market for corrugated board box", 0.027337056825669358], ["autoclave - CONSQ", 0.23505640808066372], ["transport Plastic - CONSQ", 0.0006847503755578513], ["market for polypropylene, granulate", -0.2228900503746875], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.02624270827154936], ["PP incineration no Energy Recovery - CONSQ", 0.22431432491341646], ["PE incineration no Energy Recovery - CONSQ", 0.03600008680220458], ["marginal electricity mix - CONSQ", -0.04732448942105432], ["marginal heating grid projection updated - CONSQ", -0.26962451313233715]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.4127593525451117], ["sheet manufacturing - CONSQ", 0.1260380055914172], ["packaging film production, low density polyethylene", 0.06222099943002526], ["market for corrugated board box", 0.027337056825669358], ["autoclave - CONSQ", 0.23505640808066372], ["transport Plastic - CONSQ", 0.003219989758438922], ["PP incineration no Energy Recovery - CONSQ", 0.48763983676861855], ["PE incineration no Energy Recovery - CONSQ", 0.06666682741154142], ["marginal electricity mix - CONSQ", -0.10287932481666903], ["marginal heating grid projection updated - CONSQ", -0.5861402459323403]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.16059233647617147], ["alubox production - CONSQ", 0.025719181024399827], ["market for polysulfone", 0.002189177197802492], ["autoclave - CONSQ", 0.35258461212078673], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 0.0017501770009449354], ["alubox EoL melting - CONSQ", 0.14615373580783747], ["alubox EoL mixed sorting - CONSQ", 0.0], ["alubox raw materials - CONSQ", -0.15256271965219978]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.16059233647617147], ["alubox production - CONSQ", 0.025719181024399827], ["market for polysulfone", 0.002189177197802492], ["autoclave - CONSQ", 0.35258461212078673], ["wet wipe", 0.0], ["transport Alu - CONSQ", 0.0017501770009449354], ["alubox EoL melting - CONSQ", 0.14615373580783747], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.15256271965219978]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.09595841812606423], ["alubox production - CONSQ", 0.015367930878844933], ["market for polysulfone", 0.001094588598901246], ["autoclave - CONSQ", 0.23505640808066372], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 0.0010457797684286156], ["alubox EoL melting - CONSQ", 0.08733094990140082], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.09116049721964548]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.09595841812606423], ["alubox production - CONSQ", 0.015367930878844933], ["market for polysulfone", 0.001094588598901246], ["autoclave - CONSQ", 0.23505640808066372], ["wet wipe", 0.0], ["transport Alu - CONSQ", 0.0010457797684286156], ["alubox EoL melting - CONSQ", 0.08733094990140082], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.09116049721964548]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.0022856400543405653], ["sheet manufacturing - CONSQ", 0.002379258479239628], ["packaging film production, low density polyethylene", 0.0004757341683898291], ["market for corrugated board box", 0.00014282642657079779], ["autoclave - CONSQ", 0.0010581319551087314], ["transport Plastic - CONSQ", 4.499571165695047e-06], ["market for polypropylene, granulate", -0.0012342456293694948], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.00014971537874943454], ["PP incineration no Energy Recovery - CONSQ", 0.0038826708641728587], ["PE incineration no Energy Recovery - CONSQ", 0.000530618000587303], ["marginal electricity mix - CONSQ", -0.0006712216549351856], ["marginal heating grid projection updated - CONSQ", -0.0019913788422036317]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.0022856400543405653], ["sheet manufacturing - CONSQ", 0.002379258479239628], ["packaging film production, low density polyethylene", 0.0004757341683898291], ["market for corrugated board box", 0.00014282642657079779], ["autoclave - CONSQ", 0.0010581319551087314], ["transport Plastic - CONSQ", 4.499571165695047e-06], ["PP incineration no Energy Recovery - CONSQ", 0.008440588835152746], ["PE incineration no Energy Recovery - CONSQ", 0.0011535173925796794], ["marginal electricity mix - CONSQ", -0.001459177500876142], ["marginal heating grid projection updated - CONSQ", -0.004329084437962882]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.006893200164209884], ["sheet manufacturing - CONSQ", 0.0071755414457163845], ["packaging film production, low density polyethylene", 0.0014347538119848604], ["market for corrugated board box", 0.00043074636577263535], ["autoclave - CONSQ", 0.0014108426066324028], ["transport Plastic - CONSQ", 1.3570135215439552e-05], ["market for polypropylene, granulate", -0.0037223280887940143], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.00045152256169181127], ["PP incineration no Energy Recovery - CONSQ", 0.011709642288763865], ["PE incineration no Energy Recovery - CONSQ", 0.0018785854298582953], ["marginal electricity mix - CONSQ", -0.002024319266778798], ["marginal heating grid projection updated - CONSQ", -0.006005745712532274]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.006893200164209884], ["sheet manufacturing - CONSQ", 0.0071755414457163845], ["packaging film production, low density polyethylene", 0.0014347538119848604], ["market for corrugated board box", 0.00043074636577263535], ["autoclave - CONSQ", 0.0014108426066324028], ["transport Plastic - CONSQ", 6.381259198073794e-05], ["PP incineration no Energy Recovery - CONSQ", 0.025455744106001568], ["PE incineration no Energy Recovery - CONSQ", 0.003478861907143895], ["marginal electricity mix - CONSQ", -0.004400694057791621], ["marginal heating grid projection updated - CONSQ", -0.013055968940115913]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0038208192527402953], ["alubox production - CONSQ", 0.0014510678583662482], ["market for polysulfone", 5.3890866777286184e-05], ["autoclave - CONSQ", 0.0021162639102174628], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 4.7527926522655724e-05], ["alubox EoL melting - CONSQ", 0.0019168046765830596], ["alubox EoL mixed sorting - CONSQ", 0.0], ["alubox raw materials - CONSQ", -0.0036297782900599133]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0038208192527402953], ["alubox production - CONSQ", 0.0014510678583662482], ["market for polysulfone", 5.3890866777286184e-05], ["autoclave - CONSQ", 0.0021162639102174628], ["wet wipe", 6.797999951503466e-07], ["transport Alu - CONSQ", 4.7527926522655724e-05], ["alubox EoL melting - CONSQ", 0.0019168046765830596], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.0036297782900599133]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0022830464982468188], ["alubox production - CONSQ", 0.0008670536798326995], ["market for polysulfone", 2.6945433388643092e-05], ["autoclave - CONSQ", 0.0014108426066324028], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 2.8399267026061893e-05], ["alubox EoL melting - CONSQ", 0.0011453444707094965], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.0021688941733083488]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0022830464982468188], ["alubox production - CONSQ", 0.0008670536798326995], ["market for polysulfone", 2.6945433388643092e-05], ["autoclave - CONSQ", 0.0014108426066324028], ["wet wipe", 6.797999951503466e-07], ["transport Alu - CONSQ", 2.8399267026061893e-05], ["alubox EoL melting - CONSQ", 0.0011453444707094965], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.0021688941733083488]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.003101327478915202], ["sheet manufacturing - CONSQ", 0.00309959804022401], ["packaging film production, low density polyethylene", 0.0006326924434908414], ["market for corrugated board box", 0.00020000116535890165], ["autoclave - CONSQ", 0.0009737544050856426], ["transport Plastic - CONSQ", 6.396241828479069e-06], ["market for polypropylene, granulate", -0.0016747168386446656], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.00020290888734050692], ["PP incineration no Energy Recovery - CONSQ", 0.005621185325913593], ["PE incineration no Energy Recovery - CONSQ", 0.0007682661196498161], ["marginal electricity mix - CONSQ", -0.0008509382822043261], ["marginal heating grid projection updated - CONSQ", -0.0025527076645293955]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.003101327478915202], ["sheet manufacturing - CONSQ", 0.00309959804022401], ["packaging film production, low density polyethylene", 0.0006326924434908414], ["market for corrugated board box", 0.00020000116535890165], ["autoclave - CONSQ", 0.0009737544050856426], ["transport Plastic - CONSQ", 6.396241828479069e-06], ["PP incineration no Energy Recovery - CONSQ", 0.012219968099804718], ["PE incineration no Energy Recovery - CONSQ", 0.001670143738367198], ["marginal electricity mix - CONSQ", -0.0018498658183810168], ["marginal heating grid projection updated - CONSQ", -0.00554936448604211]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.009353209857458722], ["sheet manufacturing - CONSQ", 0.009347994090100007], ["packaging film production, low density polyethylene", 0.0019081200288627144], ["market for corrugated board box", 0.0006031781176428033], ["autoclave - CONSQ", 0.0012983392065400547], ["transport Plastic - CONSQ", 1.9290253074820415e-05], ["market for polypropylene, granulate", -0.005050733323180047], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.0006119474256234091], ["PP incineration no Energy Recovery - CONSQ", 0.01695278114163002], ["PE incineration no Energy Recovery - CONSQ", 0.002719948318810872], ["marginal electricity mix - CONSQ", -0.002566321790781812], ["marginal heating grid projection updated - CONSQ", -0.007698642160237573]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.009353209857458722], ["sheet manufacturing - CONSQ", 0.009347994090100007], ["packaging film production, low density polyethylene", 0.0019081200288627144], ["market for corrugated board box", 0.0006031781176428033], ["autoclave - CONSQ", 0.0012983392065400547], ["transport Plastic - CONSQ", 9.071103783126321e-05], ["PP incineration no Energy Recovery - CONSQ", 0.03685387204701167], ["PE incineration no Energy Recovery - CONSQ", 0.0050369413311292955], ["marginal electricity mix - CONSQ", -0.005578960414211312], ["marginal heating grid projection updated - CONSQ", -0.016736178608992968]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.005350376339775814], ["alubox production - CONSQ", 0.001891918402880101], ["market for polysulfone", 6.904614888472404e-05], ["autoclave - CONSQ", 0.0019475088101712852], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 8.0322068457114e-05], ["alubox EoL melting - CONSQ", 0.00270330160299397], ["alubox EoL mixed sorting - CONSQ", 0.0], ["alubox raw materials - CONSQ", -0.005082857522726348]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.005350376339775814], ["alubox production - CONSQ", 0.001891918402880101], ["market for polysulfone", 6.904614888472404e-05], ["autoclave - CONSQ", 0.0019475088101712852], ["wet wipe", 2.2591998706634174e-06], ["transport Alu - CONSQ", 8.0322068457114e-05], ["alubox EoL melting - CONSQ", 0.00270330160299397], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.005082857522726348]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0031969996900712205], ["alubox production - CONSQ", 0.0011304742253845893], ["market for polysulfone", 3.452307444236202e-05], ["autoclave - CONSQ", 0.0012983392065400547], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 4.7994685169204124e-05], ["alubox EoL melting - CONSQ", 0.0016152984085828514], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.0030371497055335663]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0031969996900712205], ["alubox production - CONSQ", 0.0011304742253845893], ["market for polysulfone", 3.452307444236202e-05], ["autoclave - CONSQ", 0.0012983392065400547], ["wet wipe", 2.2591998706634174e-06], ["transport Alu - CONSQ", 4.7994685169204124e-05], ["alubox EoL melting - CONSQ", 0.0016152984085828514], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.0030371497055335663]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.37683259464795754], ["sheet manufacturing - CONSQ", 0.23434637909581485], ["packaging film production, low density polyethylene", 0.050972978544318946], ["market for corrugated board box", 0.014805773879959202], ["autoclave - CONSQ", 0.4023028740915676], ["transport Plastic - CONSQ", 0.0008182394343237622], ["market for polypropylene, granulate", -0.20348960110819228], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.024969496909594997], ["PP incineration no Energy Recovery - CONSQ", 0.21610896143228053], ["PE incineration no Energy Recovery - CONSQ", 0.029542509964936455], ["marginal electricity mix - CONSQ", -0.024163065194237204], ["marginal heating grid projection updated - CONSQ", -0.2003198151381057]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.37683259464795754], ["sheet manufacturing - CONSQ", 0.23434637909581485], ["packaging film production, low density polyethylene", 0.050972978544318946], ["market for corrugated board box", 0.014805773879959202], ["autoclave - CONSQ", 0.4023028740915676], ["transport Plastic - CONSQ", 0.0008182394343237622], ["PP incineration no Energy Recovery - CONSQ", 0.4698020900693408], ["PE incineration no Energy Recovery - CONSQ", 0.06422284774940919], ["marginal electricity mix - CONSQ", -0.05252840222712137], ["marginal heating grid projection updated - CONSQ", -0.435477858832194]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 1.136479253707025], ["sheet manufacturing - CONSQ", 0.7067589211852787], ["packaging film production, low density polyethylene", 0.1537280274269311], ["market for corrugated board box", 0.04465233391606264], ["autoclave - CONSQ", 0.536403832054948], ["transport Plastic - CONSQ", 0.0024677062268083105], ["market for polypropylene, granulate", -0.6136987969989978], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.07530483042477229], ["PP incineration no Energy Recovery - CONSQ", 0.6517571852731131], ["PE incineration no Energy Recovery - CONSQ", 0.10459149278766235], ["marginal electricity mix - CONSQ", -0.07287273593470037], ["marginal heating grid projection updated - CONSQ", -0.6041391248136355]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 1.136479253707025], ["sheet manufacturing - CONSQ", 0.7067589211852787], ["packaging film production, low density polyethylene", 0.1537280274269311], ["market for corrugated board box", 0.04465233391606264], ["autoclave - CONSQ", 0.536403832054948], ["transport Plastic - CONSQ", 0.011604212358208387], ["PP incineration no Energy Recovery - CONSQ", 1.4168634462420184], ["PE incineration no Energy Recovery - CONSQ", 0.19368794960531144], ["marginal electricity mix - CONSQ", -0.15841899116075872], ["marginal heating grid projection updated - CONSQ", -1.313345923486863]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.13568438920361434], ["alubox production - CONSQ", 0.06938050933546347], ["market for polysulfone", 0.008606844305076298], ["autoclave - CONSQ", 0.8046057481831352], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 0.03286863651009565], ["alubox EoL melting - CONSQ", -0.1015426037276029], ["alubox EoL mixed sorting - CONSQ", 0.0], ["alubox raw materials - CONSQ", -0.12890016972735893]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.13568438920361434], ["alubox production - CONSQ", 0.06938050933546347], ["market for polysulfone", 0.008606844305076298], ["autoclave - CONSQ", 0.8046057481831352], ["wet wipe", 0.00041551996788850116], ["transport Alu - CONSQ", 0.03286863651009565], ["alubox EoL melting - CONSQ", -0.1015426037276029], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.12890016972735893]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.08107522212804803], ["alubox production - CONSQ", 0.041456797219920176], ["market for polysulfone", 0.004303422152538149], ["autoclave - CONSQ", 0.536403832054948], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 0.01963993073817464], ["alubox EoL melting - CONSQ", -0.06067454923636391], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.0770214610197635]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.08107522212804803], ["alubox production - CONSQ", 0.041456797219920176], ["market for polysulfone", 0.004303422152538149], ["autoclave - CONSQ", 0.536403832054948], ["wet wipe", 0.00041551996788850116], ["transport Alu - CONSQ", 0.01963993073817464], ["alubox EoL melting - CONSQ", -0.06067454923636391], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.0770214610197635]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.10432477372004267], ["sheet manufacturing - CONSQ", 0.010245095401483516], ["packaging film production, low density polyethylene", 0.013085324881167096], ["market for corrugated board box", 0.0010078044055477897], ["autoclave - CONSQ", 0.06309255799011368], ["transport Plastic - CONSQ", 6.275383539134342e-05], ["market for polypropylene, granulate", -0.056335377808377704], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.006385849014989327], ["PP incineration no Energy Recovery - CONSQ", 0.00027519040154833216], ["PE incineration no Energy Recovery - CONSQ", 3.69067094624768e-05], ["marginal electricity mix - CONSQ", -0.003722304286334074], ["marginal heating grid projection updated - CONSQ", -0.013501034257537797]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.10432477372004267], ["sheet manufacturing - CONSQ", 0.010245095401483516], ["packaging film production, low density polyethylene", 0.013085324881167096], ["market for corrugated board box", 0.0010078044055477897], ["autoclave - CONSQ", 0.06309255799011368], ["transport Plastic - CONSQ", 6.275383539134342e-05], ["PP incineration no Energy Recovery - CONSQ", 0.0005982400033548442], ["PE incineration no Energy Recovery - CONSQ", 8.023197709077785e-05], ["marginal electricity mix - CONSQ", -0.008091965785506935], ["marginal heating grid projection updated - CONSQ", -0.029350074461972124]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.31463026994770155], ["sheet manufacturing - CONSQ", 0.030897906766699155], ["packaging film production, low density polyethylene", 0.039463677413364415], ["market for corrugated board box", 0.0030394101114227523], ["autoclave - CONSQ", 0.08412341065354982], ["transport Plastic - CONSQ", 0.0001892575988356665], ["market for polypropylene, granulate", -0.16990034577157334], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.019258909337614583], ["PP incineration no Energy Recovery - CONSQ", 0.0008299393062145775], ["PE incineration no Energy Recovery - CONSQ", 0.00013066350289368133], ["marginal electricity mix - CONSQ", -0.011225996998726954], ["marginal heating grid projection updated - CONSQ", -0.04071740488981081]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.31463026994770155], ["sheet manufacturing - CONSQ", 0.030897906766699155], ["packaging film production, low density polyethylene", 0.039463677413364415], ["market for corrugated board box", 0.0030394101114227523], ["autoclave - CONSQ", 0.08412341065354982], ["transport Plastic - CONSQ", 0.0008899703479400705], ["PP incineration no Energy Recovery - CONSQ", 0.0018042158831200826], ["PE incineration no Energy Recovery - CONSQ", 0.00024196944980997876], ["marginal electricity mix - CONSQ", -0.024404341298792438], ["marginal heating grid projection updated - CONSQ", -0.08851609758541922]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.034712062342997355], ["alubox production - CONSQ", 0.006309177862407238], ["market for polysulfone", 0.001156914932183265], ["autoclave - CONSQ", 0.12618511598022736], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 0.0005489538035706352], ["alubox EoL melting - CONSQ", 0.03111856753474898], ["alubox EoL mixed sorting - CONSQ", 0.0], ["alubox raw materials - CONSQ", -0.03297645922579384]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.034712062342997355], ["alubox production - CONSQ", 0.006309177862407238], ["market for polysulfone", 0.001156914932183265], ["autoclave - CONSQ", 0.12618511598022736], ["wet wipe", 0.0], ["transport Alu - CONSQ", 0.0005489538035706352], ["alubox EoL melting - CONSQ", 0.03111856753474898], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.03297645922579384]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.020741429294912413], ["alubox production - CONSQ", 0.003769910449309166], ["market for polysulfone", 0.0005784574660916325], ["autoclave - CONSQ", 0.08412341065354982], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 0.00032801527003620707], ["alubox EoL melting - CONSQ", 0.01859421551807161], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.019704357830141146]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.020741429294912413], ["alubox production - CONSQ", 0.003769910449309166], ["market for polysulfone", 0.0005784574660916325], ["autoclave - CONSQ", 0.08412341065354982], ["wet wipe", 0.0], ["transport Alu - CONSQ", 0.00032801527003620707], ["alubox EoL melting - CONSQ", 0.01859421551807161], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.019704357830141146]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 1.4292733363808177e-05], ["sheet manufacturing - CONSQ", 1.9503198971217235e-05], ["packaging film production, low density polyethylene", 4.664797255692879e-06], ["market for corrugated board box", 6.9703774036449475e-06], ["autoclave - CONSQ", 4.6369729801712826e-05], ["transport Plastic - CONSQ", 2.5474719030315482e-08], ["market for polypropylene, granulate", -7.718076016519349e-06], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -1.006639361632643e-06], ["PP incineration no Energy Recovery - CONSQ", 1.2469235060975301e-07], ["PE incineration no Energy Recovery - CONSQ", 1.573026213239601e-08], ["marginal electricity mix - CONSQ", -5.2030441356035335e-06], ["marginal heating grid projection updated - CONSQ", -7.753400583451584e-06]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 1.4292733363808177e-05], ["sheet manufacturing - CONSQ", 1.9503198971217235e-05], ["packaging film production, low density polyethylene", 4.664797255692879e-06], ["market for corrugated board box", 6.9703774036449475e-06], ["autoclave - CONSQ", 4.6369729801712826e-05], ["transport Plastic - CONSQ", 2.5474719030315482e-08], ["PP incineration no Energy Recovery - CONSQ", 2.71070327381357e-07], ["PE incineration no Energy Recovery - CONSQ", 3.419622202314179e-08], ["marginal electricity mix - CONSQ", -1.1310965436175745e-05], ["marginal heating grid projection updated - CONSQ", -1.6855218653388676e-05]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 4.310506887600977e-05], ["sheet manufacturing - CONSQ", 5.881917150134464e-05], ["packaging film production, low density polyethylene", 1.406843588240899e-05], ["market for corrugated board box", 2.10217731183176e-05], ["autoclave - CONSQ", 6.18263064019744e-05], ["transport Plastic - CONSQ", 7.682851765939126e-08], ["market for polypropylene, granulate", -2.3276737193372677e-05], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -3.0358964259666523e-06], ["PP incineration no Energy Recovery - CONSQ", 3.760562954093802e-07], ["PE incineration no Energy Recovery - CONSQ", 5.5690989008924834e-08], ["marginal electricity mix - CONSQ", -1.5691720331638778e-05], ["marginal heating grid projection updated - CONSQ", -2.3383271592903657e-05]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 4.310506887600977e-05], ["sheet manufacturing - CONSQ", 5.881917150134464e-05], ["packaging film production, low density polyethylene", 1.406843588240899e-05], ["market for corrugated board box", 2.10217731183176e-05], ["autoclave - CONSQ", 6.18263064019744e-05], ["transport Plastic - CONSQ", 3.612806194834351e-07], ["PP incineration no Energy Recovery - CONSQ", 8.175136857093945e-07], ["PE incineration no Energy Recovery - CONSQ", 1.0313146114168499e-07], ["marginal electricity mix - CONSQ", -3.411243549974792e-05], ["marginal heating grid projection updated - CONSQ", -5.083319911437242e-05]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 5.251428644684606e-05], ["alubox production - CONSQ", 1.272643130825426e-05], ["market for polysulfone", 1.9623985206605285e-07], ["autoclave - CONSQ", 9.273945960342565e-05], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 1.7167531230476142e-07], ["alubox EoL melting - CONSQ", 4.854561559184966e-05], ["alubox EoL mixed sorting - CONSQ", 0.0], ["alubox raw materials - CONSQ", -4.988857212442481e-05]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 5.251428644684606e-05], ["alubox production - CONSQ", 1.272643130825426e-05], ["market for polysulfone", 1.9623985206605285e-07], ["autoclave - CONSQ", 9.273945960342565e-05], ["wet wipe", 0.0], ["transport Alu - CONSQ", 1.7167531230476142e-07], ["alubox EoL melting - CONSQ", 4.854561559184966e-05], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 4.988857212442481e-05]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 3.137875671425036e-05], ["alubox production - CONSQ", 7.604399086160897e-06], ["market for polysulfone", 9.811992603302643e-08], ["autoclave - CONSQ", 6.18263064019744e-05], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 1.0258080654130396e-07], ["alubox EoL melting - CONSQ", 2.9007364743364318e-05], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 2.9809818878458096e-05]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 3.137875671425036e-05], ["alubox production - CONSQ", 7.604399086160897e-06], ["market for polysulfone", 9.811992603302643e-08], ["autoclave - CONSQ", 6.18263064019744e-05], ["wet wipe", 0.0], ["transport Alu - CONSQ", 1.0258080654130396e-07], ["alubox EoL melting - CONSQ", 2.9007364743364318e-05], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 2.9809818878458096e-05]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 1.6766880844736697e-06], ["sheet manufacturing - CONSQ", 2.315972006820966e-06], ["packaging film production, low density polyethylene", 6.497219432895026e-07], ["market for corrugated board box", 4.018338733114943e-07], ["autoclave - CONSQ", 0.00013736872633640347], ["transport Plastic - CONSQ", 5.4166986255656295e-09], ["market for polypropylene, granulate", -9.054115655922496e-07], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -1.1181151213342411e-07], ["PP incineration no Energy Recovery - CONSQ", 1.1608840419676603e-07], ["PE incineration no Energy Recovery - CONSQ", 1.5813325776855604e-08], ["marginal electricity mix - CONSQ", -3.7247288677713503e-07], ["marginal heating grid projection updated - CONSQ", -6.829658888548699e-07]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 1.6766880844736697e-06], ["sheet manufacturing - CONSQ", 2.315972006820966e-06], ["packaging film production, low density polyethylene", 6.497219432895026e-07], ["market for corrugated board box", 4.018338733114943e-07], ["autoclave - CONSQ", 0.00013736872633640347], ["transport Plastic - CONSQ", 5.4166986255656295e-09], ["PP incineration no Energy Recovery - CONSQ", 2.5236609607864717e-07], ["PE incineration no Energy Recovery - CONSQ", 3.437679516676155e-08], ["marginal electricity mix - CONSQ", -8.097236612857573e-07], ["marginal heating grid projection updated - CONSQ", -1.4847084534727287e-06]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 5.056678349930612e-06], ["sheet manufacturing - CONSQ", 6.984677480922749e-06], ["packaging film production, low density polyethylene", 1.9594788369035118e-06], ["market for corrugated board box", 1.2118799351665628e-06], ["autoclave - CONSQ", 0.00018315830178190182], ["transport Plastic - CONSQ", 1.6336075221593843e-08], ["market for polypropylene, granulate", -2.730606308954649e-06], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -3.372093154747414e-07], ["PP incineration no Energy Recovery - CONSQ", 3.501078856674592e-07], ["PE incineration no Energy Recovery - CONSQ", 5.598506527939877e-08], ["marginal electricity mix - CONSQ", -1.1233309230255528e-06], ["marginal heating grid projection updated - CONSQ", -2.059738394239169e-06]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 5.056678349930612e-06], ["sheet manufacturing - CONSQ", 6.984677480922749e-06], ["packaging film production, low density polyethylene", 1.9594788369035118e-06], ["market for corrugated board box", 1.2118799351665628e-06], ["autoclave - CONSQ", 0.00018315830178190182], ["transport Plastic - CONSQ", 7.681922751069629e-08], ["PP incineration no Energy Recovery - CONSQ", 7.611040992839827e-07], ["PE incineration no Energy Recovery - CONSQ", 1.0367604681456859e-07], ["marginal electricity mix - CONSQ", -2.4420237451106417e-06], ["marginal heating grid projection updated - CONSQ", -4.47769216134627e-06]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 3.7883493538848907e-06], ["alubox production - CONSQ", 2.115530290844273e-06], ["market for polysulfone", 8.682788604649358e-08], ["autoclave - CONSQ", 0.00027473745267280695], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 4.670883205015208e-08], ["alubox EoL melting - CONSQ", 3.562705650499696e-06], ["alubox EoL mixed sorting - CONSQ", 0.0], ["alubox raw materials - CONSQ", -3.598931886184589e-06]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 3.7883493538848907e-06], ["alubox production - CONSQ", 2.115530290844273e-06], ["market for polysulfone", 8.682788604649358e-08], ["autoclave - CONSQ", 0.00027473745267280695], ["wet wipe", 0.0], ["transport Alu - CONSQ", 4.670883205015208e-08], ["alubox EoL melting - CONSQ", 3.562705650499696e-06], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 3.598931886184589e-06]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 2.2636448244274092e-06], ["alubox production - CONSQ", 1.264088590170438e-06], ["market for polysulfone", 4.341394302324679e-08], ["autoclave - CONSQ", 0.00018315830178190182], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 2.7909835141588334e-08], ["alubox EoL melting - CONSQ", 2.1288163929401854e-06], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 2.150462583201846e-06]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 2.2636448244274092e-06], ["alubox production - CONSQ", 1.264088590170438e-06], ["market for polysulfone", 4.341394302324679e-08], ["autoclave - CONSQ", 0.00018315830178190182], ["wet wipe", 0.0], ["transport Alu - CONSQ", 2.7909835141588334e-08], ["alubox EoL melting - CONSQ", 2.1288163929401854e-06], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 2.150462583201846e-06]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.003120942329344581], ["sheet manufacturing - CONSQ", 0.0015781769034760376], ["packaging film production, low density polyethylene", 0.0005449558282405412], ["market for corrugated board box", 0.0002753207092151885], ["autoclave - CONSQ", 0.003767863953447906], ["transport Plastic - CONSQ", 2.604153664153109e-05], ["market for polypropylene, granulate", -0.0016853088578529123], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.00026032922242869304], ["PP incineration no Energy Recovery - CONSQ", 0.0001720418965629328], ["PE incineration no Energy Recovery - CONSQ", 2.3571724144823456e-05], ["marginal electricity mix - CONSQ", -0.00048014389693717486], ["marginal heating grid projection updated - CONSQ", -0.0007559589138941411]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.003120942329344581], ["sheet manufacturing - CONSQ", 0.0015781769034760376], ["packaging film production, low density polyethylene", 0.0005449558282405412], ["market for corrugated board box", 0.0002753207092151885], ["autoclave - CONSQ", 0.003767863953447906], ["transport Plastic - CONSQ", 2.604153664153109e-05], ["PP incineration no Energy Recovery - CONSQ", 0.0003740041229536348], ["PE incineration no Energy Recovery - CONSQ", 5.124287857422012e-05], ["marginal electricity mix - CONSQ", -0.001043791073250846], ["marginal heating grid projection updated - CONSQ", -0.0016433889426326707]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.009412365755208497], ["sheet manufacturing - CONSQ", 0.004759581137682599], ["packaging film production, low density polyethylene", 0.0016435175440861777], ["market for corrugated board box", 0.0008303322974842969], ["autoclave - CONSQ", 0.0050238186044533235], ["transport Plastic - CONSQ", 7.853796764395658e-05], ["market for polypropylene, granulate", -0.0050826775078154215], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.0007851198612620786], ["PP incineration no Energy Recovery - CONSQ", 0.0005188565134261088], ["PE incineration no Energy Recovery - CONSQ", 8.345268627021648e-05], ["marginal electricity mix - CONSQ", -0.0014480530153773191], ["marginal heating grid projection updated - CONSQ", -0.002279876088740956]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.009412365755208497], ["sheet manufacturing - CONSQ", 0.004759581137682599], ["packaging film production, low density polyethylene", 0.0016435175440861777], ["market for corrugated board box", 0.0008303322974842969], ["autoclave - CONSQ", 0.0050238186044533235], ["transport Plastic - CONSQ", 0.00036931918606159403], ["PP incineration no Energy Recovery - CONSQ", 0.0011279489422708437], ["PE incineration no Energy Recovery - CONSQ", 0.00015454201161503502], ["marginal electricity mix - CONSQ", -0.0031479413374237417], ["marginal heating grid projection updated - CONSQ", -0.004956252366766257]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.031285538113758046], ["alubox production - CONSQ", 0.0011957773186168467], ["market for polysulfone", 5.03236779959876e-05], ["autoclave - CONSQ", 0.007535727906895812], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 2.294717826646287e-05], ["alubox EoL melting - CONSQ", 0.028846660356210415], ["alubox EoL mixed sorting - CONSQ", 0.0], ["alubox raw materials - CONSQ", -0.029721261208045375]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.031285538113758046], ["alubox production - CONSQ", 0.0011957773186168467], ["market for polysulfone", 5.03236779959876e-05], ["autoclave - CONSQ", 0.007535727906895812], ["wet wipe", 5.655999578028925e-05], ["transport Alu - CONSQ", 2.294717826646287e-05], ["alubox EoL melting - CONSQ", 0.028846660356210415], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.029721261208045375]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.018693985114702542], ["alubox production - CONSQ", 0.0007145104333601738], ["market for polysulfone", 2.51618389979938e-05], ["autoclave - CONSQ", 0.0050238186044533235], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 1.371158160608423e-05], ["alubox EoL melting - CONSQ", 0.01723668735846019], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.017759285858951843]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.018693985114702542], ["alubox production - CONSQ", 0.0007145104333601738], ["market for polysulfone", 2.51618389979938e-05], ["autoclave - CONSQ", 0.0050238186044533235], ["wet wipe", 5.655999578028925e-05], ["transport Alu - CONSQ", 1.371158160608423e-05], ["alubox EoL melting - CONSQ", 0.01723668735846019], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.017759285858951843]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.052063862034754466], ["sheet manufacturing - CONSQ", 0.04310195804448259], ["packaging film production, low density polyethylene", 0.01093712379684791], ["market for corrugated board box", 0.005092068621342388], ["autoclave - CONSQ", 0.04002288158180119], ["transport Plastic - CONSQ", 8.820584767190898e-05], ["market for polypropylene, granulate", -0.02811448549915518], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.003461367295056495], ["PP incineration no Energy Recovery - CONSQ", 0.04684188527983237], ["PE incineration no Energy Recovery - CONSQ", 0.006401953712919471], ["marginal electricity mix - CONSQ", -0.011138813917437993], ["marginal heating grid projection updated - CONSQ", -0.03003321235798742]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.052063862034754466], ["sheet manufacturing - CONSQ", 0.04310195804448259], ["packaging film production, low density polyethylene", 0.01093712379684791], ["market for corrugated board box", 0.005092068621342388], ["autoclave - CONSQ", 0.04002288158180119], ["transport Plastic - CONSQ", 8.820584767190898e-05], ["PP incineration no Energy Recovery - CONSQ", 0.10183018539083384], ["PE incineration no Energy Recovery - CONSQ", 0.013917290680212241], ["marginal electricity mix - CONSQ", -0.024214812698945744], ["marginal heating grid projection updated - CONSQ", -0.06528959205806978]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.15701799661695184], ["sheet manufacturing - CONSQ", 0.12999003220825242], ["packaging film production, low density polyethylene", 0.0329849758625137], ["market for corrugated board box", 0.015357032347341933], ["autoclave - CONSQ", 0.05336384210423606], ["transport Plastic - CONSQ", 0.0002660176351781857], ["market for polypropylene, granulate", -0.0847897181740733], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.010439044011979814], ["PP incineration no Energy Recovery - CONSQ", 0.14126917782801643], ["PE incineration no Energy Recovery - CONSQ", 0.022665301505765695], ["marginal electricity mix - CONSQ", -0.033593248157067816], ["marginal heating grid projection updated - CONSQ", -0.09057635469924252]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.15701799661695184], ["sheet manufacturing - CONSQ", 0.12999003220825242], ["packaging film production, low density polyethylene", 0.0329849758625137], ["market for corrugated board box", 0.015357032347341933], ["autoclave - CONSQ", 0.05336384210423606], ["transport Plastic - CONSQ", 0.0012509289369681677], ["PP incineration no Energy Recovery - CONSQ", 0.3071069083213219], ["PE incineration no Energy Recovery - CONSQ", 0.04197278056613695], ["marginal electricity mix - CONSQ", -0.07302880033331927], ["marginal heating grid projection updated - CONSQ", -0.19690511890914514]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.1337141227711981], ["alubox production - CONSQ", 0.029302824880835243], ["market for polysulfone", 0.001468313881415679], ["autoclave - CONSQ", 0.08004576316360237], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 0.0014439525946760483], ["alubox EoL melting - CONSQ", 0.06494825997462716], ["alubox EoL mixed sorting - CONSQ", 0.0], ["alubox raw materials - CONSQ", -0.12702841663124673]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.1337141227711981], ["alubox production - CONSQ", 0.029302824880835243], ["market for polysulfone", 0.001468313881415679], ["autoclave - CONSQ", 0.08004576316360237], ["wet wipe", 0.0], ["transport Alu - CONSQ", 0.0014439525946760483], ["alubox EoL melting - CONSQ", 0.06494825997462716], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.12702841663124673]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.07989793276407749], ["alubox production - CONSQ", 0.017509258437858097], ["market for polysulfone", 0.0007341569407078394], ["autoclave - CONSQ", 0.05336384210423606], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 0.0008628021104533866], ["alubox EoL melting - CONSQ", 0.03880840408669011], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.07590303612544623]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.07989793276407749], ["alubox production - CONSQ", 0.017509258437858097], ["market for polysulfone", 0.0007341569407078394], ["autoclave - CONSQ", 0.05336384210423606], ["wet wipe", 0.0], ["transport Alu - CONSQ", 0.0008628021104533866], ["alubox EoL melting - CONSQ", 0.03880840408669011], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.07590303612544623]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.0020012263299230026], ["sheet manufacturing - CONSQ", 0.0039412913632786775], ["packaging film production, low density polyethylene", 0.0009261542488013825], ["market for corrugated board box", -9.542395253883582e-05], ["autoclave - CONSQ", 0.0016686328599342143], ["transport Plastic - CONSQ", 3.5998554514843338e-06], ["market for polypropylene, granulate", -0.0010806622181474474], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.0001548050699869926], ["PP incineration no Energy Recovery - CONSQ", 5.254299993222932e-07], ["PE incineration no Energy Recovery - CONSQ", 9.581866594068216e-08], ["marginal electricity mix - CONSQ", -4.009743224210602e-05], ["marginal heating grid projection updated - CONSQ", -0.003063397465899577]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.0020012263299230026], ["sheet manufacturing - CONSQ", 0.0039412913632786775], ["packaging film production, low density polyethylene", 0.0009261542488013825], ["market for corrugated board box", -9.542395253883582e-05], ["autoclave - CONSQ", 0.0016686328599342143], ["transport Plastic - CONSQ", 3.5998554514843338e-06], ["PP incineration no Energy Recovery - CONSQ", 1.1422391277608937e-06], ["PE incineration no Energy Recovery - CONSQ", 2.0830144750156094e-07], ["marginal electricity mix - CONSQ", -8.716832019624683e-05], ["marginal heating grid projection updated - CONSQ", -0.006659559705487802]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.006035444487000322], ["sheet manufacturing - CONSQ", 0.011886434270224953], ["packaging film production, low density polyethylene", 0.002793163550926107], ["market for corrugated board box", -0.000287786523477675], ["autoclave - CONSQ", 0.002224843813285622], ["transport Plastic - CONSQ", 1.0856706917768044e-05], ["market for polypropylene, granulate", -0.0032591400229708377], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.00046687242383998997], ["PP incineration no Energy Recovery - CONSQ", 1.584630153754517e-06], ["PE incineration no Energy Recovery - CONSQ", 3.3923377866408796e-07], ["marginal electricity mix - CONSQ", -0.00012092877426613511], ["marginal heating grid projection updated - CONSQ", -0.009238817749906198]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.006035444487000322], ["sheet manufacturing - CONSQ", 0.011886434270224953], ["packaging film production, low density polyethylene", 0.002793163550926107], ["market for corrugated board box", -0.000287786523477675], ["autoclave - CONSQ", 0.002224843813285622], ["transport Plastic - CONSQ", 5.1052889243889324e-05], ["PP incineration no Energy Recovery - CONSQ", 3.444848168899503e-06], ["PE incineration no Energy Recovery - CONSQ", 6.28210701947335e-07], ["marginal electricity mix - CONSQ", -0.0002628886206719301], ["marginal heating grid projection updated - CONSQ", -0.020084386413819898]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0008489389302054484], ["alubox production - CONSQ", 0.0019240367744805865], ["market for polysulfone", 0.00011602687293371272], ["autoclave - CONSQ", 0.0033372657198684286], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 7.449147747139974e-06], ["alubox EoL melting - CONSQ", 0.0011664864366597197], ["alubox EoL mixed sorting - CONSQ", 0.0], ["alubox raw materials - CONSQ", -0.0008064919836946475]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0008489389302054484], ["alubox production - CONSQ", 0.0019240367744805865], ["market for polysulfone", 0.00011602687293371272], ["autoclave - CONSQ", 0.0033372657198684286], ["wet wipe", 0.0], ["transport Alu - CONSQ", 7.449147747139974e-06], ["alubox EoL melting - CONSQ", 0.0011664864366597197], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.0008064919836946475]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0005072647837064073], ["alubox production - CONSQ", 0.0011496658517256685], ["market for polysulfone", 5.801343646685636e-05], ["autoclave - CONSQ", 0.002224843813285622], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 4.451074378071036e-06], ["alubox EoL melting - CONSQ", 0.0006970083111269929], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.00048190154452211064]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0005072647837064073], ["alubox production - CONSQ", 0.0011496658517256685], ["market for polysulfone", 5.801343646685636e-05], ["autoclave - CONSQ", 0.002224843813285622], ["wet wipe", 0.0], ["transport Alu - CONSQ", 4.451074378071036e-06], ["alubox EoL melting - CONSQ", 0.0006970083111269929], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.00048190154452211064]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.0015085297235492713], ["sheet manufacturing - CONSQ", 0.0022218497541273354], ["packaging film production, low density polyethylene", 0.0008158651929336762], ["market for corrugated board box", 0.005106828816104472], ["autoclave - CONSQ", 0.025437786692483113], ["transport Plastic - CONSQ", 7.892478732024939e-06], ["market for polypropylene, granulate", -0.0008146060502176224], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -9.774151223751331e-05], ["PP incineration no Energy Recovery - CONSQ", -1.6777322517640435e-05], ["PE incineration no Energy Recovery - CONSQ", -2.3178932490987266e-06], ["marginal electricity mix - CONSQ", -0.0010944723801689237], ["marginal heating grid projection updated - CONSQ", -0.014665792612951098]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.0015085297235492713], ["sheet manufacturing - CONSQ", 0.0022218497541273354], ["packaging film production, low density polyethylene", 0.0008158651929336762], ["market for corrugated board box", 0.005106828816104472], ["autoclave - CONSQ", 0.025437786692483113], ["transport Plastic - CONSQ", 7.892478732024939e-06], ["PP incineration no Energy Recovery - CONSQ", -3.6472440249173664e-05], ["PE incineration no Energy Recovery - CONSQ", -5.038898368538847e-06], ["marginal electricity mix - CONSQ", -0.002379287766941674], ["marginal heating grid projection updated - CONSQ", -0.03188215784235773]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.004549534086548313], ["sheet manufacturing - CONSQ", 0.006700816719253362], ["packaging film production, low density polyethylene", 0.002460545772636696], ["market for corrugated board box", 0.015401547219563608], ["autoclave - CONSQ", 0.03391704892400719], ["transport Plastic - CONSQ", 2.3802719559214804e-05], ["market for polypropylene, granulate", -0.0024567484054952133], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.0002947759831675797], ["PP incineration no Energy Recovery - CONSQ", -5.0598274247461796e-05], ["PE incineration no Energy Recovery - CONSQ", -8.206205749766575e-06], ["marginal electricity mix - CONSQ", -0.0033007897016484513], ["marginal heating grid projection updated - CONSQ", -0.04423016818274563]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.004549534086548313], ["sheet manufacturing - CONSQ", 0.006700816719253362], ["packaging film production, low density polyethylene", 0.002460545772636696], ["market for corrugated board box", 0.015401547219563608], ["autoclave - CONSQ", 0.03391704892400719], ["transport Plastic - CONSQ", 0.00011193057093841447], ["PP incineration no Energy Recovery - CONSQ", -0.00010999624837673184], ["PE incineration no Energy Recovery - CONSQ", -1.5196677319712623e-05], ["marginal electricity mix - CONSQ", -0.00717562978554327], ["marginal heating grid projection updated - CONSQ", -0.096152539526481]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.001539214726625129], ["alubox production - CONSQ", 0.003024158631836064], ["market for polysulfone", -2.52650852197549e-05], ["autoclave - CONSQ", 0.050875573384966226], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 7.056353752576391e-05], ["alubox EoL melting - CONSQ", 0.0012876218123940694], ["alubox EoL mixed sorting - CONSQ", 0.0], ["alubox raw materials - CONSQ", -0.001462253990203862]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.001539214726625129], ["alubox production - CONSQ", 0.003024158631836064], ["market for polysulfone", -2.52650852197549e-05], ["autoclave - CONSQ", 0.050875573384966226], ["wet wipe", 0.0], ["transport Alu - CONSQ", 7.056353752576391e-05], ["alubox EoL melting - CONSQ", 0.0012876218123940694], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.001462253990203862]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0009197239017426542], ["alubox production - CONSQ", 0.0018070194684324907], ["market for polysulfone", -1.263254260987745e-05], ["autoclave - CONSQ", 0.03391704892400719], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 4.216368966715229e-05], ["alubox EoL melting - CONSQ", 0.0007693900904754538], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.0008737377066843821]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0009197239017426542], ["alubox production - CONSQ", 0.0018070194684324907], ["market for polysulfone", -1.263254260987745e-05], ["autoclave - CONSQ", 0.03391704892400719], ["wet wipe", 0.0], ["transport Alu - CONSQ", 4.216368966715229e-05], ["alubox EoL melting - CONSQ", 0.0007693900904754538], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.0008737377066843821]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.0001370298370277186], ["sheet manufacturing - CONSQ", 6.558922878822288e-05], ["packaging film production, low density polyethylene", 2.201760014483621e-05], ["market for corrugated board box", 1.0642654311344513e-05], ["autoclave - CONSQ", 0.000820760366710643], ["transport Plastic - CONSQ", 3.864587461974845e-06], ["market for polypropylene, granulate", -7.399611201447075e-05], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -6.646838931278451e-06], ["PP incineration no Energy Recovery - CONSQ", 7.718434066130547e-06], ["PE incineration no Energy Recovery - CONSQ", 9.480740324530097e-07], ["marginal electricity mix - CONSQ", -3.268406751675442e-05], ["marginal heating grid projection updated - CONSQ", -4.7665525830544856e-05]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.0001370298370277186], ["sheet manufacturing - CONSQ", 6.558922878822288e-05], ["packaging film production, low density polyethylene", 2.201760014483621e-05], ["market for corrugated board box", 1.0642654311344513e-05], ["autoclave - CONSQ", 0.000820760366710643], ["transport Plastic - CONSQ", 3.864587461974845e-06], ["PP incineration no Energy Recovery - CONSQ", 1.6779204490635857e-05], ["PE incineration no Energy Recovery - CONSQ", 2.0610305054672694e-06], ["marginal electricity mix - CONSQ", -7.105232014969519e-05], ["marginal heating grid projection updated - CONSQ", -0.00010362070829385793]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.00041326458806458124], ["sheet manufacturing - CONSQ", 0.00019780878517213282], ["packaging film production, low density polyethylene", 6.640228475768785e-05], ["market for corrugated board box", 3.209689394064137e-05], ["autoclave - CONSQ", 0.001094347155596963], ["transport Plastic - CONSQ", 1.1655105042180711e-05], ["market for polypropylene, granulate", -0.00022316287764793068], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -2.004602178150608e-05], ["PP incineration no Energy Recovery - CONSQ", 2.3277817018325543e-05], ["PE incineration no Energy Recovery - CONSQ", 3.356535325242328e-06], ["marginal electricity mix - CONSQ", -9.857099676420285e-05], ["marginal heating grid projection updated - CONSQ", -0.0001437531729857]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.00041326458806458124], ["sheet manufacturing - CONSQ", 0.00019780878517213282], ["packaging film production, low density polyethylene", 6.640228475768785e-05], ["market for corrugated board box", 3.209689394064137e-05], ["autoclave - CONSQ", 0.001094347155596963], ["transport Plastic - CONSQ", 5.4807299400656074e-05], ["PP incineration no Energy Recovery - CONSQ", 5.060395004685126e-05], ["PE incineration no Energy Recovery - CONSQ", 6.215806159925579e-06], ["marginal electricity mix - CONSQ", -0.0002142847756501711], ["marginal heating grid projection updated - CONSQ", -0.0003125068977182916]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0019595608700344216], ["alubox production - CONSQ", 5.523512065434223e-05], ["market for polysulfone", 2.3547896267477363e-06], ["autoclave - CONSQ", 0.001641520733421286], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 7.444284265652027e-06], ["alubox EoL melting - CONSQ", 0.0017777647034078641], ["alubox EoL mixed sorting - CONSQ", 0.0], ["alubox raw materials - CONSQ", -0.001861582826535765]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0019595608700344216], ["alubox production - CONSQ", 5.523512065434223e-05], ["market for polysulfone", 2.3547896267477363e-06], ["autoclave - CONSQ", 0.001641520733421286], ["wet wipe", 0.0], ["transport Alu - CONSQ", 7.444284265652027e-06], ["alubox EoL melting - CONSQ", 0.0017777647034078641], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.001861582826535765]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0011708924935939812], ["alubox production - CONSQ", 3.300453132986153e-05], ["market for polysulfone", 1.1773948133738681e-06], ["autoclave - CONSQ", 0.001094347155596963], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 4.448168311639807e-06], ["alubox EoL melting - CONSQ", 0.0010622641931947443], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.0011123478689134838]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0011708924935939812], ["alubox production - CONSQ", 3.300453132986153e-05], ["market for polysulfone", 1.1773948133738681e-06], ["autoclave - CONSQ", 0.001094347155596963], ["wet wipe", 0.0], ["transport Alu - CONSQ", 4.448168311639807e-06], ["alubox EoL melting - CONSQ", 0.0010622641931947443], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.0011123478689134838]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 1.010700979361432e-08], ["sheet manufacturing - CONSQ", 1.3634635962189866e-08], ["packaging film production, low density polyethylene", 3.076138771759701e-09], ["market for corrugated board box", 1.2242259622340095e-09], ["autoclave - CONSQ", -2.452980801097643e-07], ["transport Plastic - CONSQ", 6.943037542437208e-11], ["market for polypropylene, granulate", -5.457785288400429e-09], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -1.2857762786041752e-09], ["PP incineration no Energy Recovery - CONSQ", 5.7747655208032674e-09], ["PE incineration no Energy Recovery - CONSQ", 7.893176660936691e-10], ["marginal electricity mix - CONSQ", -6.483303328361492e-09], ["marginal heating grid projection updated - CONSQ", -2.374649153955783e-08]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 1.010700979361432e-08], ["sheet manufacturing - CONSQ", 1.3634635962189866e-08], ["packaging film production, low density polyethylene", 3.076138771759701e-09], ["market for corrugated board box", 1.2242259622340095e-09], ["autoclave - CONSQ", -2.452980801097643e-07], ["transport Plastic - CONSQ", 6.943037542437208e-11], ["PP incineration no Energy Recovery - CONSQ", 1.2553838088675971e-08], ["PE incineration no Energy Recovery - CONSQ", 1.7159079697651014e-09], ["marginal electricity mix - CONSQ", -1.409413757570231e-08], ["marginal heating grid projection updated - CONSQ", -5.162280767544982e-08]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 3.048145810737604e-08], ["sheet manufacturing - CONSQ", 4.112033068039711e-08], ["packaging film production, low density polyethylene", 9.27724372684612e-09], ["market for corrugated board box", 3.6921100441881608e-09], ["autoclave - CONSQ", -3.270641068128926e-07], ["transport Plastic - CONSQ", 2.0939319575840515e-10], ["market for polypropylene, granulate", -1.6459987377921893e-08], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -3.8777379045612965e-09], ["PP incineration no Energy Recovery - CONSQ", 1.7415959507117595e-08], ["PE incineration no Energy Recovery - CONSQ", 2.7944786369968796e-09], ["marginal electricity mix - CONSQ", -1.955281946543705e-08], ["marginal heating grid projection updated - CONSQ", -7.161640303140404e-08]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 3.048145810737604e-08], ["sheet manufacturing - CONSQ", 4.112033068039711e-08], ["packaging film production, low density polyethylene", 9.27724372684612e-09], ["market for corrugated board box", 3.6921100441881608e-09], ["autoclave - CONSQ", -3.270641068128926e-07], ["transport Plastic - CONSQ", 9.846565550360194e-10], ["PP incineration no Energy Recovery - CONSQ", 3.786078153731102e-08], ["PE incineration no Energy Recovery - CONSQ", 5.174960438896746e-09], ["marginal electricity mix - CONSQ", -4.250612926779542e-08], ["marginal heating grid projection updated - CONSQ", -1.556878326749585e-07]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 3.019157934776932e-08], ["alubox production - CONSQ", 6.319931081508324e-09], ["market for polysulfone", 8.832244985121951e-10], ["autoclave - CONSQ", -4.905961602195286e-07], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 7.705929830905257e-10], ["alubox EoL melting - CONSQ", 2.4970577425579485e-08], ["alubox EoL mixed sorting - CONSQ", 0.0], ["alubox raw materials - CONSQ", -2.8682000380297532e-08]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 3.019157934776932e-08], ["alubox production - CONSQ", 6.319931081508324e-09], ["market for polysulfone", 8.832244985121951e-10], ["autoclave - CONSQ", -4.905961602195286e-07], ["wet wipe", 0.0], ["transport Alu - CONSQ", 7.705929830905257e-10], ["alubox EoL melting - CONSQ", 2.4970577425579485e-08], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 2.8682000380297532e-08]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 1.8040314117788417e-08], ["alubox production - CONSQ", 3.7763357989591526e-09], ["market for polysulfone", 4.4161224925609753e-10], ["autoclave - CONSQ", -3.270641068128926e-07], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 4.604508863809583e-10], ["alubox EoL melting - CONSQ", 1.4920619265120554e-08], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 1.7138298411847864e-08]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 1.8040314117788417e-08], ["alubox production - CONSQ", 3.7763357989591526e-09], ["market for polysulfone", 4.4161224925609753e-10], ["autoclave - CONSQ", -3.270641068128926e-07], ["wet wipe", 0.0], ["transport Alu - CONSQ", 4.604508863809583e-10], ["alubox EoL melting - CONSQ", 1.4920619265120554e-08], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 1.7138298411847864e-08]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.00012572490415138895], ["sheet manufacturing - CONSQ", 9.882951798941758e-05], ["packaging film production, low density polyethylene", 2.4109122727570757e-05], ["market for corrugated board box", 1.632805207425256e-05], ["autoclave - CONSQ", 0.0002074693223001382], ["transport Plastic - CONSQ", 4.4494148318360095e-07], ["market for polypropylene, granulate", -6.789144824068463e-05], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -8.303837974514304e-06], ["PP incineration no Energy Recovery - CONSQ", 1.771215230999127e-06], ["PE incineration no Energy Recovery - CONSQ", 2.34317477872916e-07], ["marginal electricity mix - CONSQ", -8.301988156209052e-06], ["marginal heating grid projection updated - CONSQ", -4.506465462848301e-05]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.00012572490415138895], ["sheet manufacturing - CONSQ", 9.882951798941758e-05], ["packaging film production, low density polyethylene", 2.4109122727570757e-05], ["market for corrugated board box", 1.632805207425256e-05], ["autoclave - CONSQ", 0.0002074693223001382], ["transport Plastic - CONSQ", 4.4494148318360095e-07], ["PP incineration no Energy Recovery - CONSQ", 3.850467893327558e-06], ["PE incineration no Energy Recovery - CONSQ", 5.093858214431948e-07], ["marginal electricity mix - CONSQ", -1.804780021754406e-05], ["marginal heating grid projection updated - CONSQ", -9.796664046017348e-05]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.000379170345852892], ["sheet manufacturing - CONSQ", 0.0002980572764815241], ["packaging film production, low density polyethylene", 7.271005119808096e-05], ["market for corrugated board box", 4.9243331643637915e-05], ["autoclave - CONSQ", 0.000276625763071466], ["transport Plastic - CONSQ", 1.3418870128817722e-06], ["market for polypropylene, granulate", -0.0002047519867613963], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -2.5043320367801153e-05], ["PP incineration no Energy Recovery - CONSQ", 5.341760220137342e-06], ["PE incineration no Energy Recovery - CONSQ", 8.295711780661598e-07], ["marginal electricity mix - CONSQ", -2.5037741934718375e-05], ["marginal heating grid projection updated - CONSQ", -0.00013590927581737667]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.000379170345852892], ["sheet manufacturing - CONSQ", 0.0002980572764815241], ["packaging film production, low density polyethylene", 7.271005119808096e-05], ["market for corrugated board box", 4.9243331643637915e-05], ["autoclave - CONSQ", 0.000276625763071466], ["transport Plastic - CONSQ", 6.31012788390235e-06], ["PP incineration no Energy Recovery - CONSQ", 1.1612522218491012e-05], ["PE incineration no Energy Recovery - CONSQ", 1.53624292236903e-06], ["marginal electricity mix - CONSQ", -5.442987376566979e-05], ["marginal heating grid projection updated - CONSQ", -0.00029545494742543347]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0003150804933965422], ["alubox production - CONSQ", 3.354210770205699e-05], ["market for polysulfone", 1.9449059649755328e-06], ["autoclave - CONSQ", 0.0004149386446002764], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 1.4479899599715667e-06], ["alubox EoL melting - CONSQ", 0.0002913098000264923], ["alubox EoL mixed sorting - CONSQ", 0.0], ["alubox raw materials - CONSQ", -0.0002993264687255364]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0003150804933965422], ["alubox production - CONSQ", 3.354210770205699e-05], ["market for polysulfone", 1.9449059649755328e-06], ["autoclave - CONSQ", 0.0004149386446002764], ["wet wipe", 0.0], ["transport Alu - CONSQ", 1.4479899599715667e-06], ["alubox EoL melting - CONSQ", 0.0002913098000264923], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.0002993264687255364]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0001882694180315919], ["alubox production - CONSQ", 2.004234863594184e-05], ["market for polysulfone", 9.724529824877664e-07], ["autoclave - CONSQ", 0.000276625763071466], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 8.652145492757718e-07], ["alubox EoL melting - CONSQ", 0.00017406576309036842], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.00017885594712972763]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0001882694180315919], ["alubox production - CONSQ", 2.004234863594184e-05], ["market for polysulfone", 9.724529824877664e-07], ["autoclave - CONSQ", 0.000276625763071466], ["wet wipe", 0.0], ["transport Alu - CONSQ", 8.652145492757718e-07], ["alubox EoL melting - CONSQ", 0.00017406576309036842], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.00017885594712972763]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.00026049611728313284], ["sheet manufacturing - CONSQ", 0.00012313865326397396], ["packaging film production, low density polyethylene", 4.324394837353855e-05], ["market for corrugated board box", 1.1226053340540693e-05], ["autoclave - CONSQ", 0.0002835158017023123], ["transport Plastic - CONSQ", 2.3446821183497546e-06], ["market for polypropylene, granulate", -0.00014066790332991226], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -1.75583627675308e-05], ["PP incineration no Energy Recovery - CONSQ", 1.2108045557351342e-05], ["PE incineration no Energy Recovery - CONSQ", 1.6487555901141015e-06], ["marginal electricity mix - CONSQ", -1.9902203716258906e-05], ["marginal heating grid projection updated - CONSQ", -9.832266250212389e-05]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.00026049611728313284], ["sheet manufacturing - CONSQ", 0.00012313865326397396], ["packaging film production, low density polyethylene", 4.324394837353855e-05], ["market for corrugated board box", 1.1226053340540693e-05], ["autoclave - CONSQ", 0.0002835158017023123], ["transport Plastic - CONSQ", 2.3446821183497546e-06], ["PP incineration no Energy Recovery - CONSQ", 2.6321838167944946e-05], ["PE incineration no Energy Recovery - CONSQ", 3.5842512828220626e-06], ["marginal electricity mix - CONSQ", -4.326565996121341e-05], ["marginal heating grid projection updated - CONSQ", -0.00021374491840318828]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.0007856232108471923], ["sheet manufacturing - CONSQ", 0.00037137054159554016], ["packaging film production, low density polyethylene", 0.00013041825435649288], ["market for corrugated board box", 3.385635133841636e-05], ["autoclave - CONSQ", 0.0003780210689362458], ["transport Plastic - CONSQ", 7.071263533122011e-06], ["market for polypropylene, granulate", -0.00042423653385628094], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -5.295379140100479e-05], ["PP incineration no Energy Recovery - CONSQ", 3.6516327870749485e-05], ["PE incineration no Energy Recovery - CONSQ", 5.837209113665673e-06], ["marginal electricity mix - CONSQ", -6.002251884837787e-05], ["marginal heating grid projection updated - CONSQ", -0.0002965286645877992]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.0007856232108471923], ["sheet manufacturing - CONSQ", 0.00037137054159554016], ["packaging film production, low density polyethylene", 0.00013041825435649288], ["market for corrugated board box", 3.385635133841636e-05], ["autoclave - CONSQ", 0.0003780210689362458], ["transport Plastic - CONSQ", 3.325211196887476e-05], ["PP incineration no Energy Recovery - CONSQ", 7.938332145898805e-05], ["PE incineration no Energy Recovery - CONSQ", 1.080964650689883e-05], ["marginal electricity mix - CONSQ", -0.0001304837366126081], ["marginal heating grid projection updated - CONSQ", -0.0006446275317045519]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0004131713628805212], ["alubox production - CONSQ", 3.643676379954262e-05], ["market for polysulfone", 3.941891481143825e-06], ["autoclave - CONSQ", 0.0005670316034046246], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 3.1726421595104636e-06], ["alubox EoL melting - CONSQ", 0.0003775896067680762], ["alubox EoL mixed sorting - CONSQ", 0.0], ["alubox raw materials - CONSQ", -0.00039251279473577326]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0004131713628805212], ["alubox production - CONSQ", 3.643676379954262e-05], ["market for polysulfone", 3.941891481143825e-06], ["autoclave - CONSQ", 0.0005670316034046246], ["wet wipe", 0.0007149199948835133], ["transport Alu - CONSQ", 3.1726421595104636e-06], ["alubox EoL melting - CONSQ", 0.0003775896067680762], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.00039251279473577326]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.00024688145939559016], ["alubox production - CONSQ", 2.1771986713363707e-05], ["market for polysulfone", 1.9709457405719124e-06], ["autoclave - CONSQ", 0.0003780210689362458], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 1.8957425340913146e-06], ["alubox EoL melting - CONSQ", 0.00022562036371969645], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.00023453738642557198]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.00024688145939559016], ["alubox production - CONSQ", 2.1771986713363707e-05], ["market for polysulfone", 1.9709457405719124e-06], ["autoclave - CONSQ", 0.0003780210689362458], ["wet wipe", 0.0007149199948835133], ["transport Alu - CONSQ", 1.8957425340913146e-06], ["alubox EoL melting - CONSQ", 0.00022562036371969645], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.00023453738642557198]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.00028185166157234195], ["sheet manufacturing - CONSQ", 0.0001268727166544331], ["packaging film production, low density polyethylene", 4.823945680101545e-05], ["market for corrugated board box", 1.1597092085653628e-05], ["autoclave - CONSQ", 0.0002914689825914016], ["transport Plastic - CONSQ", 2.39584946970623e-06], ["market for polypropylene, granulate", -0.00015219989724587677], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -1.9109636493302948e-05], ["PP incineration no Energy Recovery - CONSQ", 1.2239460427478685e-05], ["PE incineration no Energy Recovery - CONSQ", 1.6658765754337796e-06], ["marginal electricity mix - CONSQ", -2.0496970057545702e-05], ["marginal heating grid projection updated - CONSQ", -0.00010390822714739845]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.00028185166157234195], ["sheet manufacturing - CONSQ", 0.0001268727166544331], ["packaging film production, low density polyethylene", 4.823945680101545e-05], ["market for corrugated board box", 1.1597092085653628e-05], ["autoclave - CONSQ", 0.0002914689825914016], ["transport Plastic - CONSQ", 2.39584946970623e-06], ["PP incineration no Energy Recovery - CONSQ", 2.660752266821757e-05], ["PE incineration no Energy Recovery - CONSQ", 3.62147081612483e-06], ["marginal electricity mix - CONSQ", -4.4558630259629624e-05], ["marginal heating grid projection updated - CONSQ", -0.00022588745023621696]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.0008500288206078213], ["sheet manufacturing - CONSQ", 0.00038263200261458714], ["packaging film production, low density polyethylene", 0.00014548407311800566], ["market for corrugated board box", 3.497535707744545e-05], ["autoclave - CONSQ", 0.000388625310121808], ["transport Plastic - CONSQ", 7.2255777674038935e-06], ["market for polypropylene, granulate", -0.0004590155631270078], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -5.763223587602739e-05], ["PP incineration no Energy Recovery - CONSQ", 3.691265843142237e-05], ["PE incineration no Energy Recovery - CONSQ", 5.897823780954541e-06], ["marginal electricity mix - CONSQ", -6.18162585989637e-05], ["marginal heating grid projection updated - CONSQ", -0.0003133740182741545]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.0008500288206078213], ["sheet manufacturing - CONSQ", 0.00038263200261458714], ["packaging film production, low density polyethylene", 0.00014548407311800566], ["market for corrugated board box", 3.497535707744545e-05], ["autoclave - CONSQ", 0.000388625310121808], ["transport Plastic - CONSQ", 3.39777636395285e-05], ["PP incineration no Energy Recovery - CONSQ", 8.024490963438457e-05], ["PE incineration no Energy Recovery - CONSQ", 1.0921895890770616e-05], ["marginal electricity mix - CONSQ", -0.00013438317085260183], ["marginal heating grid projection updated - CONSQ", -0.000681247865804867]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0004233644886257506], ["alubox production - CONSQ", 3.9155602595241975e-05], ["market for polysulfone", 3.98247149360115e-06], ["autoclave - CONSQ", 0.0005829379651828032], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 3.5443375385846074e-06], ["alubox EoL melting - CONSQ", 0.00038627739692386555], ["alubox EoL mixed sorting - CONSQ", 0.0], ["alubox raw materials - CONSQ", -0.0004021962641937134]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0004233644886257506], ["alubox production - CONSQ", 3.9155602595241975e-05], ["market for polysulfone", 3.98247149360115e-06], ["autoclave - CONSQ", 0.0005829379651828032], ["wet wipe", 0.0011563999632328281], ["transport Alu - CONSQ", 3.5443375385846074e-06], ["alubox EoL melting - CONSQ", 0.00038627739692386555], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.0004021962641937134]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.00025297213746736027], ["alubox production - CONSQ", 2.3396569029713032e-05], ["market for polysulfone", 1.991235746800575e-06], ["autoclave - CONSQ", 0.000388625310121808], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 2.1178409317072575e-06], ["alubox EoL melting - CONSQ", 0.00023081156162275572], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.000240323530593733]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.00025297213746736027], ["alubox production - CONSQ", 2.3396569029713032e-05], ["market for polysulfone", 1.991235746800575e-06], ["autoclave - CONSQ", 0.000388625310121808], ["wet wipe", 0.0011563999632328281], ["transport Alu - CONSQ", 2.1178409317072575e-06], ["alubox EoL melting - CONSQ", 0.00023081156162275572], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.000240323530593733]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.0009935043452922018], ["sheet manufacturing - CONSQ", 0.00028519549774947225], ["packaging film production, low density polyethylene", 0.0003240164755982084], ["market for corrugated board box", 3.8061301023721094e-05], ["autoclave - CONSQ", 0.0006429489707443777], ["transport Plastic - CONSQ", 4.7112864074431723e-07], ["market for polypropylene, granulate", -0.0005364923464576143], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -7.043248914230354e-05], ["PP incineration no Energy Recovery - CONSQ", 3.6429806872556006e-05], ["PE incineration no Energy Recovery - CONSQ", 4.348760124579787e-06], ["marginal electricity mix - CONSQ", -2.8656279114855917e-05], ["marginal heating grid projection updated - CONSQ", -0.00013010044158742002]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.0009935043452922018], ["sheet manufacturing - CONSQ", 0.00028519549774947225], ["packaging film production, low density polyethylene", 0.0003240164755982084], ["market for corrugated board box", 3.8061301023721094e-05], ["autoclave - CONSQ", 0.0006429489707443777], ["transport Plastic - CONSQ", 4.7112864074431723e-07], ["PP incineration no Energy Recovery - CONSQ", 7.919523233141758e-05], ["PE incineration no Energy Recovery - CONSQ", 9.453826357760746e-06], ["marginal electricity mix - CONSQ", -6.229625852475937e-05], ["marginal heating grid projection updated - CONSQ", -0.0002828270468237024]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.0029962829461294004], ["sheet manufacturing - CONSQ", 0.0008601134059171364], ["packaging film production, low density polyethylene", 0.0009771925256525872], ["market for corrugated board box", 0.00011478805068578466], ["autoclave - CONSQ", 0.0008572652943267731], ["transport Plastic - CONSQ", 1.420864154511792e-06], ["market for polypropylene, granulate", -0.001617992790911895], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.00021241543914204234], ["PP incineration no Energy Recovery - CONSQ", 0.0001098676715195772], ["PE incineration no Energy Recovery - CONSQ", 1.5396231184893684e-05], ["marginal electricity mix - CONSQ", -8.642369849325866e-05], ["marginal heating grid projection updated - CONSQ", -0.0003923664110027261]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.0029962829461294004], ["sheet manufacturing - CONSQ", 0.0008601134059171364], ["packaging film production, low density polyethylene", 0.0009771925256525872], ["market for corrugated board box", 0.00011478805068578466], ["autoclave - CONSQ", 0.0008572652943267731], ["transport Plastic - CONSQ", 6.681512251941211e-06], ["PP incineration no Energy Recovery - CONSQ", 0.00023884276417357486], ["PE incineration no Energy Recovery - CONSQ", 2.8511539231427704e-05], ["marginal electricity mix - CONSQ", -0.00018787760539686478], ["marginal heating grid projection updated - CONSQ", -0.0008529704586910816]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0009092938753576539], ["alubox production - CONSQ", 0.0006192172871795779], ["market for polysulfone", 3.5588812009795096e-05], ["autoclave - CONSQ", 0.0012858979414887555], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 2.543086018999684e-06], ["alubox EoL melting - CONSQ", 0.0008639744857248536], ["alubox EoL mixed sorting - CONSQ", 0.0], ["alubox raw materials - CONSQ", -0.0008638291815894067]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0009092938753576539], ["alubox production - CONSQ", 0.0006192172871795779], ["market for polysulfone", 3.5588812009795096e-05], ["autoclave - CONSQ", 0.0012858979414887555], ["wet wipe", 0.0], ["transport Alu - CONSQ", 2.543086018999684e-06], ["alubox EoL melting - CONSQ", 0.0008639744857248536], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.0008638291815894067]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0005433285535640465], ["alubox production - CONSQ", 0.0003699996690876727], ["market for polysulfone", 1.7794406004897548e-05], ["autoclave - CONSQ", 0.0008572652943267731], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 1.5195651106190677e-06], ["alubox EoL melting - CONSQ", 0.0005162489491757682], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.0005161621258850601]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0005433285535640465], ["alubox production - CONSQ", 0.0003699996690876727], ["market for polysulfone", 1.7794406004897548e-05], ["autoclave - CONSQ", 0.0008572652943267731], ["wet wipe", 0.0], ["transport Alu - CONSQ", 1.5195651106190677e-06], ["alubox EoL melting - CONSQ", 0.0005162489491757682], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.0005161621258850601]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 5.108847081593792e-10], ["sheet manufacturing - CONSQ", 2.0055060407041774e-10], ["packaging film production, low density polyethylene", 8.518376808698837e-11], ["market for corrugated board box", 8.138664770407186e-11], ["autoclave - CONSQ", 8.895062016251628e-10], ["transport Plastic - CONSQ", 1.2814610975253494e-12], ["market for polypropylene, granulate", -2.758777423993188e-10], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -3.2772614458506333e-11], ["PP incineration no Energy Recovery - CONSQ", 2.1659643750856676e-10], ["PE incineration no Energy Recovery - CONSQ", 2.9608152681241675e-11], ["marginal electricity mix - CONSQ", -6.522322726009749e-11], ["marginal heating grid projection updated - CONSQ", -4.185522499500902e-10]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 5.108847081593792e-10], ["sheet manufacturing - CONSQ", 2.0055060407041774e-10], ["packaging film production, low density polyethylene", 8.518376808698837e-11], ["market for corrugated board box", 8.138664770407186e-11], ["autoclave - CONSQ", 8.895062016251628e-10], ["transport Plastic - CONSQ", 1.2814610975253494e-12], ["PP incineration no Energy Recovery - CONSQ", 4.708618206705333e-10], ["PE incineration no Energy Recovery - CONSQ", 6.43655493069912e-11], ["marginal electricity mix - CONSQ", -1.4178962352492332e-10], ["marginal heating grid projection updated - CONSQ", -9.098961952045614e-10]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 1.5407634055557485e-09], ["sheet manufacturing - CONSQ", 6.048351551474528e-10], ["packaging film production, low density polyethylene", 2.5690342238012753e-10], ["market for corrugated board box", 2.454517946114811e-10], ["autoclave - CONSQ", 1.1860082688424586e-09], ["transport Plastic - CONSQ", 3.86472399795824e-12], ["market for polypropylene, granulate", -8.320122389904092e-10], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -9.88380416012422e-11], ["PP incineration no Energy Recovery - CONSQ", 6.532273512155529e-10], ["PE incineration no Energy Recovery - CONSQ", 1.0482389246206538e-10], ["marginal electricity mix - CONSQ", -1.9670497013182241e-10], ["marginal heating grid projection updated - CONSQ", -1.2623004359275698e-09]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 1.5407634055557485e-09], ["sheet manufacturing - CONSQ", 6.048351551474528e-10], ["packaging film production, low density polyethylene", 2.5690342238012753e-10], ["market for corrugated board box", 2.454517946114811e-10], ["autoclave - CONSQ", 1.1860082688424586e-09], ["transport Plastic - CONSQ", 1.8173588542537098e-11], ["PP incineration no Energy Recovery - CONSQ", 1.4200594591654145e-09], ["PE incineration no Energy Recovery - CONSQ", 1.9411831937426329e-10], ["marginal electricity mix - CONSQ", -4.27619500240409e-10], ["marginal heating grid projection updated - CONSQ", -2.7441313824161748e-09]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 7.059022052515648e-10], ["alubox production - CONSQ", 1.2731835328723082e-10], ["market for polysulfone", 7.569921209387769e-12], ["autoclave - CONSQ", 1.7790124032503255e-09], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 7.059048181206864e-12], ["alubox EoL melting - CONSQ", 6.384564391746344e-10], ["alubox EoL mixed sorting - CONSQ", 0.0], ["alubox raw materials - CONSQ", -6.706070949865302e-10]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 7.059022052515648e-10], ["alubox production - CONSQ", 1.2731835328723082e-10], ["market for polysulfone", 7.569921209387769e-12], ["autoclave - CONSQ", 1.7790124032503255e-09], ["wet wipe", 1.488054395169408e-10], ["transport Alu - CONSQ", 7.059048181206864e-12], ["alubox EoL melting - CONSQ", 6.384564391746344e-10], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 6.706070949865302e-10]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 4.217963350786028e-10], ["alubox production - CONSQ", 7.607628139963828e-11], ["market for polysulfone", 3.7849606046938845e-12], ["autoclave - CONSQ", 1.1860082688424586e-09], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 4.217978963418171e-12], ["alubox EoL melting - CONSQ", 3.8149560116153955e-10], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 4.007065183243596e-10]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 4.217963350786028e-10], ["alubox production - CONSQ", 7.607628139963828e-11], ["market for polysulfone", 3.7849606046938845e-12], ["autoclave - CONSQ", 1.1860082688424586e-09], ["wet wipe", 1.488054395169408e-10], ["transport Alu - CONSQ", 4.217978963418171e-12], ["alubox EoL melting - CONSQ", 3.8149560116153955e-10], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 4.007065183243596e-10]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 2.3069508571518267e-07], ["sheet manufacturing - CONSQ", 1.1676351349627134e-07], ["packaging film production, low density polyethylene", 3.9367280514291904e-08], ["market for corrugated board box", 2.0845360933335005e-08], ["autoclave - CONSQ", 3.1710954693885847e-07], ["transport Plastic - CONSQ", 6.002837273599116e-10], ["market for polypropylene, granulate", -1.245753462851951e-07], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -1.5120211529084632e-08], ["PP incineration no Energy Recovery - CONSQ", 8.148726885040876e-08], ["PE incineration no Energy Recovery - CONSQ", 1.1133782181549757e-08], ["marginal electricity mix - CONSQ", -2.3997243706685002e-08], ["marginal heating grid projection updated - CONSQ", -1.2107154307726865e-07]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 2.3069508571518267e-07], ["sheet manufacturing - CONSQ", 1.1676351349627134e-07], ["packaging film production, low density polyethylene", 3.9367280514291904e-08], ["market for corrugated board box", 2.0845360933335005e-08], ["autoclave - CONSQ", 3.1710954693885847e-07], ["transport Plastic - CONSQ", 6.002837273599116e-10], ["PP incineration no Energy Recovery - CONSQ", 1.7714623663110043e-07], ["PE incineration no Energy Recovery - CONSQ", 2.420387430768112e-08], ["marginal electricity mix - CONSQ", -5.2167920749834906e-08], ["marginal heating grid projection updated - CONSQ", -2.631990065915706e-07]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 6.957470839036497e-07], ["sheet manufacturing - CONSQ", 3.5214392959992425e-07], ["packaging film production, low density polyethylene", 1.1872671660627804e-07], ["market for corrugated board box", 6.286696153366745e-08], ["autoclave - CONSQ", 4.228127292532614e-07], ["transport Plastic - CONSQ", 1.8103794952203241e-09], ["market for polypropylene, granulate", -3.757034253090213e-07], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -4.560063702091006e-08], ["PP incineration no Energy Recovery - CONSQ", 2.4575525526262653e-07], ["PE incineration no Energy Recovery - CONSQ", 3.941773735964126e-08], ["marginal electricity mix - CONSQ", -7.23726393937056e-08], ["marginal heating grid projection updated - CONSQ", -3.6513639963234e-07]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 6.957470839036497e-07], ["sheet manufacturing - CONSQ", 3.5214392959992425e-07], ["packaging film production, low density polyethylene", 1.1872671660627804e-07], ["market for corrugated board box", 6.286696153366745e-08], ["autoclave - CONSQ", 4.228127292532614e-07], ["transport Plastic - CONSQ", 8.513180336667813e-09], ["PP incineration no Energy Recovery - CONSQ", 5.34250554919588e-07], ["PE incineration no Energy Recovery - CONSQ", 7.299580992531496e-08], ["marginal electricity mix - CONSQ", -1.5733182475137465e-07], ["marginal heating grid projection updated - CONSQ", -7.937747817994183e-07]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 4.837419482800488e-07], ["alubox production - CONSQ", 5.702653101477771e-08], ["market for polysulfone", 3.839052480296054e-09], ["autoclave - CONSQ", 6.342190938777169e-07], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 2.9487876441255517e-09], ["alubox EoL melting - CONSQ", 4.315016593414792e-07], ["alubox EoL mixed sorting - CONSQ", 0.0], ["alubox raw materials - CONSQ", -4.5955485086475417e-07]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 4.837419482800488e-07], ["alubox production - CONSQ", 5.702653101477771e-08], ["market for polysulfone", 3.839052480296054e-09], ["autoclave - CONSQ", 6.342190938777169e-07], ["wet wipe", 8.37999938806309e-10], ["transport Alu - CONSQ", 2.9487876441255517e-09], ["alubox EoL melting - CONSQ", 4.315016593414792e-07], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 4.5955485086475417e-07]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 2.890493603662896e-07], ["alubox production - CONSQ", 3.4074949201963875e-08], ["market for polysulfone", 1.919526240148027e-09], ["autoclave - CONSQ", 4.228127292532614e-07], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 1.761983192530408e-09], ["alubox EoL melting - CONSQ", 2.5783432483629743e-07], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 2.745968923475381e-07]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 2.890493603662896e-07], ["alubox production - CONSQ", 3.4074949201963875e-08], ["market for polysulfone", 1.919526240148027e-09], ["autoclave - CONSQ", 4.228127292532614e-07], ["wet wipe", 8.37999938806309e-10], ["transport Alu - CONSQ", 1.761983192530408e-09], ["alubox EoL melting - CONSQ", 2.5783432483629743e-07], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 2.745968923475381e-07]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.04251274359466289], ["sheet manufacturing - CONSQ", 0.0026493980380010414], ["packaging film production, low density polyethylene", 0.00508912609558556], ["market for corrugated board box", 0.00020399786499809266], ["autoclave - CONSQ", 0.011223963601517827], ["transport Plastic - CONSQ", 2.574026110320628e-05], ["market for polypropylene, granulate", -0.02295688154091924], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.0025816737472388095], ["PP incineration no Energy Recovery - CONSQ", 9.448240520841844e-05], ["PE incineration no Energy Recovery - CONSQ", 1.271749335464092e-05], ["marginal electricity mix - CONSQ", -0.000748838048292629], ["marginal heating grid projection updated - CONSQ", -0.00460721503804492]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.04251274359466289], ["sheet manufacturing - CONSQ", 0.0026493980380010414], ["packaging film production, low density polyethylene", 0.00508912609558556], ["market for corrugated board box", 0.00020399786499809266], ["autoclave - CONSQ", 0.011223963601517827], ["transport Plastic - CONSQ", 2.574026110320628e-05], ["PP incineration no Energy Recovery - CONSQ", 0.00020539653305939564], ["PE incineration no Energy Recovery - CONSQ", 2.764672468358637e-05], ["marginal electricity mix - CONSQ", -0.0016279087896800997], ["marginal heating grid projection updated - CONSQ", -0.010015684861584773]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.12821303623707778], ["sheet manufacturing - CONSQ", 0.007990248051178211], ["packaging film production, low density polyethylene", 0.015348157755076188], ["market for corrugated board box", 0.0006152316562309265], ["autoclave - CONSQ", 0.014965284802055875], ["transport Plastic - CONSQ", 7.762935889847207e-05], ["market for polypropylene, granulate", -0.069235039567924], ["polyethylene, high density, granulate, recycled to generic market for high density PE granulate", -0.007786000032366803], ["PP incineration no Energy Recovery - CONSQ", 0.0002849469363309857], ["PE incineration no Energy Recovery - CONSQ", 4.5024664999130274e-05], ["marginal electricity mix - CONSQ", -0.0022584004519752895], ["marginal heating grid projection updated - CONSQ", -0.013894775506805658]]</t>
+  </si>
+  <si>
+    <t>[["market for polypropylene, granulate", 0.12821303623707778], ["sheet manufacturing - CONSQ", 0.007990248051178211], ["packaging film production, low density polyethylene", 0.015348157755076188], ["market for corrugated board box", 0.0006152316562309265], ["autoclave - CONSQ", 0.014965284802055875], ["transport Plastic - CONSQ", 0.00036504651847856894], ["PP incineration no Energy Recovery - CONSQ", 0.0006194498616040047], ["PE incineration no Energy Recovery - CONSQ", 8.337900925958345e-05], ["marginal electricity mix - CONSQ", -0.004909566199408771], ["marginal heating grid projection updated - CONSQ", -0.0302060337100453]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0062578899537383235], ["alubox production - CONSQ", 0.001783443188377875], ["market for polysulfone", 0.00044439248991123896], ["autoclave - CONSQ", 0.022447927203035654], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 0.00023132935403068978], ["alubox EoL melting - CONSQ", 0.005304821629162564], ["alubox EoL mixed sorting - CONSQ", 0.0], ["alubox raw materials - CONSQ", -0.005944995456033719]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.0062578899537383235], ["alubox production - CONSQ", 0.001783443188377875], ["market for polysulfone", 0.00044439248991123896], ["autoclave - CONSQ", 0.022447927203035654], ["wet wipe", 0.0], ["transport Alu - CONSQ", 0.00023132935403068978], ["alubox EoL melting - CONSQ", 0.005304821629162564], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.005944995456033719]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.003739264487599382], ["alubox production - CONSQ", 0.0010656572469862466], ["market for polysulfone", 0.00022219624495561948], ["autoclave - CONSQ", 0.014965284802055875], ["cabinet washer - CONSQ", 0.0], ["transport Alu - CONSQ", 0.00013822576697004204], ["alubox EoL melting - CONSQ", 0.0031697794748289003], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.0035523012632147515]]</t>
+  </si>
+  <si>
+    <t>[["alubox raw materials - CONSQ", 0.003739264487599382], ["alubox production - CONSQ", 0.0010656572469862466], ["market for polysulfone", 0.00022219624495561948], ["autoclave - CONSQ", 0.014965284802055875], ["wet wipe", 0.0], ["transport Alu - CONSQ", 0.00013822576697004204], ["alubox EoL melting - CONSQ", 0.0031697794748289003], ["alubox EoL mixed sorting - CONSQ", 0.0], ["avoided alubox raw materials - CONSQ", 0.0035523012632147515]]</t>
   </si>
 </sst>
 </file>
@@ -623,7 +938,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -699,64 +1014,64 @@
         <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="G2" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="H2" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="I2" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="J2" t="s">
-        <v>48</v>
+        <v>93</v>
       </c>
       <c r="K2" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="L2" t="s">
-        <v>54</v>
+        <v>109</v>
       </c>
       <c r="M2" t="s">
-        <v>57</v>
+        <v>117</v>
       </c>
       <c r="N2" t="s">
-        <v>60</v>
+        <v>125</v>
       </c>
       <c r="O2" t="s">
-        <v>63</v>
+        <v>133</v>
       </c>
       <c r="P2" t="s">
-        <v>66</v>
+        <v>141</v>
       </c>
       <c r="Q2" t="s">
-        <v>69</v>
+        <v>149</v>
       </c>
       <c r="R2" t="s">
-        <v>72</v>
+        <v>157</v>
       </c>
       <c r="S2" t="s">
-        <v>75</v>
+        <v>165</v>
       </c>
       <c r="T2" t="s">
-        <v>78</v>
+        <v>173</v>
       </c>
       <c r="U2" t="s">
-        <v>81</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -764,64 +1079,64 @@
         <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="H3" t="s">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="I3" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="J3" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="K3" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="L3" t="s">
-        <v>55</v>
+        <v>110</v>
       </c>
       <c r="M3" t="s">
-        <v>58</v>
+        <v>118</v>
       </c>
       <c r="N3" t="s">
-        <v>61</v>
+        <v>126</v>
       </c>
       <c r="O3" t="s">
-        <v>64</v>
+        <v>134</v>
       </c>
       <c r="P3" t="s">
-        <v>67</v>
+        <v>142</v>
       </c>
       <c r="Q3" t="s">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="R3" t="s">
-        <v>73</v>
+        <v>158</v>
       </c>
       <c r="S3" t="s">
-        <v>76</v>
+        <v>166</v>
       </c>
       <c r="T3" t="s">
-        <v>79</v>
+        <v>174</v>
       </c>
       <c r="U3" t="s">
-        <v>82</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -829,64 +1144,389 @@
         <v>23</v>
       </c>
       <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I4" t="s">
+        <v>87</v>
+      </c>
+      <c r="J4" t="s">
+        <v>95</v>
+      </c>
+      <c r="K4" t="s">
+        <v>103</v>
+      </c>
+      <c r="L4" t="s">
+        <v>111</v>
+      </c>
+      <c r="M4" t="s">
+        <v>119</v>
+      </c>
+      <c r="N4" t="s">
+        <v>127</v>
+      </c>
+      <c r="O4" t="s">
+        <v>135</v>
+      </c>
+      <c r="P4" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>151</v>
+      </c>
+      <c r="R4" t="s">
+        <v>159</v>
+      </c>
+      <c r="S4" t="s">
+        <v>167</v>
+      </c>
+      <c r="T4" t="s">
+        <v>175</v>
+      </c>
+      <c r="U4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H5" t="s">
+        <v>80</v>
+      </c>
+      <c r="I5" t="s">
+        <v>88</v>
+      </c>
+      <c r="J5" t="s">
+        <v>96</v>
+      </c>
+      <c r="K5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L5" t="s">
+        <v>112</v>
+      </c>
+      <c r="M5" t="s">
+        <v>120</v>
+      </c>
+      <c r="N5" t="s">
+        <v>128</v>
+      </c>
+      <c r="O5" t="s">
+        <v>136</v>
+      </c>
+      <c r="P5" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>152</v>
+      </c>
+      <c r="R5" t="s">
+        <v>160</v>
+      </c>
+      <c r="S5" t="s">
+        <v>168</v>
+      </c>
+      <c r="T5" t="s">
+        <v>176</v>
+      </c>
+      <c r="U5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J6" t="s">
+        <v>97</v>
+      </c>
+      <c r="K6" t="s">
+        <v>105</v>
+      </c>
+      <c r="L6" t="s">
+        <v>113</v>
+      </c>
+      <c r="M6" t="s">
+        <v>121</v>
+      </c>
+      <c r="N6" t="s">
+        <v>129</v>
+      </c>
+      <c r="O6" t="s">
+        <v>137</v>
+      </c>
+      <c r="P6" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>153</v>
+      </c>
+      <c r="R6" t="s">
+        <v>161</v>
+      </c>
+      <c r="S6" t="s">
+        <v>169</v>
+      </c>
+      <c r="T6" t="s">
+        <v>177</v>
+      </c>
+      <c r="U6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7" t="s">
         <v>26</v>
       </c>
-      <c r="C4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H7" t="s">
+        <v>82</v>
+      </c>
+      <c r="I7" t="s">
+        <v>90</v>
+      </c>
+      <c r="J7" t="s">
+        <v>98</v>
+      </c>
+      <c r="K7" t="s">
+        <v>106</v>
+      </c>
+      <c r="L7" t="s">
+        <v>114</v>
+      </c>
+      <c r="M7" t="s">
+        <v>122</v>
+      </c>
+      <c r="N7" t="s">
+        <v>130</v>
+      </c>
+      <c r="O7" t="s">
+        <v>138</v>
+      </c>
+      <c r="P7" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>154</v>
+      </c>
+      <c r="R7" t="s">
+        <v>162</v>
+      </c>
+      <c r="S7" t="s">
+        <v>170</v>
+      </c>
+      <c r="T7" t="s">
+        <v>178</v>
+      </c>
+      <c r="U7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
         <v>35</v>
       </c>
-      <c r="F4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" t="s">
+        <v>75</v>
+      </c>
+      <c r="H8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I8" t="s">
+        <v>91</v>
+      </c>
+      <c r="J8" t="s">
+        <v>99</v>
+      </c>
+      <c r="K8" t="s">
+        <v>107</v>
+      </c>
+      <c r="L8" t="s">
+        <v>115</v>
+      </c>
+      <c r="M8" t="s">
+        <v>123</v>
+      </c>
+      <c r="N8" t="s">
+        <v>131</v>
+      </c>
+      <c r="O8" t="s">
+        <v>139</v>
+      </c>
+      <c r="P8" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>155</v>
+      </c>
+      <c r="R8" t="s">
+        <v>163</v>
+      </c>
+      <c r="S8" t="s">
+        <v>171</v>
+      </c>
+      <c r="T8" t="s">
+        <v>179</v>
+      </c>
+      <c r="U8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
         <v>44</v>
       </c>
-      <c r="I4" t="s">
-        <v>47</v>
-      </c>
-      <c r="J4" t="s">
-        <v>50</v>
-      </c>
-      <c r="K4" t="s">
-        <v>53</v>
-      </c>
-      <c r="L4" t="s">
-        <v>56</v>
-      </c>
-      <c r="M4" t="s">
-        <v>59</v>
-      </c>
-      <c r="N4" t="s">
-        <v>62</v>
-      </c>
-      <c r="O4" t="s">
-        <v>65</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" t="s">
         <v>68</v>
       </c>
-      <c r="Q4" t="s">
-        <v>71</v>
-      </c>
-      <c r="R4" t="s">
-        <v>74</v>
-      </c>
-      <c r="S4" t="s">
-        <v>77</v>
-      </c>
-      <c r="T4" t="s">
-        <v>80</v>
-      </c>
-      <c r="U4" t="s">
-        <v>83</v>
+      <c r="G9" t="s">
+        <v>76</v>
+      </c>
+      <c r="H9" t="s">
+        <v>84</v>
+      </c>
+      <c r="I9" t="s">
+        <v>92</v>
+      </c>
+      <c r="J9" t="s">
+        <v>100</v>
+      </c>
+      <c r="K9" t="s">
+        <v>108</v>
+      </c>
+      <c r="L9" t="s">
+        <v>116</v>
+      </c>
+      <c r="M9" t="s">
+        <v>124</v>
+      </c>
+      <c r="N9" t="s">
+        <v>132</v>
+      </c>
+      <c r="O9" t="s">
+        <v>140</v>
+      </c>
+      <c r="P9" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>156</v>
+      </c>
+      <c r="R9" t="s">
+        <v>164</v>
+      </c>
+      <c r="S9" t="s">
+        <v>172</v>
+      </c>
+      <c r="T9" t="s">
+        <v>180</v>
+      </c>
+      <c r="U9" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified:   Brighway/Libaries/__pycache__/life_cycle_assessment.cpython-311.pyc 	modified:   Brighway/Libaries/life_cycle_assessment.py 	modified:   Brighway/Ofir/Ofir.ipynb 	modified:   Brighway/Results/Ananas - CONSQ_recipe.xlsx 	modified:   Brighway/Results/Ananas - CONSQ_recipe_unq.xlsx 	modified:   Brighway/Results_Ofir/GWP_life_stage_pr_scenario_CONSQ.jpg 	modified:   Brighway/Results_Ofir/break_even_large_CONSQ.jpg 	modified:   Brighway/Results_Ofir/break_even_small_CONSQ.jpg 	modified:   Brighway/Results_Ofir/scaled_impact_score_multi_CONSQ_ReCiPe 2016 v1.03, endpoint (H).jpg 	modified:   Brighway/Results_Ofir/scaled_impact_score_multi_CONSQ_ReCiPe 2016 v1.03, midpoint (H).jpg
</commit_message>
<xml_diff>
--- a/Brighway/Results/Ananas - CONSQ_recipe.xlsx
+++ b/Brighway/Results/Ananas - CONSQ_recipe.xlsx
@@ -79,508 +79,508 @@
     <t>('ReCiPe 2016 v1.03, endpoint (H)', 'total: natural resources', 'natural resources')</t>
   </si>
   <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00032945166331691244], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00015801064853070173], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.6389205711862454e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.013778491028875e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004622626384260705], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.1147787062239849e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.00017790389819113272], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.8781572123565963e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.66507922162909e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.2504469565799618e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.3860842943139076e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -8.303594843869356e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.0142047379371389e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00032945166331691244], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00015801064853070173], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.6389205711862454e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.013778491028875e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004622626384260705], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.1147787062239849e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.2315389612237151e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -2.7183629490868737e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.1871397929925744e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0001805129313821823], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.0142047379371389e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0009373131829579762], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0004495514225803063], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0001399039509001107], ["'market for corrugated board box' (kilogram, RER, None)", 6.073300209944417e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000616350184568094], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.362031019620352e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0005061491187973072], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -5.664283541570399e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.6117549334775722e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -4.427048141689966e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.78857789405792e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00023624312087142089], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.8854839025352327e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0009373131829579762], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0004495514225803063], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0001399039509001107], ["'market for corrugated board box' (kilogram, RER, None)", 6.073300209944417e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000616350184568094], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.5809710865610812e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.5038150727773306e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -8.198237299425862e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00014757778009440384], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.000513572001932085], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.8854839025352327e-05]]</t>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00032945166331691244], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00015801064853070173], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.6389205711862454e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.013778491028875e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004622626384260705], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.1147787062239849e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.00017790389819113272], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.8781572123565963e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.66507922162909e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 6.815256059071447e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.3860842943139076e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -8.303594843869356e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.0142047379371389e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00032945166331691244], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00015801064853070173], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.6389205711862454e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.013778491028875e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004622626384260705], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.1147787062239849e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.2315389612237151e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.4815774041459668e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.1871397929925744e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0001805129313821823], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.0142047379371389e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0009373131829579762], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0004495514225803063], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0001399039509001107], ["'market for corrugated board box' (kilogram, RER, None)", 6.073300209944417e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000616350184568094], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.362031019620352e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0005061491187973072], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -5.664283541570399e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.6117549334775722e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.4128545807312035e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.78857789405792e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00023624312087142089], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.8854839025352327e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0009373131829579762], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0004495514225803063], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0001399039509001107], ["'market for corrugated board box' (kilogram, RER, None)", 6.073300209944417e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000616350184568094], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.5809710865610812e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.5038150727773306e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 4.468249223576303e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00014757778009440384], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.000513572001932085], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.8854839025352327e-05]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0006799317205210687], ["'alubox production - CONSQ' (kilogram, GLO, None)", 5.9310919264254154e-05], ["'market for polysulfone' (kilogram, GLO, None)", 4.019118309206293e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000924525276852141], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.00016623361404338074], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.495551281007104e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 5.907099145686869e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0006459351344950152], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 9.505013037587547e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.3335979393624514e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -9.281865639367464e-07], ["'market for corrugated board box' (kilogram, RER, None)", 7.107201576755263e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.176104412433239e-06]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0006799317205210687], ["'alubox production - CONSQ' (kilogram, GLO, None)", 5.9310919264254154e-05], ["'market for polysulfone' (kilogram, GLO, None)", 4.019118309206293e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000924525276852141], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.495551281007104e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 5.907099145686869e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0006459351344950152], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 9.505013037587547e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -4.561969266059266e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.201080739405175e-05], ["'market for corrugated board box' (kilogram, RER, None)", 7.107201576755263e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.176104412433239e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.000406571962381337], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.927619458904985e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -4.059518539599607e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 1.6280211335475744e-06]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0006799317205210687], ["'alubox production - CONSQ' (kilogram, GLO, None)", 5.9310919264254154e-05], ["'market for polysulfone' (kilogram, GLO, None)", 4.019118309206293e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000924525276852141], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.495551281007104e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 5.907099145686869e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0006459351344950152], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 9.505013037587547e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -4.561969266059266e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.201080739405175e-05], ["'market for corrugated board box' (kilogram, RER, None)", 7.107201576755263e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.176104412433239e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.000406571962381337], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.927619458904985e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.2125415379144803e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 1.6280211335475744e-06]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00040627824320049955], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.543993514940177e-05], ["'market for polysulfone' (kilogram, GLO, None)", 2.0095591546031464e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000616350184568094], ["'cabinet washer - CONSQ' (unit, GLO, None)", 8.311680702169037e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.4911617735488555e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 3.529657156576897e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0003859643310404746], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 4.752506518793773e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.667989696812257e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.640932819683732e-07], ["'market for corrugated board box' (kilogram, RER, None)", 4.246751970234578e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.8978113291855574e-06]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00040627824320049955], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.543993514940177e-05], ["'market for polysulfone' (kilogram, GLO, None)", 2.0095591546031464e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000616350184568094], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.4911617735488555e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 3.529657156576897e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0003859643310404746], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 4.752506518793773e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -4.561969266059266e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.201080739405175e-05], ["'market for corrugated board box' (kilogram, RER, None)", 4.246751970234578e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.8978113291855574e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.000406571962381337], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.927619458904985e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -4.059518539599607e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 1.6280211335475744e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.1542416527930872], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.04709841261544819], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.02063117391319887], ["'market for corrugated board box' (kilogram, RER, None)", 0.009064392528043634], ["'autoclave - CONSQ' (unit, GLO, None)", 0.3136194154086757], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.00022704880868272586], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.08329049250826709], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.008701529761054663], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.08382272141506765], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.00012275371607556898], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0023423681624823384], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.10075442332658927], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.006893154355111719]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.1542416527930872], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.04709841261544819], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.02063117391319887], ["'market for corrugated board box' (kilogram, RER, None)", 0.009064392528043634], ["'autoclave - CONSQ' (unit, GLO, None)", 0.3136194154086757], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.00022704880868272586], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.18222330742406012], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.00026685590451210647], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.005092104723376794], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.21903135505018034], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.006893154355111719]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.4388283642845579], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.1339983006805709], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.06222099943016971], ["'market for corrugated board box' (kilogram, RER, None)", 0.02733705682567877], ["'autoclave - CONSQ' (unit, GLO, None)", 0.41815922054490096], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.000684750375565388], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.23696731671366128], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.026242708271574065], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.23848154543441785], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0004345938928302989], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.006664202419615243], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.28665342969915536], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.01961150957529672]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.4388283642845579], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.1339983006805709], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.06222099943016971], ["'market for corrugated board box' (kilogram, RER, None)", 0.02733705682567877], ["'autoclave - CONSQ' (unit, GLO, None)", 0.41815922054490096], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.003219989759056317], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.5184381422487344], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0008048035052412941], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.014487396543647602], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.6231596298265071], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.01961150957529672]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00040627824320049955], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.543993514940177e-05], ["'market for polysulfone' (kilogram, GLO, None)", 2.0095591546031464e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000616350184568094], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.4911617735488555e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 3.529657156576897e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0003859643310404746], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 4.752506518793773e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -4.561969266059266e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.201080739405175e-05], ["'market for corrugated board box' (kilogram, RER, None)", 4.246751970234578e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.8978113291855574e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.000406571962381337], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.927619458904985e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.2125415379144803e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 1.6280211335475744e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.1542416527930872], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.04709841261544819], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.02063117391319887], ["'market for corrugated board box' (kilogram, RER, None)", 0.009064392528043634], ["'autoclave - CONSQ' (unit, GLO, None)", 0.3136194154086757], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.00022704880868272586], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.08329049250826709], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.008701529761054663], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.08382272141506765], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.010168445776458772], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0023423681624823384], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.10075442332658927], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.006893154355111719]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.1542416527930872], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.04709841261544819], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.02063117391319887], ["'market for corrugated board box' (kilogram, RER, None)", 0.009064392528043634], ["'autoclave - CONSQ' (unit, GLO, None)", 0.3136194154086757], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.00022704880868272586], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.18222330742406012], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.022105316905345156], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.005092104723376794], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.21903135505018034], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.006893154355111719]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.4388283642845579], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.1339983006805709], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.06222099943016971], ["'market for corrugated board box' (kilogram, RER, None)", 0.02733705682567877], ["'autoclave - CONSQ' (unit, GLO, None)", 0.41815922054490096], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.000684750375565388], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.23696731671366128], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.026242708271574065], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.23848154543441785], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0360000868022972], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.006664202419615243], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.28665342969915536], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.01961150957529672]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.4388283642845579], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.1339983006805709], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.06222099943016971], ["'market for corrugated board box' (kilogram, RER, None)", 0.02733705682567877], ["'autoclave - CONSQ' (unit, GLO, None)", 0.41815922054490096], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.003219989759056317], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.5184381422487344], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.06666682741166148], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.014487396543647602], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.6231596298265071], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.01961150957529672]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.15652274511716874], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.02506742788826223], ["'market for polysulfone' (kilogram, GLO, None)", 0.0021337009725469172], ["'autoclave - CONSQ' (unit, GLO, None)", 0.6272388308173514], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.16276703443760637], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.0017058255370440256], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0050526572112086264], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.14869660786131028], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.000757439926670406], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00013091647106343603], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0011262459663236265], ["'market for corrugated board box' (kilogram, RER, None)", 0.0031990839685017074], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0021586743922518232]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.15652274511716874], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.02506742788826223], ["'market for polysulfone' (kilogram, GLO, None)", 0.0021337009725469172], ["'autoclave - CONSQ' (unit, GLO, None)", 0.6272388308173514], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.0017058255370440256], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0050526572112086264], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.14869660786131028], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.000757439926670406], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.004478388124218693], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.038841375330197256], ["'market for corrugated board box' (kilogram, RER, None)", 0.0031990839685017074], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0021586743922518232], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.010868049153376982], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.030809952373161937], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0003985142941020487], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 0.0018118957594268734]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.15652274511716874], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.02506742788826223], ["'market for polysulfone' (kilogram, GLO, None)", 0.0021337009725469172], ["'autoclave - CONSQ' (unit, GLO, None)", 0.6272388308173514], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.0017058255370440256], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0050526572112086264], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.14869660786131028], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.000757439926670406], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.004478388124218693], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.038841375330197256], ["'market for corrugated board box' (kilogram, RER, None)", 0.0031990839685017074], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0021586743922518232], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.010868049153376982], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.030809952373161937], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.033011391591809644], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 0.0018118957594268734]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.09352672332802628], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.01497849012867581], ["'market for polysulfone' (kilogram, GLO, None)", 0.0010668504862734586], ["'autoclave - CONSQ' (unit, GLO, None)", 0.41815922054490096], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.08138351721880319], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.0010192785267698358], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0030191041737117597], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.08885038716162497], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.000378719963335203], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.545823553171801e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0005631229831618132], ["'market for corrugated board box' (kilogram, RER, None)", 0.0019115422574496515], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0012898684002959776]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.09352672332802628], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.01497849012867581], ["'market for polysulfone' (kilogram, GLO, None)", 0.0010668504862734586], ["'autoclave - CONSQ' (unit, GLO, None)", 0.41815922054490096], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.0010192785267698358], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0030191041737117597], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.08885038716162497], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.000378719963335203], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.004478388124218693], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.038841375330197256], ["'market for corrugated board box' (kilogram, RER, None)", 0.0019115422574496515], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0012898684002959776], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.010868049153376982], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.030809952373161937], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0003985142941020487], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 0.0018118957594268734]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.002575880061279917], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.002681386540153435], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0004757341683104748], ["'market for corrugated board box' (kilogram, RER, None)", 0.0001428264265713875], ["'autoclave - CONSQ' (unit, GLO, None)", 0.008117449325061815], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 4.499571160094361e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0013909752330911553], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.00014971537875144706], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.004375708434223258], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -5.808364895075279e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.001108343554986862], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.002244252344669314], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00012908718849570378]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.002575880061279917], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.002681386540153435], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0004757341683104748], ["'market for corrugated board box' (kilogram, RER, None)", 0.0001428264265713875], ["'autoclave - CONSQ' (unit, GLO, None)", 0.008117449325061815], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 4.499571160094361e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.009512409639615778], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.00012626880206685387], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0024094425214061035], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.004878809444763506], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00012908718849570378]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.007328560174345679], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.007628733536774561], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0014347538118721001], ["'market for corrugated board box' (kilogram, RER, None)", 0.00043074636577255046], ["'autoclave - CONSQ' (unit, GLO, None)", 0.010823265766749086], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.3570135248158271e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.003957422494146667], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0004515225616910651], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.012449198643846453], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0002056377592003514], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0031533154861022395], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.006385055965478946], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.000367262141947291]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.007328560174345679], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.007628733536774561], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0014347538118721001], ["'market for corrugated board box' (kilogram, RER, None)", 0.00043074636577255046], ["'autoclave - CONSQ' (unit, GLO, None)", 0.010823265766749086], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.381259227787924e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.02706347531270968], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0003808106651858359], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.006855033655629201], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.013880556447712073], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.000367262141947291]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.09352672332802628], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.01497849012867581], ["'market for polysulfone' (kilogram, GLO, None)", 0.0010668504862734586], ["'autoclave - CONSQ' (unit, GLO, None)", 0.41815922054490096], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.0010192785267698358], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0030191041737117597], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.08885038716162497], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.000378719963335203], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.004478388124218693], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.038841375330197256], ["'market for corrugated board box' (kilogram, RER, None)", 0.0019115422574496515], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0012898684002959776], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.010868049153376982], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.030809952373161937], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.033011391591809644], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 0.0018118957594268734]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.002575880061279917], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.002681386540153435], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0004757341683104748], ["'market for corrugated board box' (kilogram, RER, None)", 0.0001428264265713875], ["'autoclave - CONSQ' (unit, GLO, None)", 0.008117449325061815], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 4.499571160094361e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0013909752330911553], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.00014971537875144706], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.004375708434223258], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0005306180005877085], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.001108343554986862], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.002244252344669314], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00012908718849570378]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.002575880061279917], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.002681386540153435], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0004757341683104748], ["'market for corrugated board box' (kilogram, RER, None)", 0.0001428264265713875], ["'autoclave - CONSQ' (unit, GLO, None)", 0.008117449325061815], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 4.499571160094361e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.009512409639615778], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.001153517392581975], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0024094425214061035], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.004878809444763506], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00012908718849570378]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.007328560174345679], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.007628733536774561], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0014347538118721001], ["'market for corrugated board box' (kilogram, RER, None)", 0.00043074636577255046], ["'autoclave - CONSQ' (unit, GLO, None)", 0.010823265766749086], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.3570135248158271e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.003957422494146667], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0004515225616910651], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.012449198643846453], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0018785854298641296], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0031533154861022395], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.006385055965478946], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.000367262141947291]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.007328560174345679], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.007628733536774561], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0014347538118721001], ["'market for corrugated board box' (kilogram, RER, None)", 0.00043074636577255046], ["'autoclave - CONSQ' (unit, GLO, None)", 0.010823265766749086], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.381259227787924e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.02706347531270968], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0034788619071557956], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.006855033655629201], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.013880556447712073], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.000367262141947291]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0037239953774620004], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0014142961560177963], ["'market for polysulfone' (kilogram, GLO, None)", 5.2525211287247595e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.01623489865012363], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.006926399749254169], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.632351514481635e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.001537849262441289], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0035377956085889], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.7775049817998695e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.194603788971084e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.508654277542893e-05], ["'market for corrugated board box' (kilogram, RER, None)", 5.0407540285717045e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.0425209391520094e-05]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0037239953774620004], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0014142961560177963], ["'market for polysulfone' (kilogram, GLO, None)", 5.2525211287247595e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.01623489865012363], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.632351514481635e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.001537849262441289], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0035377956085889], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.7775049817998695e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.002119048872721739], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0008651714215307485], ["'market for corrugated board box' (kilogram, RER, None)", 5.0407540285717045e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.0425209391520094e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -0.00301221424263572], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.000710446585812281], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0001885658951964494], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.354023179482034e-05]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0037239953774620004], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0014142961560177963], ["'market for polysulfone' (kilogram, GLO, None)", 5.2525211287247595e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.01623489865012363], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.632351514481635e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.001537849262441289], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0035377956085889], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.7775049817998695e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.002119048872721739], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0008651714215307485], ["'market for corrugated board box' (kilogram, RER, None)", 5.0407540285717045e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.0425209391520094e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -0.00301221424263572], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.000710446585812281], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0017226269371093741], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.354023179482034e-05]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0022251915214112454], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0008450815578831715], ["'market for polysulfone' (kilogram, GLO, None)", 2.6262605643623798e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.010823265766749086], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.0034631998746270844], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.767959750059128e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0009189079988399667], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0021139319453406832], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.8887524908999347e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.097301894485542e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.2543271387714466e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.0119916919646303e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.4155194667907616e-05]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0022251915214112454], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0008450815578831715], ["'market for polysulfone' (kilogram, GLO, None)", 2.6262605643623798e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.010823265766749086], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.767959750059128e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0009189079988399667], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0021139319453406832], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.8887524908999347e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.002119048872721739], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0008651714215307485], ["'market for corrugated board box' (kilogram, RER, None)", 3.0119916919646303e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.4155194667907616e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -0.00301221424263572], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.000710446585812281], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0001885658951964494], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.354023179482034e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0034951468413655707], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.003493197791441804], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0006326924433916711], ["'market for corrugated board box' (kilogram, RER, None)", 0.00020000116535978177], ["'autoclave - CONSQ' (unit, GLO, None)", 0.009204020002652483], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.396241821226289e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0018873792943374082], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.00020290888734322889], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.006334986637136535], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -7.171006407607947e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0013683607828049085], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0028768610170369943], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00016294154332445007]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0034951468413655707], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.003493197791441804], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0006326924433916711], ["'market for corrugated board box' (kilogram, RER, None)", 0.00020000116535978177], ["'autoclave - CONSQ' (unit, GLO, None)", 0.009204020002652483], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.396241821226289e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.013771710080731598], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.00015589144364365102], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.002974697366967384], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.006254045688993213], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00016294154332445007]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.009943938900786552], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0099383937164964], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0019081200287183278], ["'market for corrugated board box' (kilogram, RER, None)", 0.0006031781176429667], ["'autoclave - CONSQ' (unit, GLO, None)", 0.012272026670203311], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.929025311650959e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.005369727006424739], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0006119474256228533], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.01802348310847296], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0002538803459338703], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.003893082814962413], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.008184872187976932], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0004635801655524203]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.009943938900786552], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0099383937164964], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0019081200287183278], ["'market for corrugated board box' (kilogram, RER, None)", 0.0006031781176429667], ["'autoclave - CONSQ' (unit, GLO, None)", 0.012272026670203311], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 9.071103821371131e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.039181485018419476], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.00047014878876642645], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.008463223498675876], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.01779320040995137], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0004635801655524203]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0022251915214112454], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0008450815578831715], ["'market for polysulfone' (kilogram, GLO, None)", 2.6262605643623798e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.010823265766749086], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.767959750059128e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0009189079988399667], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0021139319453406832], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.8887524908999347e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.002119048872721739], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0008651714215307485], ["'market for corrugated board box' (kilogram, RER, None)", 3.0119916919646303e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.4155194667907616e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -0.00301221424263572], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.000710446585812281], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0017226269371093741], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.354023179482034e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0034951468413655707], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.003493197791441804], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0006326924433916711], ["'market for corrugated board box' (kilogram, RER, None)", 0.00020000116535978177], ["'autoclave - CONSQ' (unit, GLO, None)", 0.009204020002652483], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.396241821226289e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0018873792943374082], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.00020290888734322889], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.006334986637136535], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0007682661196503023], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0013683607828049085], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0028768610170369943], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00016294154332445007]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0034951468413655707], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.003493197791441804], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0006326924433916711], ["'market for corrugated board box' (kilogram, RER, None)", 0.00020000116535978177], ["'autoclave - CONSQ' (unit, GLO, None)", 0.009204020002652483], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.396241821226289e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.013771710080731598], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0016701437383702224], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.002974697366967384], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.006254045688993213], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00016294154332445007]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.009943938900786552], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0099383937164964], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0019081200287183278], ["'market for corrugated board box' (kilogram, RER, None)", 0.0006031781176429667], ["'autoclave - CONSQ' (unit, GLO, None)", 0.012272026670203311], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.929025311650959e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.005369727006424739], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0006119474256228533], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.01802348310847296], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0027199483188183843], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.003893082814962413], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.008184872187976932], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0004635801655524203]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.009943938900786552], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0099383937164964], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0019081200287183278], ["'market for corrugated board box' (kilogram, RER, None)", 0.0006031781176429667], ["'autoclave - CONSQ' (unit, GLO, None)", 0.012272026670203311], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 9.071103821371131e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.039181485018419476], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.005036941331145155], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.008463223498675876], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.01779320040995137], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0004635801655524203]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.005214791760272705], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0018439750484988964], ["'market for polysulfone' (kilogram, GLO, None)", 6.729644141243289e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.018408040005304965], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.008443231015985712], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.828661645115836e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0021159771037727914], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.004954052172259069], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 5.029642135612412e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -7.647856886706219e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.215792427900825e-05], ["'market for corrugated board box' (kilogram, RER, None)", 7.058614460976231e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -5.102710876445776e-05]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.005214791760272705], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0018439750484988964], ["'market for polysulfone' (kilogram, GLO, None)", 6.729644141243289e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.018408040005304965], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.828661645115836e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0021159771037727914], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.004954052172259069], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 5.029642135612412e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0026161774128904904], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0011090454874953188], ["'market for corrugated board box' (kilogram, RER, None)", 7.058614460976231e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -5.102710876445776e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -0.000575151872486603], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0009448431839007462], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.00023280342525597167], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 3.126067645767488e-05]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.005214791760272705], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0018439750484988964], ["'market for polysulfone' (kilogram, GLO, None)", 6.729644141243289e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.018408040005304965], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.828661645115836e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0021159771037727914], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.004954052172259069], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 5.029642135612412e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0026161774128904904], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0011090454874953188], ["'market for corrugated board box' (kilogram, RER, None)", 7.058614460976231e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -5.102710876445776e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -0.000575151872486603], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0009448431839007462], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0024941406268017227], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 3.126067645767488e-05]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.003115984107045915], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0011018267284773244], ["'market for polysulfone' (kilogram, GLO, None)", 3.3648220706216446e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.012272026670203311], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.004221615507992856], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.6778445596733054e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0012643555734015094], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0029601849016936193], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.514821067806206e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.8239284433531094e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.6078962139504127e-05], ["'market for corrugated board box' (kilogram, RER, None)", 4.2177198079363444e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.0490126435919597e-05]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.003115984107045915], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0011018267284773244], ["'market for polysulfone' (kilogram, GLO, None)", 3.3648220706216446e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.012272026670203311], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.6778445596733054e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0012643555734015094], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0029601849016936193], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.514821067806206e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0026161774128904904], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0011090454874953188], ["'market for corrugated board box' (kilogram, RER, None)", 4.2177198079363444e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.0490126435919597e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -0.000575151872486603], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0009448431839007462], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.00023280342525597167], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 3.126067645767488e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.4246843526982598], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.26410464946150747], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.05097297854386099], ["'market for corrugated board box' (kilogram, RER, None)", 0.014805773880272764], ["'autoclave - CONSQ' (unit, GLO, None)", 1.1292716339098199], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.0008182394338512325], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.22932955045706033], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.024969496910015338], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.24355136923318338], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.003639984059497851], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.06945763472986953], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.22575725177525385], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.023218345690887605]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.4246843526982598], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.26410464946150747], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.05097297854386099], ["'market for corrugated board box' (kilogram, RER, None)", 0.014805773880272764], ["'autoclave - CONSQ' (unit, GLO, None)", 1.1292716339098199], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.0008182394338512325], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.5294594983330074], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.007913008824995328], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.1509948587705053], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.49077663427695084], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.023218345690887605]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.2082568907753308], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.7513963266369649], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.1537280274149883], ["'market for corrugated board box' (kilogram, RER, None)", 0.0446523339165811], ["'autoclave - CONSQ' (unit, GLO, None)", 1.50569551187976], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.0024677062296987484], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.6524587210186786], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.07530483042536665], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.6929207969732823], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.012886899825367042], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.19761186343013165], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.6422952795934875], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.06605782859072676]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.2082568907753308], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.7513963266369649], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.1537280274149883], ["'market for corrugated board box' (kilogram, RER, None)", 0.0446523339165811], ["'autoclave - CONSQ' (unit, GLO, None)", 1.50569551187976], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.011604212383861145], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.5063495586375701], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.02386462930623526], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.429591006842007], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.3962940861752748], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.06605782859072676]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.003115984107045915], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0011018267284773244], ["'market for polysulfone' (kilogram, GLO, None)", 3.3648220706216446e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.012272026670203311], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.6778445596733054e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0012643555734015094], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0029601849016936193], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.514821067806206e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0026161774128904904], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0011090454874953188], ["'market for corrugated board box' (kilogram, RER, None)", 4.2177198079363444e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.0490126435919597e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -0.000575151872486603], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0009448431839007462], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0024941406268017227], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 3.126067645767488e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.4246843526982598], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.26410464946150747], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.05097297854386099], ["'market for corrugated board box' (kilogram, RER, None)", 0.014805773880272764], ["'autoclave - CONSQ' (unit, GLO, None)", 1.1292716339098199], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.0008182394338512325], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.22932955045706033], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.024969496910015338], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.24355136923318338], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.02954250996483097], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.06945763472986953], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.22575725177525385], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.023218345690887605]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.4246843526982598], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.26410464946150747], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.05097297854386099], ["'market for corrugated board box' (kilogram, RER, None)", 0.014805773880272764], ["'autoclave - CONSQ' (unit, GLO, None)", 1.1292716339098199], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.0008182394338512325], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.5294594983330074], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.06422284774963255], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.1509948587705053], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.49077663427695084], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.023218345690887605]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.2082568907753308], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.7513963266369649], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.1537280274149883], ["'market for corrugated board box' (kilogram, RER, None)", 0.0446523339165811], ["'autoclave - CONSQ' (unit, GLO, None)", 1.50569551187976], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.0024677062296987484], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.6524587210186786], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.07530483042536665], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.6929207969732823], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.10459149278780218], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.19761186343013165], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.6422952795934875], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.06605782859072676]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.2082568907753308], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.7513963266369649], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.1537280274149883], ["'market for corrugated board box' (kilogram, RER, None)", 0.0446523339165811], ["'autoclave - CONSQ' (unit, GLO, None)", 1.50569551187976], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.011604212383861145], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.5063495586375701], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.19368794960704105], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.429591006842007], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.3962940861752748], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.06605782859072676]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.13224599475672763], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.06762232827194302], ["'market for polysulfone' (kilogram, GLO, None)", 0.008388737139565776], ["'autoclave - CONSQ' (unit, GLO, None)", 2.2585432678196398], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.4854281992055989], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.032035708103587614], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.47366216002384215], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.12563369501889124], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.0003957376479410388], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0038820321130095775], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0025235437391768374], ["'market for corrugated board box' (kilogram, RER, None)", 0.005225382033611543], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.007271104880482139]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.13224599475672763], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.06762232827194302], ["'market for polysulfone' (kilogram, GLO, None)", 0.008388737139565776], ["'autoclave - CONSQ' (unit, GLO, None)", 2.2585432678196398], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.032035708103587614], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.47366216002384215], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.12563369501889124], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.0003957376479410388], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.13279647985862383], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.087030642032392], ["'market for corrugated board box' (kilogram, RER, None)", 0.005225382033611543], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.007271104880482139], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.02761327726609024], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.07612145813233852], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.011817040855370064], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -0.0014486263719564294]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.13224599475672763], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.06762232827194302], ["'market for polysulfone' (kilogram, GLO, None)", 0.008388737139565776], ["'autoclave - CONSQ' (unit, GLO, None)", 2.2585432678196398], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.032035708103587614], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.47366216002384215], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.12563369501889124], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.0003957376479410388], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.13279647985862383], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.087030642032392], ["'market for corrugated board box' (kilogram, RER, None)", 0.005225382033611543], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.007271104880482139], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.02761327726609024], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.07612145813233852], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.09590840001446192], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -0.0014486263719564294]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.07902068516363756], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0404062347766303], ["'market for polysulfone' (kilogram, GLO, None)", 0.004194368569782888], ["'autoclave - CONSQ' (unit, GLO, None)", 1.50569551187976], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.24271409960279944], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.019142232690710696], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.2830264046183406], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.07506965090545568], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.0001978688239705194], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0019410160565047887], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0012617718695884187], ["'market for corrugated board box' (kilogram, RER, None)", 0.0031223120952479397], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.004344688784114543]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.07902068516363756], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0404062347766303], ["'market for polysulfone' (kilogram, GLO, None)", 0.004194368569782888], ["'autoclave - CONSQ' (unit, GLO, None)", 1.50569551187976], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.019142232690710696], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.2830264046183406], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.07506965090545568], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.0001978688239705194], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.13279647985862383], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.087030642032392], ["'market for corrugated board box' (kilogram, RER, None)", 0.0031223120952479397], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.004344688784114543], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.02761327726609024], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.07612145813233852], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.011817040855370064], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -0.0014486263719564294]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.11757236403331361], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.011546059896976347], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.013085324881130274], ["'market for corrugated board box' (kilogram, RER, None)", 0.0010078044055488917], ["'autoclave - CONSQ' (unit, GLO, None)", 0.011794864263106601], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.275383538786159e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.06348907657798936], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.006385849014992495], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0003101352144363789], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -2.9267281593496865e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0005584739167065958], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.015215451300440504], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0008178808066219231]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.11757236403331361], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.011546059896976347], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.013085324881130274], ["'market for corrugated board box' (kilogram, RER, None)", 0.0010078044055488917], ["'autoclave - CONSQ' (unit, GLO, None)", 0.011794864263106601], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.275383538786159e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0006742069879051715], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -6.362452520325406e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0012140737372944197], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.03307706804328478], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0008178808066219231]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.33450165541872323], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.03284935350970735], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.03946367741350463], ["'market for corrugated board box' (kilogram, RER, None)", 0.0030394101114248266], ["'autoclave - CONSQ' (unit, GLO, None)", 0.015726485684142134], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.00018925759883661535], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.18063089392611056], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.019258909337621453], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0008823565255795569], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.000103617081803439], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0015888976321569858], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.04328903045332324], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0023269284922689485]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.33450165541872323], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.03284935350970735], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.03946367741350463], ["'market for corrugated board box' (kilogram, RER, None)", 0.0030394101114248266], ["'autoclave - CONSQ' (unit, GLO, None)", 0.015726485684142134], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.0008899703480619658], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0019181663599555584], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.00019188348482118331], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00345412528235449], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.09410658794891366], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0023269284922689485]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.07902068516363756], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0404062347766303], ["'market for polysulfone' (kilogram, GLO, None)", 0.004194368569782888], ["'autoclave - CONSQ' (unit, GLO, None)", 1.50569551187976], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.019142232690710696], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.2830264046183406], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.07506965090545568], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.0001978688239705194], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.13279647985862383], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.087030642032392], ["'market for corrugated board box' (kilogram, RER, None)", 0.0031223120952479397], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.004344688784114543], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.02761327726609024], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.07612145813233852], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.09590840001446192], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -0.0014486263719564294]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.11757236403331361], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.011546059896976347], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.013085324881130274], ["'market for corrugated board box' (kilogram, RER, None)", 0.0010078044055488917], ["'autoclave - CONSQ' (unit, GLO, None)", 0.011794864263106601], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.275383538786159e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.06348907657798936], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.006385849014992495], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0003101352144363789], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.690670946455437e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0005584739167065958], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.015215451300440504], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0008178808066219231]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.11757236403331361], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.011546059896976347], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.013085324881130274], ["'market for corrugated board box' (kilogram, RER, None)", 0.0010078044055488917], ["'autoclave - CONSQ' (unit, GLO, None)", 0.011794864263106601], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.275383538786159e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0006742069879051715], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.023197709685732e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0012140737372944197], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.03307706804328478], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0008178808066219231]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.33450165541872323], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.03284935350970735], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.03946367741350463], ["'market for corrugated board box' (kilogram, RER, None)", 0.0030394101114248266], ["'autoclave - CONSQ' (unit, GLO, None)", 0.015726485684142134], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.00018925759883661535], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.18063089392611056], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.019258909337621453], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0008823565255795569], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00013066350291084805], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0015888976321569858], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.04328903045332324], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0023269284922689485]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.33450165541872323], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.03284935350970735], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.03946367741350463], ["'market for corrugated board box' (kilogram, RER, None)", 0.0030394101114248266], ["'autoclave - CONSQ' (unit, GLO, None)", 0.015726485684142134], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.0008899703480619658], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0019181663599555584], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00024196944983490376], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00345412528235449], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.09410658794891366], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0023269284922689485]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.033832419440732626], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.006149296159342674], ["'market for polysulfone' (kilogram, GLO, None)", 0.0011275973997964702], ["'autoclave - CONSQ' (unit, GLO, None)", 0.023589728526213202], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.004343848313710668], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.000535042693546586], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.000971249625905885], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.032140798468696], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 4.876235116799861e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.1213468287034964e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00017008028121374185], ["'market for corrugated board box' (kilogram, RER, None)", 0.0003556830650484527], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00025612923521141666]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.033832419440732626], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.006149296159342674], ["'market for polysulfone' (kilogram, GLO, None)", 0.0011275973997964702], ["'autoclave - CONSQ' (unit, GLO, None)", 0.023589728526213202], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.000535042693546586], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.000971249625905885], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.032140798468696], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 4.876235116799861e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0010677497228335797], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00586563880042361], ["'market for corrugated board box' (kilogram, RER, None)", 0.0003556830650484527], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00025612923521141666], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.002322671898890378], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.019541216513959615], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -9.50148837639922e-05], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -3.41135056606014e-05]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.033832419440732626], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.006149296159342674], ["'market for polysulfone' (kilogram, GLO, None)", 0.0011275973997964702], ["'autoclave - CONSQ' (unit, GLO, None)", 0.023589728526213202], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.000535042693546586], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.000971249625905885], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.032140798468696], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 4.876235116799861e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0010677497228335797], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00586563880042361], ["'market for corrugated board box' (kilogram, RER, None)", 0.0003556830650484527], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00025612923521141666], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.002322671898890378], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.019541216513959615], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00011981593502914338], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -3.41135056606014e-05]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.02021581802812413], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0036743766545010107], ["'market for polysulfone' (kilogram, GLO, None)", 0.0005637986998982351], ["'autoclave - CONSQ' (unit, GLO, None)", 0.015726485684142134], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.002171924156855334], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.000319702992242784], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0005803488494694493], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.019205027126717927], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.4381175583999304e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.5606734143517482e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -8.504014060687093e-05], ["'market for corrugated board box' (kilogram, RER, None)", 0.00021253059181743317], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00015304439061166296]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.02021581802812413], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0036743766545010107], ["'market for polysulfone' (kilogram, GLO, None)", 0.0005637986998982351], ["'autoclave - CONSQ' (unit, GLO, None)", 0.015726485684142134], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.000319702992242784], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0005803488494694493], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.019205027126717927], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.4381175583999304e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0010677497228335797], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00586563880042361], ["'market for corrugated board box' (kilogram, RER, None)", 0.00021253059181743317], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00015304439061166296], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.002322671898890378], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.019541216513959615], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -9.50148837639922e-05], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -3.41135056606014e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.6107683632415326e-05], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 2.1979795666106068e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.66479725541961e-06], ["'market for corrugated board box' (kilogram, RER, None)", 6.970377403646815e-06], ["'autoclave - CONSQ' (unit, GLO, None)", -2.297772908378533e-05], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.5474719020016852e-08], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -8.698149161504277e-06], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.0066393616264027e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.40526299876735e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -4.784905353066169e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -9.130485265809544e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -8.73795938304418e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.590766710592349e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.6107683632415326e-05], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 2.1979795666106068e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.66479725541961e-06], ["'market for corrugated board box' (kilogram, RER, None)", 6.970377403646815e-06], ["'autoclave - CONSQ' (unit, GLO, None)", -2.297772908378533e-05], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.5474719020016852e-08], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.054919562537718e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.0401968158839498e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.9848881099664267e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.8995563875521945e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.590766710592349e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 4.5827494278139374e-05], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 6.253406654300599e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.4068435882149842e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.1021773118319107e-05], ["'autoclave - CONSQ' (unit, GLO, None)", -3.0636972111713774e-05], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.682851769883089e-08], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -2.4746846910195263e-05], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -3.035896425945613e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.998072193676123e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.6940347801229882e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.5976873736272905e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.486010978994426e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.525843317828836e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 4.5827494278139374e-05], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 6.253406654300599e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.4068435882149842e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.1021773118319107e-05], ["'autoclave - CONSQ' (unit, GLO, None)", -3.0636972111713774e-05], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.6128061994774187e-07], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.691461290600267e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -3.1371014446722e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.647146456325348e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.404371693862777e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.525843317828836e-06]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.02021581802812413], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0036743766545010107], ["'market for polysulfone' (kilogram, GLO, None)", 0.0005637986998982351], ["'autoclave - CONSQ' (unit, GLO, None)", 0.015726485684142134], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.000319702992242784], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0005803488494694493], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.019205027126717927], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.4381175583999304e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0010677497228335797], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00586563880042361], ["'market for corrugated board box' (kilogram, RER, None)", 0.00021253059181743317], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00015304439061166296], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.002322671898890378], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.019541216513959615], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00011981593502914338], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -3.41135056606014e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.6107683632415326e-05], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 2.1979795666106068e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.66479725541961e-06], ["'market for corrugated board box' (kilogram, RER, None)", 6.970377403646815e-06], ["'autoclave - CONSQ' (unit, GLO, None)", -2.297772908378533e-05], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.5474719020016852e-08], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -8.698149161504277e-06], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.0066393616264027e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.40526299876735e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.573026213528871e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -9.130485265809544e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -8.73795938304418e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.590766710592349e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.6107683632415326e-05], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 2.1979795666106068e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.66479725541961e-06], ["'market for corrugated board box' (kilogram, RER, None)", 6.970377403646815e-06], ["'autoclave - CONSQ' (unit, GLO, None)", -2.297772908378533e-05], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.5474719020016852e-08], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.054919562537718e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.419622203323633e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.9848881099664267e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.8995563875521945e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.590766710592349e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 4.5827494278139374e-05], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 6.253406654300599e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.4068435882149842e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.1021773118319107e-05], ["'autoclave - CONSQ' (unit, GLO, None)", -3.0636972111713774e-05], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.682851769883089e-08], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -2.4746846910195263e-05], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -3.035896425945613e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.998072193676123e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.569098904026384e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.5976873736272905e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.486010978994426e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.525843317828836e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 4.5827494278139374e-05], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 6.253406654300599e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.4068435882149842e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.1021773118319107e-05], ["'autoclave - CONSQ' (unit, GLO, None)", -3.0636972111713774e-05], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.6128061994774187e-07], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.691461290600267e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.0313146118567377e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.647146456325348e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.404371693862777e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.525843317828836e-06]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 5.11835150644143e-05], ["'alubox production - CONSQ' (kilogram, GLO, None)", 1.2403929145125681e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.9126691235872395e-07], ["'autoclave - CONSQ' (unit, GLO, None)", -4.595545816757066e-05], ["'cabinet washer - CONSQ' (unit, GLO, None)", 3.457256187858905e-06], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.673248658294235e-07], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 2.9829706100578206e-06], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -4.862433931119358e-05], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.6405520745686866e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.1030872483757e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -9.767403935362618e-08], ["'market for corrugated board box' (kilogram, RER, None)", 2.4600460027988033e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.981677741853955e-07]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 5.11835150644143e-05], ["'alubox production - CONSQ' (kilogram, GLO, None)", 1.2403929145125681e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.9126691235872395e-07], ["'autoclave - CONSQ' (unit, GLO, None)", -4.595545816757066e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.673248658294235e-07], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 2.9829706100578206e-06], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -4.862433931119358e-05], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.6405520745686866e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.7456631044464828e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.3685306194122313e-06], ["'market for corrugated board box' (kilogram, RER, None)", 2.4600460027988033e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.981677741853955e-07], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -5.585643992490576e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.9662628929703256e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.5533975182864459e-07], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.105538325255076e-08]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 5.11835150644143e-05], ["'alubox production - CONSQ' (kilogram, GLO, None)", 1.2403929145125681e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.9126691235872395e-07], ["'autoclave - CONSQ' (unit, GLO, None)", -4.595545816757066e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.673248658294235e-07], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 2.9829706100578206e-06], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -4.862433931119358e-05], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.6405520745686866e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.7456631044464828e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.3685306194122313e-06], ["'market for corrugated board box' (kilogram, RER, None)", 2.4600460027988033e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.981677741853955e-07], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -5.585643992490576e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.9662628929703256e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.1067572626686445e-08], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.105538325255076e-08]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 3.0583583547566214e-05], ["'alubox production - CONSQ' (kilogram, GLO, None)", 7.411695012556751e-06], ["'market for polysulfone' (kilogram, GLO, None)", 9.563345617936197e-08], ["'autoclave - CONSQ' (unit, GLO, None)", -3.0636972111713774e-05], ["'cabinet washer - CONSQ' (unit, GLO, None)", 1.7286280939294524e-06], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 9.998129294635685e-08], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.7824084719039972e-06], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -2.90544043701879e-05], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.8202760372843433e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.55154362418785e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.883701967681309e-08], ["'market for corrugated board box' (kilogram, RER, None)", 1.4699463771257078e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.976691956294648e-07]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 3.0583583547566214e-05], ["'alubox production - CONSQ' (kilogram, GLO, None)", 7.411695012556751e-06], ["'market for polysulfone' (kilogram, GLO, None)", 9.563345617936197e-08], ["'autoclave - CONSQ' (unit, GLO, None)", -3.0636972111713774e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 9.998129294635685e-08], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.7824084719039972e-06], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -2.90544043701879e-05], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.8202760372843433e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.7456631044464828e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.3685306194122313e-06], ["'market for corrugated board box' (kilogram, RER, None)", 1.4699463771257078e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.976691956294648e-07], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -5.585643992490576e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.9662628929703256e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.5533975182864459e-07], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.105538325255076e-08]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.889600857085989e-06], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 2.610063690232733e-06], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.497219433011155e-07], ["'market for corrugated board box' (kilogram, RER, None)", 4.0183387331173233e-07], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00013286553723601384], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 5.416698624596908e-09], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -1.0203844628264341e-06], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.1181151213323185e-07], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.3082978885587858e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -5.1120125029280634e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -9.75466626663982e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -7.69691715696436e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 7.777152232684407e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.889600857085989e-06], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 2.610063690232733e-06], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.497219433011155e-07], ["'market for corrugated board box' (kilogram, RER, None)", 4.0183387331173233e-07], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00013286553723601384], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 5.416698624596908e-09], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.8441258446930124e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.1113070658539269e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.1205796324810419e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.6732428601514137e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 7.777152232684407e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 5.376047508892532e-06], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 7.425815006014254e-06], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.9594788369286424e-06], ["'market for corrugated board box' (kilogram, RER, None)", 1.2118799351660813e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00017715404964801845], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.633607522116651e-08], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -2.9030656548019673e-06], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -3.3720931547561873e-07], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.7221996266038696e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.8098428991567045e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.7752712651195124e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.18982713443991e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.2126545790567683e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 5.376047508892532e-06], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 7.425815006014254e-06], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.9594788369286424e-06], ["'market for corrugated board box' (kilogram, RER, None)", 1.2118799351660813e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00017715404964801845], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.681922754974344e-08], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.091738318704064e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -3.3515609243642666e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.033198393799426e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.760493770870923e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.2126545790567683e-05]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 3.0583583547566214e-05], ["'alubox production - CONSQ' (kilogram, GLO, None)", 7.411695012556751e-06], ["'market for polysulfone' (kilogram, GLO, None)", 9.563345617936197e-08], ["'autoclave - CONSQ' (unit, GLO, None)", -3.0636972111713774e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 9.998129294635685e-08], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.7824084719039972e-06], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -2.90544043701879e-05], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.8202760372843433e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.7456631044464828e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.3685306194122313e-06], ["'market for corrugated board box' (kilogram, RER, None)", 1.4699463771257078e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.976691956294648e-07], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -5.585643992490576e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.9662628929703256e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.1067572626686445e-08], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.105538325255076e-08]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.889600857085989e-06], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 2.610063690232733e-06], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.497219433011155e-07], ["'market for corrugated board box' (kilogram, RER, None)", 4.0183387331173233e-07], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00013286553723601384], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 5.416698624596908e-09], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -1.0203844628264341e-06], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.1181151213323185e-07], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.3082978885587858e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.5813325777144055e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -9.75466626663982e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -7.69691715696436e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 7.777152232684407e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.889600857085989e-06], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 2.610063690232733e-06], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.497219433011155e-07], ["'market for corrugated board box' (kilogram, RER, None)", 4.0183387331173233e-07], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00013286553723601384], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 5.416698624596908e-09], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.8441258446930124e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.437679516770447e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.1205796324810419e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.6732428601514137e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 7.777152232684407e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 5.376047508892532e-06], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 7.425815006014254e-06], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.9594788369286424e-06], ["'market for corrugated board box' (kilogram, RER, None)", 1.2118799351660813e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00017715404964801845], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.633607522116651e-08], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -2.9030656548019673e-06], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -3.3720931547561873e-07], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.7221996266038696e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.5985065281869045e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.7752712651195124e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.18982713443991e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.2126545790567683e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 5.376047508892532e-06], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 7.425815006014254e-06], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.9594788369286424e-06], ["'market for corrugated board box' (kilogram, RER, None)", 1.2118799351660813e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00017715404964801845], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.681922754974344e-08], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.091738318704064e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.03676046818276e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.033198393799426e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.760493770870923e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.2126545790567683e-05]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 3.692348298539384e-06], ["'alubox production - CONSQ' (kilogram, GLO, None)", 2.0619203610568115e-06], ["'market for polysulfone' (kilogram, GLO, None)", 8.462756924699476e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002657310744720277], ["'cabinet washer - CONSQ' (unit, GLO, None)", 1.1320412288153831e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.5525177438659536e-08], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 6.292610430619047e-08], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -3.5077308836124148e-06], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 6.849922026495211e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.4519460453930945e-09], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -8.603713479714355e-09], ["'market for corrugated board box' (kilogram, RER, None)", 1.4181869310440799e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.435508985358827e-06]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 3.692348298539384e-06], ["'alubox production - CONSQ' (kilogram, GLO, None)", 2.0619203610568115e-06], ["'market for polysulfone' (kilogram, GLO, None)", 8.462756924699476e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002657310744720277], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.5525177438659536e-08], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 6.292610430619047e-08], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -3.5077308836124148e-06], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 6.849922026495211e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.865000654634105e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.967203208637608e-07], ["'market for corrugated board box' (kilogram, RER, None)", 1.4181869310440799e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.435508985358827e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.00012707952535413478], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 9.70274508524164e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.6595913502048998e-08], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.5676381986026424e-07]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 3.692348298539384e-06], ["'alubox production - CONSQ' (kilogram, GLO, None)", 2.0619203610568115e-06], ["'market for polysulfone' (kilogram, GLO, None)", 8.462756924699476e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002657310744720277], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.5525177438659536e-08], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 6.292610430619047e-08], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -3.5077308836124148e-06], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 6.849922026495211e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.865000654634105e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.967203208637608e-07], ["'market for corrugated board box' (kilogram, RER, None)", 1.4181869310440799e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.435508985358827e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.00012707952535413478], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 9.70274508524164e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.1337234920080076e-08], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.5676381986026424e-07]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 2.2062815055389833e-06], ["'alubox production - CONSQ' (kilogram, GLO, None)", 1.2320551558728802e-06], ["'market for polysulfone' (kilogram, GLO, None)", 4.231378462349738e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00017715404964801845], ["'cabinet washer - CONSQ' (unit, GLO, None)", 5.6602061440769155e-06], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.7202568365239955e-08], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 3.76001094483108e-08], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -2.095967430262034e-06], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.4249610132476057e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.7259730226965472e-09], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.3018567398571776e-09], ["'market for corrugated board box' (kilogram, RER, None)", 8.474064058166177e-08], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.4552848220774163e-06]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 2.2062815055389833e-06], ["'alubox production - CONSQ' (kilogram, GLO, None)", 1.2320551558728802e-06], ["'market for polysulfone' (kilogram, GLO, None)", 4.231378462349738e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00017715404964801845], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.7202568365239955e-08], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 3.76001094483108e-08], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -2.095967430262034e-06], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.4249610132476057e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.865000654634105e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.967203208637608e-07], ["'market for corrugated board box' (kilogram, RER, None)", 8.474064058166177e-08], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.4552848220774163e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.00012707952535413478], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 9.70274508524164e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.6595913502048998e-08], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.5676381986026424e-07]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.003517252466384169], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0017785803198210638], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0005449558282524257], ["'market for corrugated board box' (kilogram, RER, None)", 0.00027532070921551684], ["'autoclave - CONSQ' (unit, GLO, None)", 0.001364620512139065], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.6041536632474646e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0018993163318474513], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0002603292224294203], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00019388848660040697], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.783486055448272e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0003403221579004145], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.000851953695479976], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -7.659206092784872e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.003517252466384169], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0017785803198210638], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0005449558282524257], ["'market for corrugated board box' (kilogram, RER, None)", 0.00027532070921551684], ["'autoclave - CONSQ' (unit, GLO, None)", 0.001364620512139065], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.6041536632474646e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00042149671000088474], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -3.877143598800591e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0007398307812884433], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0018520732509789732], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -7.659206092784872e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.010006830960698621], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.005060186262026125], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0016435175439759764], ["'market for corrugated board box' (kilogram, RER, None)", 0.0008303322974843852], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00181949401618542], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.85379676415959e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.005403688718777256], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0007851198612636768], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0005516263984969325], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -6.314205161566439e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0009682405116559995], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.002423868259982945], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00021790980716459963]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.010006830960698621], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.005060186262026125], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0016435175439759764], ["'market for corrugated board box' (kilogram, RER, None)", 0.0008303322974843852], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00181949401618542], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.0003693191862716783], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0011991878228194185], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.00011692972521419331], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.002104870674500697], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.005269278826436599], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00021790980716459963]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 2.2062815055389833e-06], ["'alubox production - CONSQ' (kilogram, GLO, None)", 1.2320551558728802e-06], ["'market for polysulfone' (kilogram, GLO, None)", 4.231378462349738e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00017715404964801845], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.7202568365239955e-08], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 3.76001094483108e-08], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -2.095967430262034e-06], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.4249610132476057e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.865000654634105e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.967203208637608e-07], ["'market for corrugated board box' (kilogram, RER, None)", 8.474064058166177e-08], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.4552848220774163e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.00012707952535413478], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 9.70274508524164e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.1337234920080076e-08], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.5676381986026424e-07]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.003517252466384169], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0017785803198210638], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0005449558282524257], ["'market for corrugated board box' (kilogram, RER, None)", 0.00027532070921551684], ["'autoclave - CONSQ' (unit, GLO, None)", 0.001364620512139065], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.6041536632474646e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0018993163318474513], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0002603292224294203], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00019388848660040697], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.3571724145239736e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0003403221579004145], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.000851953695479976], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -7.659206092784872e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.003517252466384169], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0017785803198210638], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0005449558282524257], ["'market for corrugated board box' (kilogram, RER, None)", 0.00027532070921551684], ["'autoclave - CONSQ' (unit, GLO, None)", 0.001364620512139065], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.6041536632474646e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00042149671000088474], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.124287857660812e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0007398307812884433], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0018520732509789732], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -7.659206092784872e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.010006830960698621], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.005060186262026125], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0016435175439759764], ["'market for corrugated board box' (kilogram, RER, None)", 0.0008303322974843852], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00181949401618542], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.85379676415959e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.005403688718777256], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0007851198612636768], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0005516263984969325], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.345268627709203e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0009682405116559995], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.002423868259982945], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00021790980716459963]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.010006830960698621], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.005060186262026125], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0016435175439759764], ["'market for corrugated board box' (kilogram, RER, None)", 0.0008303322974843852], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00181949401618542], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.0003693191862716783], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0011991878228194185], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00015454201162424448], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.002104870674500697], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.005269278826436599], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00021790980716459963]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.03049272720877801], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.001165474968186897], ["'market for polysulfone' (kilogram, GLO, None)", 4.904841909964629e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00272924102427813], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.002007297634397571], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.2365670834025218e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00047576668126590743], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.028968090848339106], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 6.736656759332428e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.9020825440950147e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -9.523248521989348e-06], ["'market for corrugated board box' (kilogram, RER, None)", 9.716857079202168e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.3985727296550403e-05]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.03049272720877801], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.001165474968186897], ["'market for polysulfone' (kilogram, GLO, None)", 4.904841909964629e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00272924102427813], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.2365670834025218e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00047576668126590743], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.028968090848339106], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 6.736656759332428e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0006506640308560747], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00032843275915364747], ["'market for corrugated board box' (kilogram, RER, None)", 9.716857079202168e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.3985727296550403e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0003744621018078424], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.000813820056220492], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -5.7900054609366824e-05], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.640739817933754e-06]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.03049272720877801], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.001165474968186897], ["'market for polysulfone' (kilogram, GLO, None)", 4.904841909964629e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00272924102427813], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.2365670834025218e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00047576668126590743], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.028968090848339106], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 6.736656759332428e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0006506640308560747], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00032843275915364747], ["'market for corrugated board box' (kilogram, RER, None)", 9.716857079202168e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.3985727296550403e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0003744621018078424], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.000813820056220492], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 7.652451843270921e-05], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.640739817933754e-06]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.018220258397829116], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0006964039303920935], ["'market for polysulfone' (kilogram, GLO, None)", 2.4524209549823146e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00181949401618542], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.0010036488171987854], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.3364114631223246e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0002842839149935723], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.017309245477937663], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.368328379666214e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -9.510412720475074e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.761624260994674e-06], ["'market for corrugated board box' (kilogram, RER, None)", 5.806094213023414e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.4332143749416316e-05]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.018220258397829116], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0006964039303920935], ["'market for polysulfone' (kilogram, GLO, None)", 2.4524209549823146e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00181949401618542], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.3364114631223246e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0002842839149935723], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.017309245477937663], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.368328379666214e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0006506640308560747], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00032843275915364747], ["'market for corrugated board box' (kilogram, RER, None)", 5.806094213023414e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.4332143749416316e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0003744621018078424], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.000813820056220492], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -5.7900054609366824e-05], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.640739817933754e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.05867514610319985], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.04857522255953673], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.010937123796594487], ["'market for corrugated board box' (kilogram, RER, None)", 0.005092068621364678], ["'autoclave - CONSQ' (unit, GLO, None)", 0.030221729446096055], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 8.820584758614293e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.03168457889572792], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.003461367295099731], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.05279006118834249], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.000578297916757895], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.011034994882025827], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.033846953585926466], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.007571224971604384]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.05867514610319985], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.04857522255953673], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.010937123796594487], ["'market for corrugated board box' (kilogram, RER, None)", 0.005092068621364678], ["'autoclave - CONSQ' (unit, GLO, None)", 0.030221729446096055], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 8.820584758614293e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.11476100258335324], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0012571693842562935], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.023989119413941037], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0735803338798882], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.007571224971604384]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.16693492271614604], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.13819992897220307], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.03298497586122507], ["'market for corrugated board box' (kilogram, RER, None)", 0.01535703234737849], ["'autoclave - CONSQ' (unit, GLO, None)", 0.04029563926146141], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.00026601763564448053], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.09014485826671886], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.010439044011849703], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.15019144169077725], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.00204739009859992], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.03139533774882958], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.09629696652448094], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.021540668230827467]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.16693492271614604], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.13819992897220307], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.03298497586122507], ["'market for corrugated board box' (kilogram, RER, None)", 0.01535703234737849], ["'autoclave - CONSQ' (unit, GLO, None)", 0.04029563926146141], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.0012509289415085633], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.3265031341103853], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.003791463145555407], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.06825073413891031], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.20934123159032242], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.021540668230827467]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.018220258397829116], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0006964039303920935], ["'market for polysulfone' (kilogram, GLO, None)", 2.4524209549823146e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00181949401618542], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.3364114631223246e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0002842839149935723], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.017309245477937663], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.368328379666214e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0006506640308560747], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00032843275915364747], ["'market for corrugated board box' (kilogram, RER, None)", 5.806094213023414e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.4332143749416316e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0003744621018078424], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.000813820056220492], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 7.652451843270921e-05], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.640739817933754e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.05867514610319985], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.04857522255953673], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.010937123796594487], ["'market for corrugated board box' (kilogram, RER, None)", 0.005092068621364678], ["'autoclave - CONSQ' (unit, GLO, None)", 0.030221729446096055], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 8.820584758614293e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.03168457889572792], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.003461367295099731], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.05279006118834249], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.006401953712917623], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.011034994882025827], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.033846953585926466], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.007571224971604384]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.05867514610319985], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.04857522255953673], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.010937123796594487], ["'market for corrugated board box' (kilogram, RER, None)", 0.005092068621364678], ["'autoclave - CONSQ' (unit, GLO, None)", 0.030221729446096055], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 8.820584758614293e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.11476100258335324], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.013917290680255701], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.023989119413941037], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0735803338798882], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.007571224971604384]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.16693492271614604], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.13819992897220307], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.03298497586122507], ["'market for corrugated board box' (kilogram, RER, None)", 0.01535703234737849], ["'autoclave - CONSQ' (unit, GLO, None)", 0.04029563926146141], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.00026601763564448053], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.09014485826671886], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.010439044011849703], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.15019144169077725], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.022665301505849826], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.03139533774882958], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.09629696652448094], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.021540668230827467]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.16693492271614604], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.13819992897220307], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.03298497586122507], ["'market for corrugated board box' (kilogram, RER, None)", 0.01535703234737849], ["'autoclave - CONSQ' (unit, GLO, None)", 0.04029563926146141], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.0012509289415085633], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.3265031341103853], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.04197278056638856], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.06825073413891031], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.20934123159032242], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.021540668230827467]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.13032565584744885], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.02856025811114962], ["'market for polysulfone' (kilogram, GLO, None)", 0.0014311051476188273], ["'autoclave - CONSQ' (unit, GLO, None)", 0.06044345889219211], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.062405983766129255], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.00140736120379972], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.043111645823239425], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.1238093730550764], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.0007369206162690872], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0006167529986519748], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0003783456218584972], ["'market for corrugated board box' (kilogram, RER, None)", 0.0017971369887965557], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0023710203808304294]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.13032565584744885], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.02856025811114962], ["'market for polysulfone' (kilogram, GLO, None)", 0.0014311051476188273], ["'autoclave - CONSQ' (unit, GLO, None)", 0.06044345889219211], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.00140736120379972], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.043111645823239425], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.1238093730550764], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.0007369206162690872], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.021097874715862962], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.013048183738329177], ["'market for corrugated board box' (kilogram, RER, None)", 0.0017971369887965557], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0023710203808304294], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.03006852054364752], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.016333159939913692], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0018774175922754415], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 0.00045464490567682323]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.13032565584744885], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.02856025811114962], ["'market for polysulfone' (kilogram, GLO, None)", 0.0014311051476188273], ["'autoclave - CONSQ' (unit, GLO, None)", 0.06044345889219211], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.00140736120379972], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.043111645823239425], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.1238093730550764], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.0007369206162690872], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.021097874715862962], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.013048183738329177], ["'market for corrugated board box' (kilogram, RER, None)", 0.0017971369887965557], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0023710203808304294], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.03006852054364752], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.016333159939913692], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.020783648319100637], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 0.00045464490567682323]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0778732288899202], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.017065553996890095], ["'market for polysulfone' (kilogram, GLO, None)", 0.0007155525738094137], ["'autoclave - CONSQ' (unit, GLO, None)", 0.04029563926146141], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.031202991883064628], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.000840937729732779], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.025760415638683427], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.07397956744542418], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.0003684603081345436], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0003083764993259874], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0001891728109292486], ["'market for corrugated board box' (kilogram, RER, None)", 0.0010738396773371857], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0014167510749505082]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0778732288899202], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.017065553996890095], ["'market for polysulfone' (kilogram, GLO, None)", 0.0007155525738094137], ["'autoclave - CONSQ' (unit, GLO, None)", 0.04029563926146141], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.000840937729732779], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.025760415638683427], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.07397956744542418], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.0003684603081345436], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.021097874715862962], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.013048183738329177], ["'market for corrugated board box' (kilogram, RER, None)", 0.0010738396773371857], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0014167510749505082], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.03006852054364752], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.016333159939913692], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0018774175922754415], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 0.00045464490567682323]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.002255350308311721], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.004441772806237658], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0009261542488092973], ["'market for corrugated board box' (kilogram, RER, None)", -9.542395253881106e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.001106686692725594], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.5998554509729677e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0012178891664883292], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0001548050699876318], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.921512688146157e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -2.9712864071981104e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.669764553239924e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0034524003173216104], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0001837103101131711]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.002255350308311721], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.004441772806237658], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0009261542488092973], ["'market for corrugated board box' (kilogram, RER, None)", -9.542395253881106e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.001106686692725594], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.5998554509729677e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.2872853669882952e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -6.459318276517631e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.2325575169785046e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0075052180808727505], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0001837103101131711]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.006416630454633346], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.012637156434647984], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0027931635509381237], ["'market for corrugated board box' (kilogram, RER, None)", -0.00028778652347785823], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0014755822569674588], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.0856706918376308e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.003464980445502007], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0004668724238384532], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.6847120605711605e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.0519460980089878e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.61308795344571e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00982232202795531], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0005226687696603586]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.006416630454633346], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.012637156434647984], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0027931635509381237], ["'market for corrugated board box' (kilogram, RER, None)", -0.00028778652347785823], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0014755822569674588], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 5.1052889259655955e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.662417522980783e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.9480483296462735e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.5067129372547175e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.02135287397538301], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0005226687696603586]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0778732288899202], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.017065553996890095], ["'market for polysulfone' (kilogram, GLO, None)", 0.0007155525738094137], ["'autoclave - CONSQ' (unit, GLO, None)", 0.04029563926146141], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.000840937729732779], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.025760415638683427], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.07397956744542418], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.0003684603081345436], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.021097874715862962], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.013048183738329177], ["'market for corrugated board box' (kilogram, RER, None)", 0.0010738396773371857], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0014167510749505082], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.03006852054364752], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.016333159939913692], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.020783648319100637], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 0.00045464490567682323]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.002255350308311721], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.004441772806237658], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0009261542488092973], ["'market for corrugated board box' (kilogram, RER, None)", -9.542395253881106e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.001106686692725594], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.5998554509729677e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0012178891664883292], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0001548050699876318], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.921512688146157e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 9.581866602559197e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.669764553239924e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0034524003173216104], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0001837103101131711]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.002255350308311721], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.004441772806237658], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0009261542488092973], ["'market for corrugated board box' (kilogram, RER, None)", -9.542395253881106e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.001106686692725594], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.5998554509729677e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.2872853669882952e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.0830144788172169e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.2325575169785046e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0075052180808727505], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0001837103101131711]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.006416630454633346], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.012637156434647984], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0027931635509381237], ["'market for corrugated board box' (kilogram, RER, None)", -0.00028778652347785823], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0014755822569674588], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.0856706918376308e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.003464980445502007], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0004668724238384532], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.6847120605711605e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.392337796782687e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.61308795344571e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00982232202795531], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0005226687696603586]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.006416630454633346], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.012637156434647984], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0027931635509381237], ["'market for corrugated board box' (kilogram, RER, None)", -0.00028778652347785823], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0014755822569674588], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 5.1052889259655955e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.662417522980783e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 6.282107031079051e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.5067129372547175e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.02135287397538301], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0005226687696603586]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0008274258581216459], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0018752795072104864], ["'market for polysulfone' (kilogram, GLO, None)", 0.00011308662079259678], ["'autoclave - CONSQ' (unit, GLO, None)", 0.002213373385451188], ["'cabinet washer - CONSQ' (unit, GLO, None)", 8.559651273248125e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.260377921681201e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00018725643970961882], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0007860545652155636], ["'plastic incineration - CONSQ' (kilogram, CH, None)", -7.254875744731232e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.1688680667692706e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.85913769653005e-05], ["'market for corrugated board box' (kilogram, RER, None)", -3.367784833164815e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -5.7531098478864144e-05]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0008274258581216459], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0018752795072104864], ["'market for polysulfone' (kilogram, GLO, None)", 0.00011308662079259678], ["'autoclave - CONSQ' (unit, GLO, None)", 0.002213373385451188], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.260377921681201e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00018725643970961882], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0007860545652155636], ["'plastic incineration - CONSQ' (kilogram, CH, None)", -7.254875744731232e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.0840057788113499e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0013309190017446375], ["'market for corrugated board box' (kilogram, RER, None)", -3.367784833164815e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -5.7531098478864144e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0003322238773375482], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0013830899015281333], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -9.646144678916427e-07], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -2.364164646650264e-06]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0008274258581216459], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0018752795072104864], ["'market for polysulfone' (kilogram, GLO, None)", 0.00011308662079259678], ["'autoclave - CONSQ' (unit, GLO, None)", 0.002213373385451188], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.260377921681201e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00018725643970961882], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0007860545652155636], ["'plastic incineration - CONSQ' (kilogram, CH, None)", -7.254875744731232e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.0840057788113499e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0013309190017446375], ["'market for corrugated board box' (kilogram, RER, None)", -3.367784833164815e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -5.7531098478864144e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0003322238773375482], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0013830899015281333], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.1107089279058106e-07], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -2.364164646650264e-06]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0004944101207084536], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.001120532019179074], ["'market for polysulfone' (kilogram, GLO, None)", 5.654331039629839e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0014755822569674588], ["'cabinet washer - CONSQ' (unit, GLO, None)", 4.279825636624063e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.33827912122086e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00011189096648543079], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0004696896146730309], ["'plastic incineration - CONSQ' (kilogram, CH, None)", -3.627437872365616e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.5844340333846353e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.929568848265025e-05], ["'market for corrugated board box' (kilogram, RER, None)", -2.0123457483385945e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.4376442426221206e-05]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0004944101207084536], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.001120532019179074], ["'market for polysulfone' (kilogram, GLO, None)", 5.654331039629839e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0014755822569674588], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.33827912122086e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00011189096648543079], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0004696896146730309], ["'plastic incineration - CONSQ' (kilogram, CH, None)", -3.627437872365616e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.0840057788113499e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0013309190017446375], ["'market for corrugated board box' (kilogram, RER, None)", -2.0123457483385945e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.4376442426221206e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0003322238773375482], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0013830899015281333], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -9.646144678916427e-07], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -2.364164646650264e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0017000890525980025], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.002503989405533837], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0008158651922520887], ["'market for corrugated board box' (kilogram, RER, None)", 0.005106828816268815], ["'autoclave - CONSQ' (unit, GLO, None)", 0.16825543378483399], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.892479440964108e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0009180480884029214], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -9.774151212120025e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.890777616975627e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0005851693666298558], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.011166114867022986], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.016528115476612544], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.006324265221133046]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0017000890525980025], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.002503989405533837], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0008158651922520887], ["'market for corrugated board box' (kilogram, RER, None)", 0.005106828816268815], ["'autoclave - CONSQ' (unit, GLO, None)", 0.16825543378483399], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.892479440964108e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -4.110386123860059e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0012721073187605561], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.024274162860836918], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.03593068581747251], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.006324265221133046]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0048368730792224856], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.007124026196025846], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.002460545768059087], ["'market for corrugated board box' (kilogram, RER, None)", 0.015401547220890875], ["'autoclave - CONSQ' (unit, GLO, None)", 0.22434057837977864], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.3802715780351274e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0026119114627801425], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0002947759829655848], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -5.3793954736489674e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.002071717591442624], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.03176838334229084], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.04702365247506063], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.017992979926380392]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0048368730792224856], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.007124026196025846], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.002460545768059087], ["'market for corrugated board box' (kilogram, RER, None)", 0.015401547220890875], ["'autoclave - CONSQ' (unit, GLO, None)", 0.22434057837977864], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.0001119305717608042], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.00011694337986193407], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0038365140582270808], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.06906170281918723], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.10222533147502556], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.017992979926380392]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0004944101207084536], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.001120532019179074], ["'market for polysulfone' (kilogram, GLO, None)", 5.654331039629839e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0014755822569674588], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.33827912122086e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00011189096648543079], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0004696896146730309], ["'plastic incineration - CONSQ' (kilogram, CH, None)", -3.627437872365616e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.0840057788113499e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0013309190017446375], ["'market for corrugated board box' (kilogram, RER, None)", -2.0123457483385945e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.4376442426221206e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0003322238773375482], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0013830899015281333], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.1107089279058106e-07], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -2.364164646650264e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0017000890525980025], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.002503989405533837], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0008158651922520887], ["'market for corrugated board box' (kilogram, RER, None)", 0.005106828816268815], ["'autoclave - CONSQ' (unit, GLO, None)", 0.16825543378483399], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.892479440964108e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0009180480884029214], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -9.774151212120025e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.890777616975627e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -2.317893248869346e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.011166114867022986], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.016528115476612544], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.006324265221133046]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0017000890525980025], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.002503989405533837], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0008158651922520887], ["'market for corrugated board box' (kilogram, RER, None)", 0.005106828816268815], ["'autoclave - CONSQ' (unit, GLO, None)", 0.16825543378483399], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.892479440964108e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -4.110386123860059e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -5.038898367107273e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.024274162860836918], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.03593068581747251], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.006324265221133046]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0048368730792224856], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.007124026196025846], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.002460545768059087], ["'market for corrugated board box' (kilogram, RER, None)", 0.015401547220890875], ["'autoclave - CONSQ' (unit, GLO, None)", 0.22434057837977864], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.3802715780351274e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0026119114627801425], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0002947759829655848], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -5.3793954736489674e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -8.20620574591048e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.03176838334229084], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.04702365247506063], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.017992979926380392]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0048368730792224856], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.007124026196025846], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.002460545768059087], ["'market for corrugated board box' (kilogram, RER, None)", 0.015401547220890875], ["'autoclave - CONSQ' (unit, GLO, None)", 0.22434057837977864], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.0001119305717608042], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.00011694337986193407], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.5196677307241627e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.06906170281918723], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.10222533147502556], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.017992979926380392]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0015002092875017413], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0029475230312975362], ["'market for polysulfone' (kilogram, GLO, None)", -2.4624839406446756e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.33651086756966797], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.069985841831298], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 6.877537770762638e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0010375830249309001], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0014251988231266542], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.1170202915333108e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0006240813793893255], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00018475341103514135], ["'market for corrugated board box' (kilogram, RER, None)", 0.001802346284702894], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0019805199012473667]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0015002092875017413], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0029475230312975362], ["'market for polysulfone' (kilogram, GLO, None)", -2.4624839406446756e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.33651086756966797], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 6.877537770762638e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0010375830249309001], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0014251988231266542], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.1170202915333108e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.02134856382317935], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0063716779425854915], ["'market for corrugated board box' (kilogram, RER, None)", 0.001802346284702894], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0019805199012473667], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -0.010429304020692188], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0012183876604387558], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0018997254382839182], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -0.0004015194186031602]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0015002092875017413], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0029475230312975362], ["'market for polysulfone' (kilogram, GLO, None)", -2.4624839406446756e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.33651086756966797], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 6.877537770762638e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0010375830249309001], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0014251988231266542], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.1170202915333108e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.02134856382317935], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0063716779425854915], ["'market for corrugated board box' (kilogram, RER, None)", 0.001802346284702894], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0019805199012473667], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -0.010429304020692188], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0012183876604387558], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -7.5249338383240476e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -0.0004015194186031602]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0008964170597779814], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0017612275509529892], ["'market for polysulfone' (kilogram, GLO, None)", -1.2312419703223378e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.22434057837977864], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.034992920915649], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.109521410339819e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0006199849129270385], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0008515962067890824], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 5.585101457666554e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00031204068969466274], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -9.237670551757067e-05], ["'market for corrugated board box' (kilogram, RER, None)", 0.0010769523775209166], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0011834161029313202]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0008964170597779814], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0017612275509529892], ["'market for polysulfone' (kilogram, GLO, None)", -1.2312419703223378e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.22434057837977864], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.109521410339819e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0006199849129270385], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0008515962067890824], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 5.585101457666554e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.02134856382317935], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0063716779425854915], ["'market for corrugated board box' (kilogram, RER, None)", 0.0010769523775209166], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0011834161029313202], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -0.010429304020692188], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0012183876604387558], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0018997254382839182], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -0.0004015194186031602]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00015443045132739234], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 7.391801978784976e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.2017600119227295e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.064265430836516e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0006835164091632984], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.864587460542977e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -8.339244371679187e-05], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -6.646838932200662e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.698552676877363e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.542409954457635e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.9432037467552094e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.371829091195071e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.238972508580597e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00015443045132739234], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 7.391801978784976e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.2017600119227295e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.064265430836516e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0006835164091632984], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.864587460542977e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.8909897123646443e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -3.3530651183861628e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.398269042740835e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0001167788932827854], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.238972508580597e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0004393655094103275], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00021030197179078383], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.640228472872845e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.209689394007594e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0009113552122177312], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.1655105042678095e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.00023725737508157685], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -2.0046021770399717e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.4747994939848278e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -5.460705939323969e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -8.373621979971138e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0001528323205977195], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.2060175307085602e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0004393655094103275], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00021030197179078383], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.640228472872845e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.209689394007594e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0009113552122177312], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 5.480729944421238e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.379998899967016e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.0112418406155496e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0001820352601736389], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0003322441752368176], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.2060175307085602e-05]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0008964170597779814], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0017612275509529892], ["'market for polysulfone' (kilogram, GLO, None)", -1.2312419703223378e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.22434057837977864], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.109521410339819e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0006199849129270385], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0008515962067890824], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 5.585101457666554e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.02134856382317935], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0063716779425854915], ["'market for corrugated board box' (kilogram, RER, None)", 0.0010769523775209166], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0011834161029313202], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -0.010429304020692188], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0012183876604387558], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -7.5249338383240476e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -0.0004015194186031602]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00015443045132739234], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 7.391801978784976e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.2017600119227295e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.064265430836516e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0006835164091632984], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.864587460542977e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -8.339244371679187e-05], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -6.646838932200662e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.698552676877363e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 9.480740327022601e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.9432037467552094e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.371829091195071e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.238972508580597e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00015443045132739234], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 7.391801978784976e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.2017600119227295e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.064265430836516e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0006835164091632984], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.864587460542977e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.8909897123646443e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.0610305058744784e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.398269042740835e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0001167788932827854], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.238972508580597e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0004393655094103275], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00021030197179078383], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.640228472872845e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.209689394007594e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0009113552122177312], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.1655105042678095e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.00023725737508157685], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -2.0046021770399717e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.4747994939848278e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.356535327286918e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -8.373621979971138e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0001528323205977195], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.2060175307085602e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0004393655094103275], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00021030197179078383], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.640228472872845e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.209689394007594e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0009113552122177312], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 5.480729944421238e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.379998899967016e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 6.21580616164244e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0001820352601736389], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0003322441752368176], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.2060175307085602e-05]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.001909903381614274], ["'alubox production - CONSQ' (kilogram, GLO, None)", 5.383540016672161e-05], ["'market for polysulfone' (kilogram, GLO, None)", 2.2951165960977628e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0013670328183265968], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.0001925900372458725], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.255637685124479e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", -0.00018516774676524117], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.00181440821253356], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 8.908884162993076e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.6449756033976153e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -6.004699988334661e-07], ["'market for corrugated board box' (kilogram, RER, None)", 3.7560977941833362e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.3274853473934867e-06]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.001909903381614274], ["'alubox production - CONSQ' (kilogram, GLO, None)", 5.383540016672161e-05], ["'market for polysulfone' (kilogram, GLO, None)", 2.2951165960977628e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0013670328183265968], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.255637685124479e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", -0.00018516774676524117], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.00181440821253356], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 8.908884162993076e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.627129380317419e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.0708691792563442e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.7560977941833362e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.3274853473934867e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 2.90697019629001e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.288039807617217e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -5.007362985559282e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 8.483230911981653e-07]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.001909903381614274], ["'alubox production - CONSQ' (kilogram, GLO, None)", 5.383540016672161e-05], ["'market for polysulfone' (kilogram, GLO, None)", 2.2951165960977628e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0013670328183265968], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.255637685124479e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", -0.00018516774676524117], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.00181440821253356], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 8.908884162993076e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.627129380317419e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.0708691792563442e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.7560977941833362e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.3274853473934867e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 2.90697019629001e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.288039807617217e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.077878747607377e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 8.483230911981653e-07]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.001141220753710808], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.216815915717201e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.1475582980488814e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0009113552122177312], ["'cabinet washer - CONSQ' (unit, GLO, None)", 9.629501862293625e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.335446697136949e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", -0.00011064291396130866], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0010841597160252676], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 4.454442081496538e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -8.224878016988077e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.002349994167331e-07], ["'market for corrugated board box' (kilogram, RER, None)", 2.2443736167567994e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -7.93209669603121e-07]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.001141220753710808], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.216815915717201e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.1475582980488814e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0009113552122177312], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.335446697136949e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", -0.00011064291396130866], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0010841597160252676], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 4.454442081496538e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.627129380317419e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.0708691792563442e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.2443736167567994e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -7.93209669603121e-07], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 2.90697019629001e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.288039807617217e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -5.007362985559282e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 8.483230911981653e-07]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.1390439608595256e-08], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 1.5366018306686846e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.0761387717593778e-09], ["'market for corrugated board box' (kilogram, RER, None)", 1.2242259622376303e-09], ["'autoclave - CONSQ' (unit, GLO, None)", -1.944112734983769e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.943037542027535e-11], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -6.150837388641439e-09], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.2857762786126436e-09], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 6.5080690789901095e-09], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -5.618410544827927e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.0720967482449381e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.6761919027072856e-08], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -9.475535564947016e-10]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.1390439608595256e-08], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 1.5366018306686846e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.0761387717593778e-09], ["'market for corrugated board box' (kilogram, RER, None)", 1.2242259622376303e-09], ["'autoclave - CONSQ' (unit, GLO, None)", -1.944112734983769e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.943037542027535e-11], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.4147976258674152e-08], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.2213935967017234e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.330645115099883e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.81780848394381e-08], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -9.475535564947016e-10]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 3.2406602830087913e-08], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 4.371740419648934e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 9.27724372689787e-09], ["'market for corrugated board box' (kilogram, RER, None)", 3.6921100441779405e-09], ["'autoclave - CONSQ' (unit, GLO, None)", -2.592150313311692e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.0939319576485633e-10], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -1.7499565528247473e-08], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -3.877737904564959e-09], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.8515914844450735e-08], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.9891266743341663e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.050190767681859e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -7.613954426174581e-08], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.6958565975708696e-09]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 3.2406602830087913e-08], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 4.371740419648934e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 9.27724372689787e-09], ["'market for corrugated board box' (kilogram, RER, None)", 3.6921100441779405e-09], ["'autoclave - CONSQ' (unit, GLO, None)", -2.592150313311692e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 9.846565552040756e-10], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 4.02519887922842e-08], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -3.6835679154336406e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.630849485470951e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.6552074840724738e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.6958565975708696e-09]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.001141220753710808], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.216815915717201e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.1475582980488814e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0009113552122177312], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.335446697136949e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", -0.00011064291396130866], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0010841597160252676], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 4.454442081496538e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.627129380317419e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.0708691792563442e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.2443736167567994e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -7.93209669603121e-07], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 2.90697019629001e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.288039807617217e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.077878747607377e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 8.483230911981653e-07]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.1390439608595256e-08], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 1.5366018306686846e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.0761387717593778e-09], ["'market for corrugated board box' (kilogram, RER, None)", 1.2242259622376303e-09], ["'autoclave - CONSQ' (unit, GLO, None)", -1.944112734983769e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.943037542027535e-11], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -6.150837388641439e-09], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.2857762786126436e-09], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 6.5080690789901095e-09], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 7.893176660960214e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.0720967482449381e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.6761919027072856e-08], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -9.475535564947016e-10]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.1390439608595256e-08], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 1.5366018306686846e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.0761387717593778e-09], ["'market for corrugated board box' (kilogram, RER, None)", 1.2242259622376303e-09], ["'autoclave - CONSQ' (unit, GLO, None)", -1.944112734983769e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.943037542027535e-11], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.4147976258674152e-08], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.7159079697739596e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.330645115099883e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.81780848394381e-08], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -9.475535564947016e-10]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 3.2406602830087913e-08], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 4.371740419648934e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 9.27724372689787e-09], ["'market for corrugated board box' (kilogram, RER, None)", 3.6921100441779405e-09], ["'autoclave - CONSQ' (unit, GLO, None)", -2.592150313311692e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.0939319576485633e-10], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -1.7499565528247473e-08], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -3.877737904564959e-09], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.8515914844450735e-08], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.794478637023258e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.050190767681859e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -7.613954426174581e-08], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.6958565975708696e-09]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 3.2406602830087913e-08], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 4.371740419648934e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 9.27724372689787e-09], ["'market for corrugated board box' (kilogram, RER, None)", 3.6921100441779405e-09], ["'autoclave - CONSQ' (unit, GLO, None)", -2.592150313311692e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 9.846565552040756e-10], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 4.02519887922842e-08], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.1749604389319584e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.630849485470951e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.6552074840724738e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.6958565975708696e-09]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 2.9426490598608053e-08], ["'alubox production - CONSQ' (kilogram, GLO, None)", 6.159776879286204e-09], ["'market for polysulfone' (kilogram, GLO, None)", 8.608425911461889e-10], ["'autoclave - CONSQ' (unit, GLO, None)", -3.888225469967538e-07], ["'cabinet washer - CONSQ' (unit, GLO, None)", 3.865988162882121e-08], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.510652856842942e-10], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 2.8252359290012935e-09], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -2.7955166068677648e-08], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.2674656970296917e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.992018042546741e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.9914818982807066e-10], ["'market for corrugated board box' (kilogram, RER, None)", 4.320644364750669e-10], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.967378202078723e-10]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 2.9426490598608053e-08], ["'alubox production - CONSQ' (kilogram, GLO, None)", 6.159776879286204e-09], ["'market for polysulfone' (kilogram, GLO, None)", 8.608425911461889e-10], ["'autoclave - CONSQ' (unit, GLO, None)", -3.888225469967538e-07], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.510652856842942e-10], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 2.8252359290012935e-09], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -2.7955166068677648e-08], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.2674656970296917e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.04974837954826e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.0316864581890436e-08], ["'market for corrugated board box' (kilogram, RER, None)", 4.320644364750669e-10], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.967378202078723e-10], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 1.7828518486191989e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.593809806940272e-09], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.8239911457093788e-09], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.304408595474606e-08]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 2.9426490598608053e-08], ["'alubox production - CONSQ' (kilogram, GLO, None)", 6.159776879286204e-09], ["'market for polysulfone' (kilogram, GLO, None)", 8.608425911461889e-10], ["'autoclave - CONSQ' (unit, GLO, None)", -3.888225469967538e-07], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.510652856842942e-10], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 2.8252359290012935e-09], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -2.7955166068677648e-08], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.2674656970296917e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.04974837954826e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.0316864581890436e-08], ["'market for corrugated board box' (kilogram, RER, None)", 4.320644364750669e-10], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.967378202078723e-10], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 1.7828518486191989e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.593809806940272e-09], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.562483504229626e-09], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.304408595474606e-08]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 1.7583152165332816e-08], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.6806391781598138e-09], ["'market for polysulfone' (kilogram, GLO, None)", 4.3042129557309444e-10], ["'autoclave - CONSQ' (unit, GLO, None)", -2.592150313311692e-07], ["'cabinet washer - CONSQ' (unit, GLO, None)", 1.9329940814410604e-08], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.487825403451534e-10], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.6881575829142531e-09], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -1.6703994557066173e-08], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.6337328485148458e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.9960090212733706e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.4957409491403533e-10], ["'market for corrugated board box' (kilogram, RER, None)", 2.5817060020780766e-10], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.773091573387197e-10]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 1.7583152165332816e-08], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.6806391781598138e-09], ["'market for polysulfone' (kilogram, GLO, None)", 4.3042129557309444e-10], ["'autoclave - CONSQ' (unit, GLO, None)", -2.592150313311692e-07], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.487825403451534e-10], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.6881575829142531e-09], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -1.6703994557066173e-08], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.6337328485148458e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.04974837954826e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.0316864581890436e-08], ["'market for corrugated board box' (kilogram, RER, None)", 2.5817060020780766e-10], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.773091573387197e-10], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 1.7828518486191989e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.593809806940272e-09], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.8239911457093788e-09], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.304408595474606e-08]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00014168997134467824], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00011137929805245783], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.4109122727607444e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.6328052074237104e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002012539542205681], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 4.449414831409708e-07], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -7.651258452612626e-05], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -8.30383797456183e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.996131450780361e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -4.4095347002889386e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -8.414208566166241e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.0787150428346334e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -8.888003634907142e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00014168997134467824], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00011137929805245783], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.4109122727607444e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.6328052074237104e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002012539542205681], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 4.449414831409708e-07], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 4.339416197348611e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -9.585945000628128e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.829175783274234e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00011040684875343242], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -8.888003634907142e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0004031179466426057], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00031688194657178144], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 7.27100511976521e-05], ["'market for corrugated board box' (kilogram, RER, None)", 4.9243331643582276e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002683386056274241], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.3418870129864744e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.00021768369118700708], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -2.5043320368352365e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.679134550107507e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.5611395827635214e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.3939016070969654e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.000144493019504886], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.5286996259120968e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0004031179466426057], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00031688194657178144], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 7.27100511976521e-05], ["'market for corrugated board box' (kilogram, RER, None)", 4.9243331643582276e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002683386056274241], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.310127885741498e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.2345944674146753e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -2.890999227339854e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.204133921023868e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0003141152598162838], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.5286996259120968e-05]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 1.7583152165332816e-08], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.6806391781598138e-09], ["'market for polysulfone' (kilogram, GLO, None)", 4.3042129557309444e-10], ["'autoclave - CONSQ' (unit, GLO, None)", -2.592150313311692e-07], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.487825403451534e-10], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.6881575829142531e-09], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -1.6703994557066173e-08], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.6337328485148458e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.04974837954826e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.0316864581890436e-08], ["'market for corrugated board box' (kilogram, RER, None)", 2.5817060020780766e-10], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.773091573387197e-10], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 1.7828518486191989e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.593809806940272e-09], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.562483504229626e-09], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.304408595474606e-08]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00014168997134467824], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00011137929805245783], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.4109122727607444e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.6328052074237104e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002012539542205681], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 4.449414831409708e-07], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -7.651258452612626e-05], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -8.30383797456183e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.996131450780361e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.3431747788794499e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -8.414208566166241e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.0787150428346334e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -8.888003634907142e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00014168997134467824], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00011137929805245783], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.4109122727607444e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.6328052074237104e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002012539542205681], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 4.449414831409708e-07], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 4.339416197348611e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.093858214955326e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.829175783274234e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00011040684875343242], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -8.888003634907142e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0004031179466426057], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00031688194657178144], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 7.27100511976521e-05], ["'market for corrugated board box' (kilogram, RER, None)", 4.9243331643582276e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002683386056274241], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.3418870129864744e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.00021768369118700708], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -2.5043320368352365e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.679134550107507e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.295711782021299e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.3939016070969654e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.000144493019504886], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.5286996259120968e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0004031179466426057], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00031688194657178144], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 7.27100511976521e-05], ["'market for corrugated board box' (kilogram, RER, None)", 4.9243331643582276e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002683386056274241], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.310127885741498e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.2345944674146753e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.5362429225965368e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.204133921023868e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0003141152598162838], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.5286996259120968e-05]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0003070959975220654], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.269211273872963e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.8956198489533308e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004025079084411362], ["'cabinet washer - CONSQ' (unit, GLO, None)", 6.212970614681401e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.411296257488632e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.9268351301255548e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0002917411976459621], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.50440480181107e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -4.702755569845327e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.677053316616167e-07], ["'market for corrugated board box' (kilogram, RER, None)", 5.762637646808395e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.7833854947245283e-06]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0003070959975220654], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.269211273872963e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.8956198489533308e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004025079084411362], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.411296257488632e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.9268351301255548e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0002917411976459621], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.50440480181107e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.6087177208506912e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.9578721277024118e-05], ["'market for corrugated board box' (kilogram, RER, None)", 5.762637646808395e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.7833854947245283e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 4.867140766356924e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.600381277970284e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.4315351620983423e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 5.476801820179796e-07]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0003070959975220654], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.269211273872963e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.8956198489533308e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004025079084411362], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.411296257488632e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.9268351301255548e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0002917411976459621], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.50440480181107e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.6087177208506912e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.9578721277024118e-05], ["'market for corrugated board box' (kilogram, RER, None)", 5.762637646808395e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.7833854947245283e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 4.867140766356924e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.600381277970284e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 7.607009162867332e-07], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 5.476801820179796e-07]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00018349845815629013], ["'alubox production - CONSQ' (kilogram, GLO, None)", 1.9534452841566142e-05], ["'market for polysulfone' (kilogram, GLO, None)", 9.478099244766654e-07], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002683386056274241], ["'cabinet washer - CONSQ' (unit, GLO, None)", 3.1064853073407005e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 8.432890345055666e-07], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.1513379475875757e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.00017432353524847563], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.752202400905535e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.3513777849226634e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.8385266583080837e-07], ["'market for corrugated board box' (kilogram, RER, None)", 3.443337369291871e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.6631507782617617e-06]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00018349845815629013], ["'alubox production - CONSQ' (kilogram, GLO, None)", 1.9534452841566142e-05], ["'market for polysulfone' (kilogram, GLO, None)", 9.478099244766654e-07], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002683386056274241], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 8.432890345055666e-07], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.1513379475875757e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.00017432353524847563], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.752202400905535e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.6087177208506912e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.9578721277024118e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.443337369291871e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.6631507782617617e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 4.867140766356924e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.600381277970284e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.4315351620983423e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 5.476801820179796e-07]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0002935749893174448], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0001387753076477897], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.3243948373555644e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.1226053340561828e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00037007040312632286], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.3446821182988132e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0001585304942314202], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.7558362767586567e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.3645575151839235e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.4600373811464844e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.7860216268534373e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00011080807991803284], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.326310774277151e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0002935749893174448], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0001387753076477897], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.3243948373555644e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.1226053340561828e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00037007040312632286], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.3446821182988132e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.966429380834616e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -3.1739943068401833e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.0565687805864964e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00024088713024821013], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.326310774277151e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0008352415189031528], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.000394825523166951], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00013041825435768927], ["'market for corrugated board box' (kilogram, RER, None)", 3.385635133844707e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004934272041684305], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.07126353316432e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0004510304202077025], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -5.2953791400972424e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.882262226297923e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -5.169076337856718e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -7.926427776879018e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00031525679070111627], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.7734475552932816e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0008352415189031528], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.000394825523166951], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00013041825435768927], ["'market for corrugated board box' (kilogram, RER, None)", 3.385635133844707e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004934272041684305], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.3252111970843614e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.439700491952006e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -9.572363588623551e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00017231364707685353], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0006853408494005509], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.7734475552932816e-05]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00018349845815629013], ["'alubox production - CONSQ' (kilogram, GLO, None)", 1.9534452841566142e-05], ["'market for polysulfone' (kilogram, GLO, None)", 9.478099244766654e-07], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002683386056274241], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 8.432890345055666e-07], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.1513379475875757e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.00017432353524847563], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.752202400905535e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.6087177208506912e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.9578721277024118e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.443337369291871e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.6631507782617617e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 4.867140766356924e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.600381277970284e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 7.607009162867332e-07], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 5.476801820179796e-07]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0002935749893174448], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0001387753076477897], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.3243948373555644e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.1226053340561828e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00037007040312632286], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.3446821182988132e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0001585304942314202], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.7558362767586567e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.3645575151839235e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.6487555901412544e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.7860216268534373e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00011080807991803284], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.326310774277151e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0002935749893174448], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0001387753076477897], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.3243948373555644e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.1226053340561828e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00037007040312632286], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.3446821182988132e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.966429380834616e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.5842512829157703e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.0565687805864964e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00024088713024821013], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.326310774277151e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0008352415189031528], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.000394825523166951], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00013041825435768927], ["'market for corrugated board box' (kilogram, RER, None)", 3.385635133844707e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004934272041684305], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.07126353316432e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0004510304202077025], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -5.2953791400972424e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.882262226297923e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.837209113930959e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -7.926427776879018e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00031525679070111627], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.7734475552932816e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0008352415189031528], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.000394825523166951], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00013041825435768927], ["'market for corrugated board box' (kilogram, RER, None)", 3.385635133844707e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004934272041684305], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.3252111970843614e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.439700491952006e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.0809646507279553e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00017231364707685353], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0006853408494005509], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.7734475552932816e-05]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00040270113347142325], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.55134149702434e-05], ["'market for polysulfone' (kilogram, GLO, None)", 3.841999494362337e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0007401408062526457], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.00017398150328724294], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 3.092243820393865e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.7908722229360266e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0003825660767978521], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.012315978333832e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.5571255003207255e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.238627039124905e-06], ["'market for corrugated board box' (kilogram, RER, None)", 3.961996036714828e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.15350209367736e-06]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00040270113347142325], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.55134149702434e-05], ["'market for polysulfone' (kilogram, GLO, None)", 3.841999494362337e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0007401408062526457], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 3.092243820393865e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.7908722229360266e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0003825660767978521], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.012315978333832e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.3266119166742874e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.2717114342105416e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.961996036714828e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.15350209367736e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0007846475745748834], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.457916526816494e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -4.739944214413862e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.816899922592571e-06]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00040270113347142325], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.55134149702434e-05], ["'market for polysulfone' (kilogram, GLO, None)", 3.841999494362337e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0007401408062526457], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 3.092243820393865e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.7908722229360266e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0003825660767978521], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.012315978333832e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.3266119166742874e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.2717114342105416e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.961996036714828e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.15350209367736e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0007846475745748834], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.457916526816494e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.352609201235566e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.816899922592571e-06]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00024062520412525756], ["'alubox production - CONSQ' (kilogram, GLO, None)", 2.1220259930075914e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.9209997471811684e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004934272041684305], ["'cabinet washer - CONSQ' (unit, GLO, None)", 8.699075164362147e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.8477022750673254e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.0700963031603065e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0002285939439189947], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.006157989166916e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -7.785627501603627e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -6.193135195624525e-07], ["'market for corrugated board box' (kilogram, RER, None)", 2.3674035825872675e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.481833814505466e-06]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00024062520412525756], ["'alubox production - CONSQ' (kilogram, GLO, None)", 2.1220259930075914e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.9209997471811684e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004934272041684305], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.8477022750673254e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.0700963031603065e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0002285939439189947], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.006157989166916e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.3266119166742874e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.2717114342105416e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.3674035825872675e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.481833814505466e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0007846475745748834], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.457916526816494e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -4.739944214413862e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.816899922592571e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.000317642348754344], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00014298353781804255], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.8239456800970866e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.1597092085675906e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0003776406112181805], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.395849469652867e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0001715268683273458], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.910963649336365e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.379367762451718e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.4920981622522928e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.8471995327673646e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0001171029226109728], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.3605872382790101e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.000317642348754344], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00014298353781804255], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.8239456800970866e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.1597092085675906e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0003776406112181805], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.395849469652867e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.998625570547213e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -3.2436916570702013e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.189564228808637e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0002545715708845599], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.3605872382790101e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0009037148513855984], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0004067982343555577], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00014548407311930413], ["'market for corrugated board box' (kilogram, RER, None)", 3.497535707747824e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000503520814957574], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.2255777674457005e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0004880060197482232], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -5.763223587600363e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.924398422749959e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -5.282583448789114e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -8.100483228600373e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0003331660614583805], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.870966509222013e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0009037148513855984], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0004067982343555577], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00014548407311930413], ["'market for corrugated board box' (kilogram, RER, None)", 3.497535707747824e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000503520814957574], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.397776364157455e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.531300919021649e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -9.782561942202061e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00017609746123929397], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0007242740467018087], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.870966509222013e-05]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00024062520412525756], ["'alubox production - CONSQ' (kilogram, GLO, None)", 2.1220259930075914e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.9209997471811684e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004934272041684305], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.8477022750673254e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.0700963031603065e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0002285939439189947], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.006157989166916e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.3266119166742874e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.2717114342105416e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.3674035825872675e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.481833814505466e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0007846475745748834], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.457916526816494e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.352609201235566e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.816899922592571e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.000317642348754344], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00014298353781804255], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.8239456800970866e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.1597092085675906e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0003776406112181805], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.395849469652867e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0001715268683273458], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.910963649336365e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.379367762451718e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.6658765754626403e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.8471995327673646e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0001171029226109728], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.3605872382790101e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.000317642348754344], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00014298353781804255], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.8239456800970866e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.1597092085675906e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0003776406112181805], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.395849469652867e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.998625570547213e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.6214708162231313e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.189564228808637e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0002545715708845599], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.3605872382790101e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0009037148513855984], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0004067982343555577], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00014548407311930413], ["'market for corrugated board box' (kilogram, RER, None)", 3.497535707747824e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000503520814957574], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.2255777674457005e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0004880060197482232], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -5.763223587600363e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.924398422749959e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.8978237812322e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -8.100483228600373e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0003331660614583805], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.870966509222013e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0009037148513855984], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0004067982343555577], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00014548407311930413], ["'market for corrugated board box' (kilogram, RER, None)", 3.497535707747824e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000503520814957574], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.397776364157455e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.531300919021649e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.0921895891170739e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00017609746123929397], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0007242740467018087], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.870966509222013e-05]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0004126359538879128], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.816335531480803e-05], ["'market for polysulfone' (kilogram, GLO, None)", 3.88155116343156e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000755281222436361], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.00017789009719927412], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 3.4545200183282885e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.8623214273884847e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0003920041561935171], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.0352750182351766e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.5913182274828571e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.3089916043468713e-06], ["'market for corrugated board box' (kilogram, RER, None)", 4.0929462462865255e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.2608429731730944e-06]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0004126359538879128], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.816335531480803e-05], ["'market for polysulfone' (kilogram, GLO, None)", 3.88155116343156e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000755281222436361], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 3.4545200183282885e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.8623214273884847e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0003920041561935171], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.0352750182351766e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.4435783319875614e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.514381025885438e-05], ["'market for corrugated board box' (kilogram, RER, None)", 4.0929462462865255e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.2608429731730944e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0012260816744973165], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 7.203930192233402e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -4.844028065878497e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.7009143857956334e-06]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0004126359538879128], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.816335531480803e-05], ["'market for polysulfone' (kilogram, GLO, None)", 3.88155116343156e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000755281222436361], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 3.4545200183282885e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.8623214273884847e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0003920041561935171], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.0352750182351766e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.4435783319875614e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.514381025885438e-05], ["'market for corrugated board box' (kilogram, RER, None)", 4.0929462462865255e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.2608429731730944e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0012260816744973165], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 7.203930192233402e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.4081916927300264e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.7009143857956334e-06]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00024656153752978025], ["'alubox production - CONSQ' (kilogram, GLO, None)", 2.2803673492471236e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.94077558171578e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000503520814957574], ["'cabinet washer - CONSQ' (unit, GLO, None)", 8.894504859963706e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.0641724481861174e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.1127892036191524e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.00023423346065329126], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.0176375091175883e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -7.956591137414286e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -6.544958021734357e-07], ["'market for corrugated board box' (kilogram, RER, None)", 2.4456499999001035e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.5459729959487106e-06]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00024656153752978025], ["'alubox production - CONSQ' (kilogram, GLO, None)", 2.2803673492471236e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.94077558171578e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000503520814957574], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.0641724481861174e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.1127892036191524e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.00023423346065329126], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.0176375091175883e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.4435783319875614e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.514381025885438e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.4456499999001035e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.5459729959487106e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0012260816744973165], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 7.203930192233402e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -4.844028065878497e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.7009143857956334e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0011196636272355163], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00032141079905200864], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00032401647559544063], ["'market for corrugated board box' (kilogram, RER, None)", 3.806130102374293e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0005504119066706546], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 4.711286406182188e-07], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0006046183587071789], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -7.04324891423178e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 4.1055814094313594e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.2988225258344675e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.4783938364494434e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00014662113252027055], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0002098095686832082]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0011196636272355163], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00032141079905200864], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00032401647559544063], ["'market for corrugated board box' (kilogram, RER, None)", 3.806130102374293e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0005504119066706546], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 4.711286406182188e-07], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.925176977024695e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -2.823527230074929e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.387812711558447e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00031874159242427835], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0002098095686832082]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0031855218690362576], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.000914436357866278], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0009771925256512753], ["'market for corrugated board box' (kilogram, RER, None)", 0.00011478805068582941], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0007338825422275394], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.420864154604482e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0017201818092795792], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.00021241543914212013], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00011680668235283588], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -4.598315681543951e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -7.051205043754697e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0004171474473837644], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0005969229982741224]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0031855218690362576], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.000914436357866278], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0009771925256512753], ["'market for corrugated board box' (kilogram, RER, None)", 0.00011478805068582941], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0007338825422275394], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.6815122562860895e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0002539275703322519], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -8.515399410266577e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00015328706594920652], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0009068422769877813], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0005969229982741224]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00024656153752978025], ["'alubox production - CONSQ' (kilogram, GLO, None)", 2.2803673492471236e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.94077558171578e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000503520814957574], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.0641724481861174e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.1127892036191524e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.00023423346065329126], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.0176375091175883e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.4435783319875614e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.514381025885438e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.4456499999001035e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.5459729959487106e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0012260816744973165], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 7.203930192233402e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.4081916927300264e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.7009143857956334e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0011196636272355163], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00032141079905200864], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00032401647559544063], ["'market for corrugated board box' (kilogram, RER, None)", 3.806130102374293e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0005504119066706546], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 4.711286406182188e-07], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0006046183587071789], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -7.04324891423178e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 4.1055814094313594e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 4.348760124618535e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.4783938364494434e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00014662113252027055], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0002098095686832082]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0011196636272355163], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00032141079905200864], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00032401647559544063], ["'market for corrugated board box' (kilogram, RER, None)", 3.806130102374293e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0005504119066706546], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 4.711286406182188e-07], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.925176977024695e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 9.45382635786638e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.387812711558447e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00031874159242427835], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0002098095686832082]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0031855218690362576], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.000914436357866278], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0009771925256512753], ["'market for corrugated board box' (kilogram, RER, None)", 0.00011478805068582941], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0007338825422275394], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.420864154604482e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0017201818092795792], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.00021241543914212013], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00011680668235283588], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.5396231185210454e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -7.051205043754697e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0004171474473837644], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0005969229982741224]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0031855218690362576], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.000914436357866278], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0009771925256512753], ["'market for corrugated board box' (kilogram, RER, None)", 0.00011478805068582941], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0007338825422275394], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.6815122562860895e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0002539275703322519], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.8511539231871207e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00015328706594920652], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0009068422769877813], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0005969229982741224]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0008862513405582456], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0006035256209839753], ["'market for polysulfone' (kilogram, GLO, None)", 3.468695127676702e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0011008238133413091], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.00018270602189388239], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.4786413443271393e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.257875181621341e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0008419387735303332], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.1081310681762825e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.3851903392909875e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.6389499699034864e-06], ["'market for corrugated board box' (kilogram, RER, None)", 1.3432924219539876e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -6.57043959606068e-05]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0008862513405582456], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0006035256209839753], ["'market for polysulfone' (kilogram, GLO, None)", 3.468695127676702e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0011008238133413091], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.4786413443271393e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.257875181621341e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0008419387735303332], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.1081310681762825e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -4.738456448507028e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.6523239888918186e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.3432924219539876e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -6.57043959606068e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.010838951150681493], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00048387611016301375], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -4.2165676005125665e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 3.718321589217504e-06]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0008862513405582456], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0006035256209839753], ["'market for polysulfone' (kilogram, GLO, None)", 3.468695127676702e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0011008238133413091], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.4786413443271393e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.257875181621341e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0008419387735303332], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.1081310681762825e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -4.738456448507028e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.6523239888918186e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.3432924219539876e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -6.57043959606068e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.010838951150681493], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00048387611016301375], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.4118049755940637e-05], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 3.718321589217504e-06]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0005295599937596006], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0003606234591202047], ["'market for polysulfone' (kilogram, GLO, None)", 1.734347563838351e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0007338825422275394], ["'cabinet washer - CONSQ' (unit, GLO, None)", 9.135301094694119e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.4810576128520979e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 7.516156454106661e-06], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0005030819940716205], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 5.540655340881412e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.925951696454937e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -8.194749849517432e-07], ["'market for corrugated board box' (kilogram, RER, None)", 8.026548393100001e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.9260216554343014e-05]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0005295599937596006], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0003606234591202047], ["'market for polysulfone' (kilogram, GLO, None)", 1.734347563838351e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0007338825422275394], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.4810576128520979e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 7.516156454106661e-06], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0005030819940716205], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 5.540655340881412e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -4.738456448507028e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.6523239888918186e-05], ["'market for corrugated board box' (kilogram, RER, None)", 8.026548393100001e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.9260216554343014e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.010838951150681493], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00048387611016301375], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -4.2165676005125665e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 3.718321589217504e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 5.757589568054192e-10], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 2.2601734744686658e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 8.518376808030966e-11], ["'market for corrugated board box' (kilogram, RER, None)", 8.138664770554284e-11], ["'autoclave - CONSQ' (unit, GLO, None)", 2.5211332673493153e-09], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.2814611037247904e-12], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -3.109098366749264e-10], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -3.2772614457535437e-11], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.441007470333537e-10], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -6.111343873626605e-12], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.1661575532875856e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.717017418144127e-10], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -8.071351980028816e-11]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 5.757589568054192e-10], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 2.2601734744686658e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 8.518376808030966e-11], ["'market for corrugated board box' (kilogram, RER, None)", 8.138664770554284e-11], ["'autoclave - CONSQ' (unit, GLO, None)", 2.5211332673493153e-09], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.2814611037247904e-12], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.30653797898595e-10], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.3285530160057834e-11], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.535125126958779e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.0254385691260812e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -8.071351980028816e-11]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.6380747785168264e-09], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 6.430352702009443e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.5690342233961884e-10], ["'market for corrugated board box' (kilogram, RER, None)", 2.454517946232539e-10], ["'autoclave - CONSQ' (unit, GLO, None)", 3.3615110231324204e-09], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.864723964591084e-12], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -8.845603803990862e-10], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -9.883804159989819e-11], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 6.944838155033444e-10], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -2.1636434393798238e-11], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.31780038370903e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.3420246736748824e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.2963564790122821e-10]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.6380747785168264e-09], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 6.430352702009443e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.5690342233961884e-10], ["'market for corrugated board box' (kilogram, RER, None)", 2.454517946232539e-10], ["'autoclave - CONSQ' (unit, GLO, None)", 3.3615110231324204e-09], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.817358855376704e-11], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.5097474250072704e-09], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -4.006747109962636e-11], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -7.212609519480051e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.9174449429855987e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.2963564790122821e-10]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0005295599937596006], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0003606234591202047], ["'market for polysulfone' (kilogram, GLO, None)", 1.734347563838351e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0007338825422275394], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.4810576128520979e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 7.516156454106661e-06], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0005030819940716205], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 5.540655340881412e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -4.738456448507028e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.6523239888918186e-05], ["'market for corrugated board box' (kilogram, RER, None)", 8.026548393100001e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.9260216554343014e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.010838951150681493], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00048387611016301375], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.4118049755940637e-05], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 3.718321589217504e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 5.757589568054192e-10], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 2.2601734744686658e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 8.518376808030966e-11], ["'market for corrugated board box' (kilogram, RER, None)", 8.138664770554284e-11], ["'autoclave - CONSQ' (unit, GLO, None)", 2.5211332673493153e-09], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.2814611037247904e-12], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -3.109098366749264e-10], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -3.2772614457535437e-11], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.441007470333537e-10], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.960815268128032e-11], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.1661575532875856e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.717017418144127e-10], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -8.071351980028816e-11]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 5.757589568054192e-10], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 2.2601734744686658e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 8.518376808030966e-11], ["'market for corrugated board box' (kilogram, RER, None)", 8.138664770554284e-11], ["'autoclave - CONSQ' (unit, GLO, None)", 2.5211332673493153e-09], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.2814611037247904e-12], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.30653797898595e-10], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 6.436554930713113e-11], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.535125126958779e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.0254385691260812e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -8.071351980028816e-11]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.6380747785168264e-09], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 6.430352702009443e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.5690342233961884e-10], ["'market for corrugated board box' (kilogram, RER, None)", 2.454517946232539e-10], ["'autoclave - CONSQ' (unit, GLO, None)", 3.3615110231324204e-09], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.864723964591084e-12], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -8.845603803990862e-10], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -9.883804159989819e-11], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 6.944838155033444e-10], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.0482389246244923e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.31780038370903e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.3420246736748824e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.2963564790122821e-10]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.6380747785168264e-09], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 6.430352702009443e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.5690342233961884e-10], ["'market for corrugated board box' (kilogram, RER, None)", 2.454517946232539e-10], ["'autoclave - CONSQ' (unit, GLO, None)", 3.3615110231324204e-09], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.817358855376704e-11], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.5097474250072704e-09], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.9411831937490595e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -7.212609519480051e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.9174449429855987e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.2963564790122821e-10]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 6.880138454036532e-10], ["'alubox production - CONSQ' (kilogram, GLO, None)", 1.240919621881071e-10], ["'market for polysulfone' (kilogram, GLO, None)", 7.37809084738171e-12], ["'autoclave - CONSQ' (unit, GLO, None)", 5.0422665346986306e-09], ["'cabinet washer - CONSQ' (unit, GLO, None)", 1.14807229314759e-09], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 6.8801639197282534e-12], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 4.697413903335787e-11], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -6.536131531334705e-10], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.2066908919746314e-12], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.517729963448163e-12], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.272743036842063e-12], ["'market for corrugated board box' (kilogram, RER, None)", 2.872368105412271e-11], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.527641183200643e-11]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 6.880138454036532e-10], ["'alubox production - CONSQ' (kilogram, GLO, None)", 1.240919621881071e-10], ["'market for polysulfone' (kilogram, GLO, None)", 7.37809084738171e-12], ["'autoclave - CONSQ' (unit, GLO, None)", 5.0422665346986306e-09], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 6.8801639197282534e-12], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 4.697413903335787e-11], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -6.536131531334705e-10], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.2066908919746314e-12], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.2295838123399307e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.8184357363977212e-10], ["'market for corrugated board box' (kilogram, RER, None)", 2.872368105412271e-11], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.527641183200643e-11], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 1.4282697117787904e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.272107854144826e-10], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.984019684026415e-11], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.49490926141749e-12]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 6.880138454036532e-10], ["'alubox production - CONSQ' (kilogram, GLO, None)", 1.240919621881071e-10], ["'market for polysulfone' (kilogram, GLO, None)", 7.37809084738171e-12], ["'autoclave - CONSQ' (unit, GLO, None)", 5.0422665346986306e-09], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 6.8801639197282534e-12], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 4.697413903335787e-11], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -6.536131531334705e-10], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.2066908919746314e-12], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.2295838123399307e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.8184357363977212e-10], ["'market for corrugated board box' (kilogram, RER, None)", 2.872368105412271e-11], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.527641183200643e-11], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 1.4282697117787904e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.272107854144826e-10], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 9.612150607466991e-11], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.49490926141749e-12]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 4.1110753914231425e-10], ["'alubox production - CONSQ' (kilogram, GLO, None)", 7.414842236577893e-11], ["'market for polysulfone' (kilogram, GLO, None)", 3.689045423690855e-12], ["'autoclave - CONSQ' (unit, GLO, None)", 3.3615110231324204e-09], ["'cabinet washer - CONSQ' (unit, GLO, None)", 5.74036146573795e-10], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.111090607887061e-12], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 2.806836349347417e-11], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -3.9055216218519856e-10], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.1033454459873157e-12], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.2588649817240815e-12], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.6363715184210316e-12], ["'market for corrugated board box' (kilogram, RER, None)", 1.7163203799923082e-11], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.5103363903326964e-11]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 4.1110753914231425e-10], ["'alubox production - CONSQ' (kilogram, GLO, None)", 7.414842236577893e-11], ["'market for polysulfone' (kilogram, GLO, None)", 3.689045423690855e-12], ["'autoclave - CONSQ' (unit, GLO, None)", 3.3615110231324204e-09], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.111090607887061e-12], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 2.806836349347417e-11], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -3.9055216218519856e-10], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.1033454459873157e-12], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.2295838123399307e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.8184357363977212e-10], ["'market for corrugated board box' (kilogram, RER, None)", 1.7163203799923082e-11], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.5103363903326964e-11], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 1.4282697117787904e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.272107854144826e-10], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.984019684026415e-11], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.49490926141749e-12]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 2.5998969977386397e-07], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 1.315906263224426e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.936728051402973e-08], ["'market for corrugated board box' (kilogram, RER, None)", 2.084536093333721e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 4.303883193640819e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.002837272676786e-10], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -1.4039443787788655e-07], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.5120211529131917e-08], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 9.183485854562929e-08], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -5.867817909548312e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.1196882908300931e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.3644570721830188e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.4445082352527581e-08]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 2.5998969977386397e-07], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 1.315906263224426e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.936728051402973e-08], ["'market for corrugated board box' (kilogram, RER, None)", 2.084536093333721e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 4.303883193640819e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.002837272676786e-10], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.9964099683832457e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.2756125890322416e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.434104990738661e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.9662110263815975e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.4445082352527581e-08]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 7.396890049904298e-07], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 3.7438459883286484e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.1872671660548197e-07], ["'market for corrugated board box' (kilogram, RER, None)", 6.286696153365e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 5.738510924854425e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.8103794953917617e-09], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -3.994320626948321e-07], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -4.5600637021254796e-08], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.6127663980587493e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -2.077426174340871e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.185592058703976e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.88197645825155e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.109727655561152e-08]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 7.396890049904298e-07], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 3.7438459883286484e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.1872671660548197e-07], ["'market for corrugated board box' (kilogram, RER, None)", 6.286696153365e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 5.738510924854425e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 8.513180340140398e-09], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.679926952301628e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -3.84708550803865e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.925200117706473e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -8.439079257687942e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.109727655561152e-08]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 4.1110753914231425e-10], ["'alubox production - CONSQ' (kilogram, GLO, None)", 7.414842236577893e-11], ["'market for polysulfone' (kilogram, GLO, None)", 3.689045423690855e-12], ["'autoclave - CONSQ' (unit, GLO, None)", 3.3615110231324204e-09], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.111090607887061e-12], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 2.806836349347417e-11], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -3.9055216218519856e-10], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.1033454459873157e-12], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.2295838123399307e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.8184357363977212e-10], ["'market for corrugated board box' (kilogram, RER, None)", 1.7163203799923082e-11], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.5103363903326964e-11], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 1.4282697117787904e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.272107854144826e-10], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 9.612150607466991e-11], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.49490926141749e-12]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 2.5998969977386397e-07], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 1.315906263224426e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.936728051402973e-08], ["'market for corrugated board box' (kilogram, RER, None)", 2.084536093333721e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 4.303883193640819e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.002837272676786e-10], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -1.4039443787788655e-07], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.5120211529131917e-08], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 9.183485854562929e-08], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.1133782181569887e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.1196882908300931e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.3644570721830188e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.4445082352527581e-08]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 2.5998969977386397e-07], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 1.315906263224426e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.936728051402973e-08], ["'market for corrugated board box' (kilogram, RER, None)", 2.084536093333721e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 4.303883193640819e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.002837272676786e-10], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.9964099683832457e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.4203874307760626e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.434104990738661e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.9662110263815975e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.4445082352527581e-08]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 7.396890049904298e-07], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 3.7438459883286484e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.1872671660548197e-07], ["'market for corrugated board box' (kilogram, RER, None)", 6.286696153365e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 5.738510924854425e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.8103794953917617e-09], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -3.994320626948321e-07], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -4.5600637021254796e-08], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.6127663980587493e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.941773735985571e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.185592058703976e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.88197645825155e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.109727655561152e-08]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 7.396890049904298e-07], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 3.7438459883286484e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.1872671660548197e-07], ["'market for corrugated board box' (kilogram, RER, None)", 6.286696153365e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 5.738510924854425e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 8.513180340140398e-09], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.679926952301628e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 7.299580992565871e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.925200117706473e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -8.439079257687942e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.109727655561152e-08]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 4.7148338047659613e-07], ["'alubox production - CONSQ' (kilogram, GLO, None)", 5.558141419749438e-08], ["'market for polysulfone' (kilogram, GLO, None)", 3.741766550065263e-09], ["'autoclave - CONSQ' (unit, GLO, None)", 8.607766387281638e-07], ["'cabinet washer - CONSQ' (unit, GLO, None)", 2.11584331074012e-07], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.8740620316219478e-09], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 2.823891033022743e-08], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -4.4790921145276626e-07], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 9.182376688278926e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.258010251094816e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.5252077507175098e-09], ["'market for corrugated board box' (kilogram, RER, None)", 7.356925439091028e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.523651692964974e-09]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 4.7148338047659613e-07], ["'alubox production - CONSQ' (kilogram, GLO, None)", 5.558141419749438e-08], ["'market for polysulfone' (kilogram, GLO, None)", 3.741766550065263e-09], ["'autoclave - CONSQ' (unit, GLO, None)", 8.607766387281638e-07], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.8740620316219478e-09], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 2.823891033022743e-08], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -4.4790921145276626e-07], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 9.182376688278926e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.1407389430900466e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.2600558380265754e-08], ["'market for corrugated board box' (kilogram, RER, None)", 7.356925439091028e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.523651692964974e-09], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 7.368453535230518e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 5.878987026143975e-08], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.904960099703577e-09], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.164226678597048e-09]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 4.7148338047659613e-07], ["'alubox production - CONSQ' (kilogram, GLO, None)", 5.558141419749438e-08], ["'market for polysulfone' (kilogram, GLO, None)", 3.741766550065263e-09], ["'autoclave - CONSQ' (unit, GLO, None)", 8.607766387281638e-07], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.8740620316219478e-09], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 2.823891033022743e-08], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -4.4790921145276626e-07], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 9.182376688278926e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.1407389430900466e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.2600558380265754e-08], ["'market for corrugated board box' (kilogram, RER, None)", 7.356925439091028e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.523651692964974e-09], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 7.368453535230518e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 5.878987026143975e-08], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.6145311837588914e-08], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.164226678597048e-09]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 2.8172452282630134e-07], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.3211451434346776e-08], ["'market for polysulfone' (kilogram, GLO, None)", 1.8708832750326313e-09], ["'autoclave - CONSQ' (unit, GLO, None)", 5.738510924854425e-07], ["'cabinet washer - CONSQ' (unit, GLO, None)", 1.05792165537006e-07], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.7173325465118384e-09], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.687353969905826e-08], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -2.676382966849863e-07], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 4.591188344139463e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.129005125547408e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -7.626038753587549e-10], ["'market for corrugated board box' (kilogram, RER, None)", 4.395968971178735e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.7030085656476538e-09]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 2.8172452282630134e-07], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.3211451434346776e-08], ["'market for polysulfone' (kilogram, GLO, None)", 1.8708832750326313e-09], ["'autoclave - CONSQ' (unit, GLO, None)", 5.738510924854425e-07], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.7173325465118384e-09], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.687353969905826e-08], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -2.676382966849863e-07], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 4.591188344139463e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.1407389430900466e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.2600558380265754e-08], ["'market for corrugated board box' (kilogram, RER, None)", 4.395968971178735e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.7030085656476538e-09], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 7.368453535230518e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 5.878987026143975e-08], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.904960099703577e-09], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.164226678597048e-09]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.04791118722555781], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.002985829534919112], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.005089126095588483], ["'market for corrugated board box' (kilogram, RER, None)", 0.00020399786499775133], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0019518319803824608], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.5740261101999055e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.02587204110180122], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.002581673747240563], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00010648017094743199], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -9.72324535852973e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00018553752254476212], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.005192258215602436], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00027187662283107366]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.04791118722555781], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.002985829534919112], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.005089126095588483], ["'market for corrugated board box' (kilogram, RER, None)", 0.00020399786499775133], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0019518319803824608], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.5740261101999055e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00023147863249441738], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -2.1137489909847236e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0004033424420833057], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.011287517859612484], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00027187662283107366]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.13631070168398135], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00849489529653043], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.015348157755148117], ["'market for corrugated board box' (kilogram, RER, None)", 0.0006152316562314952], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0026024426405099475], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.762935889866213e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.07360777890934994], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0077860000323671736], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0003029435849490319], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -3.442391144155824e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0005278673209773634], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.014772340272958212], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0007735081382584998]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.13631070168398135], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00849489529653043], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.015348157755148117], ["'market for corrugated board box' (kilogram, RER, None)", 0.0006152316562314952], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0026024426405099475], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.00036504651852057256], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0006585730107587649], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -6.374798415103376e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0011475376526563395], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.032113783204439944], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0007735081382584998]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 2.8172452282630134e-07], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.3211451434346776e-08], ["'market for polysulfone' (kilogram, GLO, None)", 1.8708832750326313e-09], ["'autoclave - CONSQ' (unit, GLO, None)", 5.738510924854425e-07], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.7173325465118384e-09], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.687353969905826e-08], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -2.676382966849863e-07], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 4.591188344139463e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.1407389430900466e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.2600558380265754e-08], ["'market for corrugated board box' (kilogram, RER, None)", 4.395968971178735e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.7030085656476538e-09], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 7.368453535230518e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 5.878987026143975e-08], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.6145311837588914e-08], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.164226678597048e-09]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.04791118722555781], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.002985829534919112], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.005089126095588483], ["'market for corrugated board box' (kilogram, RER, None)", 0.00020399786499775133], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0019518319803824608], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.5740261101999055e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.02587204110180122], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.002581673747240563], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00010648017094743199], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.2717493355269386e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00018553752254476212], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.005192258215602436], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00027187662283107366]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.04791118722555781], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.002985829534919112], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.005089126095588483], ["'market for corrugated board box' (kilogram, RER, None)", 0.00020399786499775133], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0019518319803824608], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.5740261101999055e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00023147863249441738], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.7646724685368232e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0004033424420833057], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.011287517859612484], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00027187662283107366]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.13631070168398135], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00849489529653043], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.015348157755148117], ["'market for corrugated board box' (kilogram, RER, None)", 0.0006152316562314952], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0026024426405099475], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.762935889866213e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.07360777890934994], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0077860000323671736], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0003029435849490319], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 4.502466500409254e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0005278673209773634], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.014772340272958212], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0007735081382584998]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.13631070168398135], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00849489529653043], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.015348157755148117], ["'market for corrugated board box' (kilogram, RER, None)", 0.0006152316562314952], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0026024426405099475], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.00036504651852057256], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0006585730107587649], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.337900926683803e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0011475376526563395], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.032113783204439944], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0007735081382584998]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00609930794777992], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0017382487207744984], ["'market for polysulfone' (kilogram, GLO, None)", 0.0004331310817870554], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0039036639607649215], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.0012840456470791324], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.00022546720665815237], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00019556570070000507], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.005794342550390923], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.6488607208151193e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.036981209464168e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.803973342666852e-05], ["'market for corrugated board box' (kilogram, RER, None)", 7.199669448380936e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -8.514144226614146e-05]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00609930794777992], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0017382487207744984], ["'market for polysulfone' (kilogram, GLO, None)", 0.0004331310817870554], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0039036639607649215], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.00022546720665815237], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00019556570070000507], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.005794342550390923], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.6488607208151193e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00035473033269068174], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.002001643635136486], ["'market for corrugated board box' (kilogram, RER, None)", 7.199669448380936e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -8.514144226614146e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.000672543007716674], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.007599942363230531], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -3.156606890866001e-05], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -2.322725349258902e-05]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00609930794777992], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0017382487207744984], ["'market for polysulfone' (kilogram, GLO, None)", 0.0004331310817870554], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0039036639607649215], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.00022546720665815237], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00019556570070000507], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.005794342550390923], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.6488607208151193e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00035473033269068174], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.002001643635136486], ["'market for corrugated board box' (kilogram, RER, None)", 7.199669448380936e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -8.514144226614146e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.000672543007716674], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.007599942363230531], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 4.128675733207683e-05], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -2.322725349258902e-05]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.003644507298267878], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0010386522869981264], ["'market for polysulfone' (kilogram, GLO, None)", 0.0002165655408935277], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0026024426405099475], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.0006420228235395662], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.00013472296975672516], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00011685598261216989], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0034622819333544838], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 8.244303604075597e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.18490604732084e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.901986671333426e-05], ["'market for corrugated board box' (kilogram, RER, None)", 4.302004112975829e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -5.087439603161276e-05]]</t>
   </si>
   <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.003644507298267878], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0010386522869981264], ["'market for polysulfone' (kilogram, GLO, None)", 0.0002165655408935277], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0026024426405099475], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.00013472296975672516], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00011685598261216989], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0034622819333544838], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 8.244303604075597e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00035473033269068174], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.002001643635136486], ["'market for corrugated board box' (kilogram, RER, None)", 4.302004112975829e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -5.087439603161276e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.000672543007716674], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.007599942363230531], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -3.156606890866001e-05], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -2.322725349258902e-05]]</t>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.003644507298267878], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0010386522869981264], ["'market for polysulfone' (kilogram, GLO, None)", 0.0002165655408935277], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0026024426405099475], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.00013472296975672516], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00011685598261216989], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0034622819333544838], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 8.244303604075597e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00035473033269068174], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.002001643635136486], ["'market for corrugated board box' (kilogram, RER, None)", 4.302004112975829e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -5.087439603161276e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.000672543007716674], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.007599942363230531], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 4.128675733207683e-05], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -2.322725349258902e-05]]</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
modified:   Brighway/Libaries/LCA_plots.py 	modified:   Brighway/Libaries/__pycache__/LCA_plots.cpython-311.pyc 	modified:   Brighway/Libaries/__pycache__/box_plot.cpython-311.pyc 	modified:   Brighway/Libaries/__pycache__/life_cycle_assessment.cpython-311.pyc 	modified:   Brighway/Libaries/life_cycle_assessment.py 	modified:   Brighway/Ofir/Ofir.ipynb 	modified:   Brighway/Results/Ananas - CONSQ_recipe.xlsx 	modified:   Brighway/Results_Ofir/GWP_life_stage_pr_scenario_CONSQ.jpg 	modified:   Brighway/Results_Ofir/break_even_large_CONSQ.jpg 	modified:   Brighway/Results_Ofir/break_even_small_CONSQ.jpg 	modified:   Brighway/Results_Ofir/scaled_impact_score_multi_CONSQ_ReCiPe 2016 v1.03, endpoint (H).jpg 	modified:   Brighway/Results_Ofir/scaled_impact_score_multi_CONSQ_ReCiPe 2016 v1.03, midpoint (H).jpg
</commit_message>
<xml_diff>
--- a/Brighway/Results/Ananas - CONSQ_recipe.xlsx
+++ b/Brighway/Results/Ananas - CONSQ_recipe.xlsx
@@ -88,7 +88,7 @@
     <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0009373131829579762], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0004495514225803063], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0001399039509001107], ["'market for corrugated board box' (kilogram, RER, None)", 6.073300209944417e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000616350184568094], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.362031019620352e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0005061491187973072], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -5.664283541570399e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.6117549334775722e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.4128545807312035e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.78857789405792e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00023624312087142089], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.8854839025352327e-05]]</t>
   </si>
   <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0009373131829579762], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0004495514225803063], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0001399039509001107], ["'market for corrugated board box' (kilogram, RER, None)", 6.073300209944417e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000616350184568094], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.5809710865610812e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.5038150727773306e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 4.468249223576303e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00014757778009440384], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.000513572001932085], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.8854839025352327e-05]]</t>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0009373131829579762], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0004495514225803063], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0001399039509001107], ["'market for corrugated board box' (kilogram, RER, None)", 6.073300209944417e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000616350184568094], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.3620310201579298e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.5038150727773306e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 4.468249223576303e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00014757778009440384], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.000513572001932085], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.8854839025352327e-05]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0006799317205210687], ["'alubox production - CONSQ' (kilogram, GLO, None)", 5.9310919264254154e-05], ["'market for polysulfone' (kilogram, GLO, None)", 4.019118309206293e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000924525276852141], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.00016623361404338074], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.495551281007104e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 5.907099145686869e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0006459351344950152], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 9.505013037587547e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.3335979393624514e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -9.281865639367464e-07], ["'market for corrugated board box' (kilogram, RER, None)", 7.107201576755263e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.176104412433239e-06]]</t>
@@ -112,7 +112,7 @@
     <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.4388283642845579], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.1339983006805709], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.06222099943016971], ["'market for corrugated board box' (kilogram, RER, None)", 0.02733705682567877], ["'autoclave - CONSQ' (unit, GLO, None)", 0.41815922054490096], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.000684750375565388], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.23696731671366128], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.026242708271574065], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.23848154543441785], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0360000868022972], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.006664202419615243], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.28665342969915536], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.01961150957529672]]</t>
   </si>
   <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.4388283642845579], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.1339983006805709], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.06222099943016971], ["'market for corrugated board box' (kilogram, RER, None)", 0.02733705682567877], ["'autoclave - CONSQ' (unit, GLO, None)", 0.41815922054490096], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.003219989759056317], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.5184381422487344], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.06666682741166148], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.014487396543647602], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.6231596298265071], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.01961150957529672]]</t>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.4388283642845579], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.1339983006805709], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.06222099943016971], ["'market for corrugated board box' (kilogram, RER, None)", 0.02733705682567877], ["'autoclave - CONSQ' (unit, GLO, None)", 0.41815922054490096], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.0006847503756748774], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.5184381422487344], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.06666682741166148], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.014487396543647602], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.6231596298265071], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.01961150957529672]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.15652274511716874], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.02506742788826223], ["'market for polysulfone' (kilogram, GLO, None)", 0.0021337009725469172], ["'autoclave - CONSQ' (unit, GLO, None)", 0.6272388308173514], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.16276703443760637], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.0017058255370440256], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0050526572112086264], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.14869660786131028], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.000757439926670406], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00013091647106343603], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0011262459663236265], ["'market for corrugated board box' (kilogram, RER, None)", 0.0031990839685017074], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0021586743922518232]]</t>
@@ -136,7 +136,7 @@
     <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.007328560174345679], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.007628733536774561], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0014347538118721001], ["'market for corrugated board box' (kilogram, RER, None)", 0.00043074636577255046], ["'autoclave - CONSQ' (unit, GLO, None)", 0.010823265766749086], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.3570135248158271e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.003957422494146667], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0004515225616910651], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.012449198643846453], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0018785854298641296], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0031533154861022395], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.006385055965478946], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.000367262141947291]]</t>
   </si>
   <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.007328560174345679], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.007628733536774561], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0014347538118721001], ["'market for corrugated board box' (kilogram, RER, None)", 0.00043074636577255046], ["'autoclave - CONSQ' (unit, GLO, None)", 0.010823265766749086], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.381259227787924e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.02706347531270968], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0034788619071557956], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.006855033655629201], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.013880556447712073], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.000367262141947291]]</t>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.007328560174345679], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.007628733536774561], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0014347538118721001], ["'market for corrugated board box' (kilogram, RER, None)", 0.00043074636577255046], ["'autoclave - CONSQ' (unit, GLO, None)", 0.010823265766749086], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.3570135250328094e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.02706347531270968], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0034788619071557956], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.006855033655629201], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.013880556447712073], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.000367262141947291]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0037239953774620004], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0014142961560177963], ["'market for polysulfone' (kilogram, GLO, None)", 5.2525211287247595e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.01623489865012363], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.006926399749254169], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.632351514481635e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.001537849262441289], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0035377956085889], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.7775049817998695e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.194603788971084e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.508654277542893e-05], ["'market for corrugated board box' (kilogram, RER, None)", 5.0407540285717045e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.0425209391520094e-05]]</t>
@@ -160,7 +160,7 @@
     <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.009943938900786552], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0099383937164964], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0019081200287183278], ["'market for corrugated board box' (kilogram, RER, None)", 0.0006031781176429667], ["'autoclave - CONSQ' (unit, GLO, None)", 0.012272026670203311], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.929025311650959e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.005369727006424739], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0006119474256228533], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.01802348310847296], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0027199483188183843], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.003893082814962413], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.008184872187976932], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0004635801655524203]]</t>
   </si>
   <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.009943938900786552], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0099383937164964], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0019081200287183278], ["'market for corrugated board box' (kilogram, RER, None)", 0.0006031781176429667], ["'autoclave - CONSQ' (unit, GLO, None)", 0.012272026670203311], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 9.071103821371131e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.039181485018419476], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.005036941331145155], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.008463223498675876], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.01779320040995137], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0004635801655524203]]</t>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.009943938900786552], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0099383937164964], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0019081200287183278], ["'market for corrugated board box' (kilogram, RER, None)", 0.0006031781176429667], ["'autoclave - CONSQ' (unit, GLO, None)", 0.012272026670203311], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.929025311959404e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.039181485018419476], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.005036941331145155], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.008463223498675876], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.01779320040995137], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0004635801655524203]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.005214791760272705], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0018439750484988964], ["'market for polysulfone' (kilogram, GLO, None)", 6.729644141243289e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.018408040005304965], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.008443231015985712], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.828661645115836e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0021159771037727914], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.004954052172259069], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 5.029642135612412e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -7.647856886706219e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.215792427900825e-05], ["'market for corrugated board box' (kilogram, RER, None)", 7.058614460976231e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -5.102710876445776e-05]]</t>
@@ -184,7 +184,7 @@
     <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.2082568907753308], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.7513963266369649], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.1537280274149883], ["'market for corrugated board box' (kilogram, RER, None)", 0.0446523339165811], ["'autoclave - CONSQ' (unit, GLO, None)", 1.50569551187976], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.0024677062296987484], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.6524587210186786], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.07530483042536665], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.6929207969732823], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.10459149278780218], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.19761186343013165], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.6422952795934875], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.06605782859072676]]</t>
   </si>
   <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.2082568907753308], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.7513963266369649], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.1537280274149883], ["'market for corrugated board box' (kilogram, RER, None)", 0.0446523339165811], ["'autoclave - CONSQ' (unit, GLO, None)", 1.50569551187976], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.011604212383861145], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.5063495586375701], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.19368794960704105], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.429591006842007], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.3962940861752748], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.06605782859072676]]</t>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.2082568907753308], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.7513963266369649], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.1537280274149883], ["'market for corrugated board box' (kilogram, RER, None)", 0.0446523339165811], ["'autoclave - CONSQ' (unit, GLO, None)", 1.50569551187976], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.002467706230093327], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.5063495586375701], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.19368794960704105], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.429591006842007], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.3962940861752748], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.06605782859072676]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.13224599475672763], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.06762232827194302], ["'market for polysulfone' (kilogram, GLO, None)", 0.008388737139565776], ["'autoclave - CONSQ' (unit, GLO, None)", 2.2585432678196398], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.4854281992055989], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.032035708103587614], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.47366216002384215], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.12563369501889124], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.0003957376479410388], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0038820321130095775], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0025235437391768374], ["'market for corrugated board box' (kilogram, RER, None)", 0.005225382033611543], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.007271104880482139]]</t>
@@ -208,7 +208,7 @@
     <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.33450165541872323], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.03284935350970735], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.03946367741350463], ["'market for corrugated board box' (kilogram, RER, None)", 0.0030394101114248266], ["'autoclave - CONSQ' (unit, GLO, None)", 0.015726485684142134], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.00018925759883661535], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.18063089392611056], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.019258909337621453], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0008823565255795569], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00013066350291084805], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0015888976321569858], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.04328903045332324], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0023269284922689485]]</t>
   </si>
   <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.33450165541872323], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.03284935350970735], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.03946367741350463], ["'market for corrugated board box' (kilogram, RER, None)", 0.0030394101114248266], ["'autoclave - CONSQ' (unit, GLO, None)", 0.015726485684142134], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.0008899703480619658], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0019181663599555584], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00024196944983490376], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00345412528235449], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.09410658794891366], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0023269284922689485]]</t>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.33450165541872323], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.03284935350970735], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.03946367741350463], ["'market for corrugated board box' (kilogram, RER, None)", 0.0030394101114248266], ["'autoclave - CONSQ' (unit, GLO, None)", 0.015726485684142134], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.00018925759886687704], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0019181663599555584], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00024196944983490376], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00345412528235449], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.09410658794891366], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0023269284922689485]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.033832419440732626], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.006149296159342674], ["'market for polysulfone' (kilogram, GLO, None)", 0.0011275973997964702], ["'autoclave - CONSQ' (unit, GLO, None)", 0.023589728526213202], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.004343848313710668], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.000535042693546586], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.000971249625905885], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.032140798468696], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 4.876235116799861e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.1213468287034964e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00017008028121374185], ["'market for corrugated board box' (kilogram, RER, None)", 0.0003556830650484527], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00025612923521141666]]</t>
@@ -232,7 +232,7 @@
     <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 4.5827494278139374e-05], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 6.253406654300599e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.4068435882149842e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.1021773118319107e-05], ["'autoclave - CONSQ' (unit, GLO, None)", -3.0636972111713774e-05], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.682851769883089e-08], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -2.4746846910195263e-05], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -3.035896425945613e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.998072193676123e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.569098904026384e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.5976873736272905e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.486010978994426e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.525843317828836e-06]]</t>
   </si>
   <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 4.5827494278139374e-05], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 6.253406654300599e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.4068435882149842e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.1021773118319107e-05], ["'autoclave - CONSQ' (unit, GLO, None)", -3.0636972111713774e-05], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.6128061994774187e-07], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.691461290600267e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.0313146118567377e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.647146456325348e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.404371693862777e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.525843317828836e-06]]</t>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 4.5827494278139374e-05], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 6.253406654300599e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.4068435882149842e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.1021773118319107e-05], ["'autoclave - CONSQ' (unit, GLO, None)", -3.0636972111713774e-05], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.682851771111553e-08], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.691461290600267e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.0313146118567377e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.647146456325348e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.404371693862777e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.525843317828836e-06]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 5.11835150644143e-05], ["'alubox production - CONSQ' (kilogram, GLO, None)", 1.2403929145125681e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.9126691235872395e-07], ["'autoclave - CONSQ' (unit, GLO, None)", -4.595545816757066e-05], ["'cabinet washer - CONSQ' (unit, GLO, None)", 3.457256187858905e-06], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.673248658294235e-07], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 2.9829706100578206e-06], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -4.862433931119358e-05], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.6405520745686866e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.1030872483757e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -9.767403935362618e-08], ["'market for corrugated board box' (kilogram, RER, None)", 2.4600460027988033e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.981677741853955e-07]]</t>
@@ -256,7 +256,7 @@
     <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 5.376047508892532e-06], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 7.425815006014254e-06], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.9594788369286424e-06], ["'market for corrugated board box' (kilogram, RER, None)", 1.2118799351660813e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00017715404964801845], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.633607522116651e-08], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -2.9030656548019673e-06], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -3.3720931547561873e-07], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.7221996266038696e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.5985065281869045e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.7752712651195124e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.18982713443991e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.2126545790567683e-05]]</t>
   </si>
   <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 5.376047508892532e-06], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 7.425815006014254e-06], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.9594788369286424e-06], ["'market for corrugated board box' (kilogram, RER, None)", 1.2118799351660813e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00017715404964801845], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.681922754974344e-08], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.091738318704064e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.03676046818276e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.033198393799426e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.760493770870923e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.2126545790567683e-05]]</t>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 5.376047508892532e-06], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 7.425815006014254e-06], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.9594788369286424e-06], ["'market for corrugated board box' (kilogram, RER, None)", 1.2118799351660813e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00017715404964801845], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.6336075223778596e-08], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.091738318704064e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.03676046818276e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.033198393799426e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.760493770870923e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.2126545790567683e-05]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 3.692348298539384e-06], ["'alubox production - CONSQ' (kilogram, GLO, None)", 2.0619203610568115e-06], ["'market for polysulfone' (kilogram, GLO, None)", 8.462756924699476e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002657310744720277], ["'cabinet washer - CONSQ' (unit, GLO, None)", 1.1320412288153831e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.5525177438659536e-08], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 6.292610430619047e-08], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -3.5077308836124148e-06], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 6.849922026495211e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.4519460453930945e-09], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -8.603713479714355e-09], ["'market for corrugated board box' (kilogram, RER, None)", 1.4181869310440799e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.435508985358827e-06]]</t>
@@ -280,7 +280,7 @@
     <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.010006830960698621], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.005060186262026125], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0016435175439759764], ["'market for corrugated board box' (kilogram, RER, None)", 0.0008303322974843852], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00181949401618542], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.85379676415959e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.005403688718777256], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0007851198612636768], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0005516263984969325], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.345268627709203e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0009682405116559995], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.002423868259982945], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00021790980716459963]]</t>
   </si>
   <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.010006830960698621], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.005060186262026125], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0016435175439759764], ["'market for corrugated board box' (kilogram, RER, None)", 0.0008303322974843852], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00181949401618542], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.0003693191862716783], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0011991878228194185], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00015454201162424448], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.002104870674500697], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.005269278826436599], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00021790980716459963]]</t>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.010006830960698621], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.005060186262026125], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0016435175439759764], ["'market for corrugated board box' (kilogram, RER, None)", 0.0008303322974843852], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00181949401618542], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.853796765415388e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0011991878228194185], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00015454201162424448], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.002104870674500697], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.005269278826436599], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00021790980716459963]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.03049272720877801], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.001165474968186897], ["'market for polysulfone' (kilogram, GLO, None)", 4.904841909964629e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00272924102427813], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.002007297634397571], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.2365670834025218e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00047576668126590743], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.028968090848339106], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 6.736656759332428e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.9020825440950147e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -9.523248521989348e-06], ["'market for corrugated board box' (kilogram, RER, None)", 9.716857079202168e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.3985727296550403e-05]]</t>
@@ -304,7 +304,7 @@
     <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.16693492271614604], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.13819992897220307], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.03298497586122507], ["'market for corrugated board box' (kilogram, RER, None)", 0.01535703234737849], ["'autoclave - CONSQ' (unit, GLO, None)", 0.04029563926146141], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.00026601763564448053], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.09014485826671886], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.010439044011849703], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.15019144169077725], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.022665301505849826], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.03139533774882958], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.09629696652448094], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.021540668230827467]]</t>
   </si>
   <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.16693492271614604], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.13819992897220307], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.03298497586122507], ["'market for corrugated board box' (kilogram, RER, None)", 0.01535703234737849], ["'autoclave - CONSQ' (unit, GLO, None)", 0.04029563926146141], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.0012509289415085633], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.3265031341103853], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.04197278056638856], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.06825073413891031], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.20934123159032242], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.021540668230827467]]</t>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.16693492271614604], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.13819992897220307], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.03298497586122507], ["'market for corrugated board box' (kilogram, RER, None)", 0.01535703234737849], ["'autoclave - CONSQ' (unit, GLO, None)", 0.04029563926146141], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.00026601763568701595], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.3265031341103853], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.04197278056638856], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.06825073413891031], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.20934123159032242], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.021540668230827467]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.13032565584744885], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.02856025811114962], ["'market for polysulfone' (kilogram, GLO, None)", 0.0014311051476188273], ["'autoclave - CONSQ' (unit, GLO, None)", 0.06044345889219211], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.062405983766129255], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.00140736120379972], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.043111645823239425], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.1238093730550764], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.0007369206162690872], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0006167529986519748], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0003783456218584972], ["'market for corrugated board box' (kilogram, RER, None)", 0.0017971369887965557], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0023710203808304294]]</t>
@@ -328,7 +328,7 @@
     <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.006416630454633346], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.012637156434647984], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0027931635509381237], ["'market for corrugated board box' (kilogram, RER, None)", -0.00028778652347785823], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0014755822569674588], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.0856706918376308e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.003464980445502007], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0004668724238384532], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.6847120605711605e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.392337796782687e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.61308795344571e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00982232202795531], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0005226687696603586]]</t>
   </si>
   <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.006416630454633346], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.012637156434647984], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0027931635509381237], ["'market for corrugated board box' (kilogram, RER, None)", -0.00028778652347785823], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0014755822569674588], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 5.1052889259655955e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.662417522980783e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 6.282107031079051e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.5067129372547175e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.02135287397538301], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0005226687696603586]]</t>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.006416630454633346], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.012637156434647984], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0027931635509381237], ["'market for corrugated board box' (kilogram, RER, None)", -0.00028778652347785823], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0014755822569674588], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.0856706920112262e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.662417522980783e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 6.282107031079051e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.5067129372547175e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.02135287397538301], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0005226687696603586]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0008274258581216459], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0018752795072104864], ["'market for polysulfone' (kilogram, GLO, None)", 0.00011308662079259678], ["'autoclave - CONSQ' (unit, GLO, None)", 0.002213373385451188], ["'cabinet washer - CONSQ' (unit, GLO, None)", 8.559651273248125e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.260377921681201e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00018725643970961882], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0007860545652155636], ["'plastic incineration - CONSQ' (kilogram, CH, None)", -7.254875744731232e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.1688680667692706e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.85913769653005e-05], ["'market for corrugated board box' (kilogram, RER, None)", -3.367784833164815e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -5.7531098478864144e-05]]</t>
@@ -352,7 +352,7 @@
     <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0048368730792224856], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.007124026196025846], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.002460545768059087], ["'market for corrugated board box' (kilogram, RER, None)", 0.015401547220890875], ["'autoclave - CONSQ' (unit, GLO, None)", 0.22434057837977864], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.3802715780351274e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0026119114627801425], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0002947759829655848], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -5.3793954736489674e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -8.20620574591048e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.03176838334229084], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.04702365247506063], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.017992979926380392]]</t>
   </si>
   <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0048368730792224856], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.007124026196025846], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.002460545768059087], ["'market for corrugated board box' (kilogram, RER, None)", 0.015401547220890875], ["'autoclave - CONSQ' (unit, GLO, None)", 0.22434057837977864], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.0001119305717608042], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.00011694337986193407], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.5196677307241627e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.06906170281918723], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.10222533147502556], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.017992979926380392]]</t>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0048368730792224856], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.007124026196025846], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.002460545768059087], ["'market for corrugated board box' (kilogram, RER, None)", 0.015401547220890875], ["'autoclave - CONSQ' (unit, GLO, None)", 0.22434057837977864], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.3802715784157254e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.00011694337986193407], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.5196677307241627e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.06906170281918723], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.10222533147502556], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.017992979926380392]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0015002092875017413], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0029475230312975362], ["'market for polysulfone' (kilogram, GLO, None)", -2.4624839406446756e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.33651086756966797], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.069985841831298], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 6.877537770762638e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0010375830249309001], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0014251988231266542], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.1170202915333108e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0006240813793893255], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00018475341103514135], ["'market for corrugated board box' (kilogram, RER, None)", 0.001802346284702894], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0019805199012473667]]</t>
@@ -376,7 +376,7 @@
     <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0004393655094103275], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00021030197179078383], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.640228472872845e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.209689394007594e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0009113552122177312], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.1655105042678095e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.00023725737508157685], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -2.0046021770399717e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.4747994939848278e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.356535327286918e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -8.373621979971138e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0001528323205977195], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.2060175307085602e-05]]</t>
   </si>
   <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0004393655094103275], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00021030197179078383], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.640228472872845e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.209689394007594e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0009113552122177312], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 5.480729944421238e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.379998899967016e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 6.21580616164244e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0001820352601736389], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0003322441752368176], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.2060175307085602e-05]]</t>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0004393655094103275], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00021030197179078383], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.640228472872845e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.209689394007594e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0009113552122177312], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.165510504454171e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.379998899967016e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 6.21580616164244e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0001820352601736389], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0003322441752368176], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.2060175307085602e-05]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.001909903381614274], ["'alubox production - CONSQ' (kilogram, GLO, None)", 5.383540016672161e-05], ["'market for polysulfone' (kilogram, GLO, None)", 2.2951165960977628e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0013670328183265968], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.0001925900372458725], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.255637685124479e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", -0.00018516774676524117], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.00181440821253356], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 8.908884162993076e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.6449756033976153e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -6.004699988334661e-07], ["'market for corrugated board box' (kilogram, RER, None)", 3.7560977941833362e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.3274853473934867e-06]]</t>
@@ -400,7 +400,7 @@
     <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 3.2406602830087913e-08], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 4.371740419648934e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 9.27724372689787e-09], ["'market for corrugated board box' (kilogram, RER, None)", 3.6921100441779405e-09], ["'autoclave - CONSQ' (unit, GLO, None)", -2.592150313311692e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.0939319576485633e-10], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -1.7499565528247473e-08], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -3.877737904564959e-09], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.8515914844450735e-08], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.794478637023258e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.050190767681859e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -7.613954426174581e-08], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.6958565975708696e-09]]</t>
   </si>
   <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 3.2406602830087913e-08], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 4.371740419648934e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 9.27724372689787e-09], ["'market for corrugated board box' (kilogram, RER, None)", 3.6921100441779405e-09], ["'autoclave - CONSQ' (unit, GLO, None)", -2.592150313311692e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 9.846565552040756e-10], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 4.02519887922842e-08], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.1749604389319584e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.630849485470951e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.6552074840724738e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.6958565975708696e-09]]</t>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 3.2406602830087913e-08], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 4.371740419648934e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 9.27724372689787e-09], ["'market for corrugated board box' (kilogram, RER, None)", 3.6921100441779405e-09], ["'autoclave - CONSQ' (unit, GLO, None)", -2.592150313311692e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.0939319579833765e-10], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 4.02519887922842e-08], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.1749604389319584e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.630849485470951e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.6552074840724738e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.6958565975708696e-09]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 2.9426490598608053e-08], ["'alubox production - CONSQ' (kilogram, GLO, None)", 6.159776879286204e-09], ["'market for polysulfone' (kilogram, GLO, None)", 8.608425911461889e-10], ["'autoclave - CONSQ' (unit, GLO, None)", -3.888225469967538e-07], ["'cabinet washer - CONSQ' (unit, GLO, None)", 3.865988162882121e-08], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.510652856842942e-10], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 2.8252359290012935e-09], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -2.7955166068677648e-08], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.2674656970296917e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.992018042546741e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.9914818982807066e-10], ["'market for corrugated board box' (kilogram, RER, None)", 4.320644364750669e-10], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.967378202078723e-10]]</t>
@@ -424,7 +424,7 @@
     <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0004031179466426057], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00031688194657178144], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 7.27100511976521e-05], ["'market for corrugated board box' (kilogram, RER, None)", 4.9243331643582276e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002683386056274241], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.3418870129864744e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.00021768369118700708], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -2.5043320368352365e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.679134550107507e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.295711782021299e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.3939016070969654e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.000144493019504886], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.5286996259120968e-05]]</t>
   </si>
   <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0004031179466426057], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00031688194657178144], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 7.27100511976521e-05], ["'market for corrugated board box' (kilogram, RER, None)", 4.9243331643582276e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002683386056274241], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.310127885741498e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.2345944674146753e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.5362429225965368e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.204133921023868e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0003141152598162838], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.5286996259120968e-05]]</t>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0004031179466426057], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00031688194657178144], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 7.27100511976521e-05], ["'market for corrugated board box' (kilogram, RER, None)", 4.9243331643582276e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002683386056274241], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.341887013201038e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.2345944674146753e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.5362429225965368e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.204133921023868e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0003141152598162838], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.5286996259120968e-05]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0003070959975220654], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.269211273872963e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.8956198489533308e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004025079084411362], ["'cabinet washer - CONSQ' (unit, GLO, None)", 6.212970614681401e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.411296257488632e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.9268351301255548e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0002917411976459621], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.50440480181107e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -4.702755569845327e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.677053316616167e-07], ["'market for corrugated board box' (kilogram, RER, None)", 5.762637646808395e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.7833854947245283e-06]]</t>
@@ -448,7 +448,7 @@
     <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0008352415189031528], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.000394825523166951], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00013041825435768927], ["'market for corrugated board box' (kilogram, RER, None)", 3.385635133844707e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004934272041684305], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.07126353316432e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0004510304202077025], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -5.2953791400972424e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.882262226297923e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.837209113930959e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -7.926427776879018e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00031525679070111627], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.7734475552932816e-05]]</t>
   </si>
   <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0008352415189031528], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.000394825523166951], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00013041825435768927], ["'market for corrugated board box' (kilogram, RER, None)", 3.385635133844707e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004934272041684305], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.3252111970843614e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.439700491952006e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.0809646507279553e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00017231364707685353], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0006853408494005509], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.7734475552932816e-05]]</t>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0008352415189031528], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.000394825523166951], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00013041825435768927], ["'market for corrugated board box' (kilogram, RER, None)", 3.385635133844707e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004934272041684305], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.071263534294993e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.439700491952006e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.0809646507279553e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00017231364707685353], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0006853408494005509], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.7734475552932816e-05]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00040270113347142325], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.55134149702434e-05], ["'market for polysulfone' (kilogram, GLO, None)", 3.841999494362337e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0007401408062526457], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.00017398150328724294], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 3.092243820393865e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.7908722229360266e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0003825660767978521], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.012315978333832e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.5571255003207255e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.238627039124905e-06], ["'market for corrugated board box' (kilogram, RER, None)", 3.961996036714828e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.15350209367736e-06]]</t>
@@ -472,7 +472,7 @@
     <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0009037148513855984], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0004067982343555577], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00014548407311930413], ["'market for corrugated board box' (kilogram, RER, None)", 3.497535707747824e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000503520814957574], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.2255777674457005e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0004880060197482232], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -5.763223587600363e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.924398422749959e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.8978237812322e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -8.100483228600373e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0003331660614583805], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.870966509222013e-05]]</t>
   </si>
   <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0009037148513855984], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0004067982343555577], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00014548407311930413], ["'market for corrugated board box' (kilogram, RER, None)", 3.497535707747824e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000503520814957574], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.397776364157455e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.531300919021649e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.0921895891170739e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00017609746123929397], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0007242740467018087], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.870966509222013e-05]]</t>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0009037148513855984], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0004067982343555577], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00014548407311930413], ["'market for corrugated board box' (kilogram, RER, None)", 3.497535707747824e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000503520814957574], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.2255777686010475e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.531300919021649e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.0921895891170739e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00017609746123929397], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0007242740467018087], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.870966509222013e-05]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0004126359538879128], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.816335531480803e-05], ["'market for polysulfone' (kilogram, GLO, None)", 3.88155116343156e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000755281222436361], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.00017789009719927412], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 3.4545200183282885e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.8623214273884847e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0003920041561935171], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.0352750182351766e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.5913182274828571e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.3089916043468713e-06], ["'market for corrugated board box' (kilogram, RER, None)", 4.0929462462865255e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.2608429731730944e-06]]</t>
@@ -496,7 +496,7 @@
     <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0031855218690362576], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.000914436357866278], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0009771925256512753], ["'market for corrugated board box' (kilogram, RER, None)", 0.00011478805068582941], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0007338825422275394], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.420864154604482e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0017201818092795792], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.00021241543914212013], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00011680668235283588], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.5396231185210454e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -7.051205043754697e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0004171474473837644], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0005969229982741224]]</t>
   </si>
   <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0031855218690362576], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.000914436357866278], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0009771925256512753], ["'market for corrugated board box' (kilogram, RER, None)", 0.00011478805068582941], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0007338825422275394], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.6815122562860895e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0002539275703322519], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.8511539231871207e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00015328706594920652], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0009068422769877813], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0005969229982741224]]</t>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0031855218690362576], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.000914436357866278], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0009771925256512753], ["'market for corrugated board box' (kilogram, RER, None)", 0.00011478805068582941], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0007338825422275394], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.4208641548316735e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0002539275703322519], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.8511539231871207e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00015328706594920652], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0009068422769877813], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0005969229982741224]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0008862513405582456], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0006035256209839753], ["'market for polysulfone' (kilogram, GLO, None)", 3.468695127676702e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0011008238133413091], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.00018270602189388239], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.4786413443271393e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.257875181621341e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0008419387735303332], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.1081310681762825e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.3851903392909875e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.6389499699034864e-06], ["'market for corrugated board box' (kilogram, RER, None)", 1.3432924219539876e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -6.57043959606068e-05]]</t>
@@ -520,7 +520,7 @@
     <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.6380747785168264e-09], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 6.430352702009443e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.5690342233961884e-10], ["'market for corrugated board box' (kilogram, RER, None)", 2.454517946232539e-10], ["'autoclave - CONSQ' (unit, GLO, None)", 3.3615110231324204e-09], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.864723964591084e-12], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -8.845603803990862e-10], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -9.883804159989819e-11], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 6.944838155033444e-10], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.0482389246244923e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.31780038370903e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.3420246736748824e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.2963564790122821e-10]]</t>
   </si>
   <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.6380747785168264e-09], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 6.430352702009443e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.5690342233961884e-10], ["'market for corrugated board box' (kilogram, RER, None)", 2.454517946232539e-10], ["'autoclave - CONSQ' (unit, GLO, None)", 3.3615110231324204e-09], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.817358855376704e-11], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.5097474250072704e-09], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.9411831937490595e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -7.212609519480051e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.9174449429855987e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.2963564790122821e-10]]</t>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.6380747785168264e-09], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 6.430352702009443e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.5690342233961884e-10], ["'market for corrugated board box' (kilogram, RER, None)", 2.454517946232539e-10], ["'autoclave - CONSQ' (unit, GLO, None)", 3.3615110231324204e-09], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.864723965209041e-12], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.5097474250072704e-09], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.9411831937490595e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -7.212609519480051e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.9174449429855987e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.2963564790122821e-10]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 6.880138454036532e-10], ["'alubox production - CONSQ' (kilogram, GLO, None)", 1.240919621881071e-10], ["'market for polysulfone' (kilogram, GLO, None)", 7.37809084738171e-12], ["'autoclave - CONSQ' (unit, GLO, None)", 5.0422665346986306e-09], ["'cabinet washer - CONSQ' (unit, GLO, None)", 1.14807229314759e-09], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 6.8801639197282534e-12], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 4.697413903335787e-11], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -6.536131531334705e-10], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.2066908919746314e-12], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.517729963448163e-12], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.272743036842063e-12], ["'market for corrugated board box' (kilogram, RER, None)", 2.872368105412271e-11], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.527641183200643e-11]]</t>
@@ -544,7 +544,7 @@
     <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 7.396890049904298e-07], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 3.7438459883286484e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.1872671660548197e-07], ["'market for corrugated board box' (kilogram, RER, None)", 6.286696153365e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 5.738510924854425e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.8103794953917617e-09], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -3.994320626948321e-07], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -4.5600637021254796e-08], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.6127663980587493e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.941773735985571e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.185592058703976e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.88197645825155e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.109727655561152e-08]]</t>
   </si>
   <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 7.396890049904298e-07], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 3.7438459883286484e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.1872671660548197e-07], ["'market for corrugated board box' (kilogram, RER, None)", 6.286696153365e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 5.738510924854425e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 8.513180340140398e-09], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.679926952301628e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 7.299580992565871e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.925200117706473e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -8.439079257687942e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.109727655561152e-08]]</t>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 7.396890049904298e-07], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 3.7438459883286484e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.1872671660548197e-07], ["'market for corrugated board box' (kilogram, RER, None)", 6.286696153365e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 5.738510924854425e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.8103794956812358e-09], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.679926952301628e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 7.299580992565871e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.925200117706473e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -8.439079257687942e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.109727655561152e-08]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 4.7148338047659613e-07], ["'alubox production - CONSQ' (kilogram, GLO, None)", 5.558141419749438e-08], ["'market for polysulfone' (kilogram, GLO, None)", 3.741766550065263e-09], ["'autoclave - CONSQ' (unit, GLO, None)", 8.607766387281638e-07], ["'cabinet washer - CONSQ' (unit, GLO, None)", 2.11584331074012e-07], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.8740620316219478e-09], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 2.823891033022743e-08], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -4.4790921145276626e-07], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 9.182376688278926e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.258010251094816e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.5252077507175098e-09], ["'market for corrugated board box' (kilogram, RER, None)", 7.356925439091028e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.523651692964974e-09]]</t>
@@ -568,7 +568,7 @@
     <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.13631070168398135], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00849489529653043], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.015348157755148117], ["'market for corrugated board box' (kilogram, RER, None)", 0.0006152316562314952], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0026024426405099475], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.762935889866213e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.07360777890934994], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0077860000323671736], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0003029435849490319], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 4.502466500409254e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0005278673209773634], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.014772340272958212], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0007735081382584998]]</t>
   </si>
   <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.13631070168398135], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00849489529653043], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.015348157755148117], ["'market for corrugated board box' (kilogram, RER, None)", 0.0006152316562314952], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0026024426405099475], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.00036504651852057256], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0006585730107587649], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.337900926683803e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0011475376526563395], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.032113783204439944], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0007735081382584998]]</t>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.13631070168398135], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00849489529653043], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.015348157755148117], ["'market for corrugated board box' (kilogram, RER, None)", 0.0006152316562314952], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0026024426405099475], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.762935891107482e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0006585730107587649], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.337900926683803e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0011475376526563395], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.032113783204439944], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0007735081382584998]]</t>
   </si>
   <si>
     <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00609930794777992], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0017382487207744984], ["'market for polysulfone' (kilogram, GLO, None)", 0.0004331310817870554], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0039036639607649215], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.0012840456470791324], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.00022546720665815237], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00019556570070000507], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.005794342550390923], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.6488607208151193e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.036981209464168e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.803973342666852e-05], ["'market for corrugated board box' (kilogram, RER, None)", 7.199669448380936e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -8.514144226614146e-05]]</t>

</xml_diff>